<commit_message>
Update lot codes - 2025-01-21 09:25:50
</commit_message>
<xml_diff>
--- a/LotCode.xlsx
+++ b/LotCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf.sharepoint.com/sites/production-warehouse/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7103" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{314746CC-B8D5-4694-BB14-BE2708A7788F}"/>
+  <xr:revisionPtr revIDLastSave="7107" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C37D98F4-7BE3-4AEA-8ACB-8CA449C7E860}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
   </bookViews>
@@ -1096,8 +1096,8 @@
   <dimension ref="A1:AE283"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC4" sqref="AC4"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC28" sqref="AC28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,7 +1122,7 @@
     <col min="19" max="19" width="18.28515625" customWidth="1"/>
     <col min="20" max="20" width="13" customWidth="1"/>
     <col min="21" max="21" width="1.42578125" customWidth="1"/>
-    <col min="22" max="22" width="26.42578125" customWidth="1"/>
+    <col min="22" max="22" width="29.7109375" customWidth="1"/>
     <col min="23" max="23" width="26.28515625" customWidth="1"/>
     <col min="24" max="24" width="9.7109375" customWidth="1"/>
     <col min="26" max="26" width="18.28515625" customWidth="1"/>

</xml_diff>

<commit_message>
Update lot codes - 2025-01-21 14:37:57
</commit_message>
<xml_diff>
--- a/LotCode.xlsx
+++ b/LotCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf.sharepoint.com/sites/production-warehouse/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7107" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C37D98F4-7BE3-4AEA-8ACB-8CA449C7E860}"/>
+  <xr:revisionPtr revIDLastSave="7129" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B79622C6-E74E-4161-A858-A3523E24195C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
   </bookViews>
@@ -1096,8 +1096,8 @@
   <dimension ref="A1:AE283"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC28" sqref="AC28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,10 +1284,10 @@
         <v>10</v>
       </c>
       <c r="Q3" s="12">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="R3" s="7">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="S3" s="14">
         <v>46291</v>
@@ -1354,7 +1354,7 @@
         <v>10</v>
       </c>
       <c r="Q4" s="7">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="R4" s="28"/>
       <c r="S4" s="14">
@@ -1454,7 +1454,7 @@
       </c>
       <c r="Q6" s="49">
         <f>SUM(Q3:Q5)*30+R3+R5</f>
-        <v>7803</v>
+        <v>7809</v>
       </c>
       <c r="R6" s="50"/>
       <c r="U6" s="33"/>
@@ -1555,10 +1555,10 @@
         <v>52</v>
       </c>
       <c r="Q8" s="7">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="R8" s="7">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="S8" s="14">
         <v>46291</v>
@@ -1623,7 +1623,7 @@
         <v>52</v>
       </c>
       <c r="Q9" s="7">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="R9" s="15"/>
       <c r="S9" s="14">
@@ -1711,7 +1711,7 @@
       </c>
       <c r="Q11" s="49">
         <f>SUM(Q8:Q10)*30+R8</f>
-        <v>6356</v>
+        <v>6337</v>
       </c>
       <c r="R11" s="50"/>
       <c r="U11" s="33"/>
@@ -1814,7 +1814,7 @@
         <v>9</v>
       </c>
       <c r="R13" s="7">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="S13" s="14">
         <v>46199</v>
@@ -1914,7 +1914,7 @@
       </c>
       <c r="Q15" s="49">
         <f>SUM(Q13:Q14)*30+R13+R14</f>
-        <v>3903</v>
+        <v>3879</v>
       </c>
       <c r="R15" s="50"/>
       <c r="U15" s="33"/>
@@ -2023,7 +2023,7 @@
         <v>9</v>
       </c>
       <c r="R17" s="7">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="S17" s="14">
         <v>46199</v>
@@ -2083,7 +2083,7 @@
         <v>83</v>
       </c>
       <c r="Q18" s="7">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R18" s="7">
         <v>18</v>
@@ -2127,7 +2127,7 @@
       </c>
       <c r="Q19" s="49">
         <f>SUM(Q17:Q18)*30+R17+R18</f>
-        <v>1340</v>
+        <v>1385</v>
       </c>
       <c r="R19" s="50"/>
       <c r="U19" s="33"/>
@@ -2225,10 +2225,10 @@
         <v>54</v>
       </c>
       <c r="Q21" s="7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="R21" s="7">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="S21" s="14">
         <v>46291</v>
@@ -2278,7 +2278,7 @@
         <v>54</v>
       </c>
       <c r="Q22" s="7">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="R22" s="7"/>
       <c r="S22" s="14">
@@ -2318,7 +2318,7 @@
       </c>
       <c r="Q23" s="49">
         <f>SUM(Q21:Q22)*30+R21</f>
-        <v>1838</v>
+        <v>1841</v>
       </c>
       <c r="R23" s="50"/>
       <c r="U23" s="33"/>
@@ -2413,10 +2413,10 @@
         <v>27</v>
       </c>
       <c r="Q25" s="7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="R25" s="7">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="S25" s="14">
         <v>46199</v>
@@ -2463,7 +2463,7 @@
         <v>27</v>
       </c>
       <c r="Q26" s="7">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R26" s="15">
         <v>9</v>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="Q28" s="49">
         <f>SUM(Q25:Q27)*30+R25+R26+R27</f>
-        <v>2422</v>
+        <v>2418</v>
       </c>
       <c r="R28" s="50"/>
       <c r="U28" s="33"/>
@@ -2662,10 +2662,10 @@
         <v>55</v>
       </c>
       <c r="Q30" s="7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="R30" s="7">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="S30" s="14">
         <v>46352</v>
@@ -2714,7 +2714,7 @@
         <v>55</v>
       </c>
       <c r="Q31" s="7">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="R31" s="7"/>
       <c r="S31" s="14">
@@ -2769,7 +2769,7 @@
       </c>
       <c r="Q32" s="49">
         <f>SUM(Q30:Q31)*30+R30</f>
-        <v>624</v>
+        <v>609</v>
       </c>
       <c r="R32" s="50"/>
       <c r="U32" s="33"/>
@@ -2856,10 +2856,10 @@
         <v>35</v>
       </c>
       <c r="Q34" s="7">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="R34" s="7">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="S34" s="14">
         <v>46016</v>
@@ -2909,7 +2909,7 @@
         <v>35</v>
       </c>
       <c r="Q35" s="7">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="R35" s="7"/>
       <c r="S35" s="14">
@@ -2962,7 +2962,7 @@
       </c>
       <c r="Q36" s="49">
         <f>SUM(Q34:Q35)*30+R34</f>
-        <v>823</v>
+        <v>828</v>
       </c>
       <c r="R36" s="50"/>
       <c r="S36" s="7"/>

</xml_diff>

<commit_message>
Update lot codes - 2025-01-22 09:17:43
</commit_message>
<xml_diff>
--- a/LotCode.xlsx
+++ b/LotCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf.sharepoint.com/sites/production-warehouse/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7129" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B79622C6-E74E-4161-A858-A3523E24195C}"/>
+  <xr:revisionPtr revIDLastSave="7130" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{067CF2CC-6964-4501-8D78-942246605E76}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
   </bookViews>
@@ -1097,7 +1097,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O35" sqref="O35"/>
+      <selection pane="bottomLeft" activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4562,7 +4562,7 @@
     <row r="282" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="283" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" deleteColumns="0" deleteRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="3m+/sAiyTu18zbqFO8q4Cx1g8/pxO1BAFE3y/E5w6Ky70OZDEEXKDIuVB/99KYenwOKq5XsJwLYewU8OtOuj3w==" saltValue="oTtqUHozhy0RIDQsm5OFXQ==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="44">
     <mergeCell ref="X24:Y24"/>
     <mergeCell ref="V26:V27"/>

</xml_diff>

<commit_message>
Update lot codes - 2025-01-22 09:59:48
</commit_message>
<xml_diff>
--- a/LotCode.xlsx
+++ b/LotCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf.sharepoint.com/sites/production-warehouse/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7130" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{067CF2CC-6964-4501-8D78-942246605E76}"/>
+  <xr:revisionPtr revIDLastSave="7133" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2817158D-9936-4510-B75C-504B8EA41158}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
   </bookViews>
@@ -1095,9 +1095,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4D02CE-C7F3-446F-985C-950AF7BFACB9}">
   <dimension ref="A1:AE283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R27" sqref="R27"/>
+      <selection pane="bottomLeft" activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,7 +1213,7 @@
         <v>6</v>
       </c>
       <c r="AC1" s="20">
-        <v>45678</v>
+        <v>45679</v>
       </c>
       <c r="AE1" s="5"/>
     </row>
@@ -1254,7 +1254,7 @@
       </c>
       <c r="F3" s="9">
         <f t="shared" ref="F3:F5" si="0">(E3-$AC$1)/365*12</f>
-        <v>20.580821917808219</v>
+        <v>20.547945205479451</v>
       </c>
       <c r="G3" s="33"/>
       <c r="H3" s="6" t="s">
@@ -1274,7 +1274,7 @@
       </c>
       <c r="M3" s="9">
         <f t="shared" ref="M3:M4" si="1">(L3-$AC$1)/365*12</f>
-        <v>13.676712328767124</v>
+        <v>13.643835616438357</v>
       </c>
       <c r="N3" s="33"/>
       <c r="O3" s="6" t="s">
@@ -1294,7 +1294,7 @@
       </c>
       <c r="T3" s="9">
         <f t="shared" ref="T3:T5" si="2">(S3-$AC$1)/365*12</f>
-        <v>20.153424657534249</v>
+        <v>20.12054794520548</v>
       </c>
       <c r="U3" s="33"/>
       <c r="V3" s="6" t="s">
@@ -1314,7 +1314,7 @@
       </c>
       <c r="AA3" s="9">
         <f t="shared" ref="AA3" si="3">(Z3-$AC$1)/365*12</f>
-        <v>43.232876712328768</v>
+        <v>43.2</v>
       </c>
       <c r="AB3" s="12"/>
     </row>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="F4" s="9">
         <f t="shared" si="0"/>
-        <v>21.205479452054796</v>
+        <v>21.172602739726027</v>
       </c>
       <c r="G4" s="33"/>
       <c r="I4" s="7">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="M4" s="9">
         <f t="shared" si="1"/>
-        <v>20.778082191780822</v>
+        <v>20.745205479452054</v>
       </c>
       <c r="N4" s="33"/>
       <c r="O4" s="27"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="T4" s="9">
         <f t="shared" si="2"/>
-        <v>20.153424657534249</v>
+        <v>20.12054794520548</v>
       </c>
       <c r="U4" s="33"/>
       <c r="W4" s="7" t="s">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="AA4" s="9">
         <f t="shared" ref="AA4" si="4">(Z4-$AC$1)/365*12</f>
-        <v>44.252054794520546</v>
+        <v>44.219178082191782</v>
       </c>
       <c r="AB4" s="7"/>
     </row>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="F5" s="9">
         <f t="shared" si="0"/>
-        <v>21.205479452054796</v>
+        <v>21.172602739726027</v>
       </c>
       <c r="G5" s="33"/>
       <c r="I5" s="46" t="s">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="T5" s="9">
         <f t="shared" si="2"/>
-        <v>24.197260273972603</v>
+        <v>24.164383561643838</v>
       </c>
       <c r="U5" s="33"/>
       <c r="W5" s="46" t="s">
@@ -1486,7 +1486,7 @@
       </c>
       <c r="M7" s="9">
         <f t="shared" ref="M7:M8" si="5">(L7-$AC$1)/365*12</f>
-        <v>16.668493150684931</v>
+        <v>16.635616438356166</v>
       </c>
       <c r="N7" s="33"/>
       <c r="U7" s="33"/>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="AA7" s="9">
         <f t="shared" ref="AA7" si="6">(Z7-$AC$1)/365*12</f>
-        <v>43.232876712328768</v>
+        <v>43.2</v>
       </c>
       <c r="AB7" s="7"/>
     </row>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="F8" s="9">
         <f t="shared" ref="F8" si="7">(E8-$AC$1)/365*12</f>
-        <v>18.805479452054794</v>
+        <v>18.772602739726025</v>
       </c>
       <c r="G8" s="33"/>
       <c r="H8" s="27"/>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="M8" s="9">
         <f t="shared" si="5"/>
-        <v>20.778082191780822</v>
+        <v>20.745205479452054</v>
       </c>
       <c r="N8" s="33"/>
       <c r="O8" s="6" t="s">
@@ -1565,7 +1565,7 @@
       </c>
       <c r="T8" s="9">
         <f t="shared" ref="T8:T10" si="8">(S8-$AC$1)/365*12</f>
-        <v>20.153424657534249</v>
+        <v>20.12054794520548</v>
       </c>
       <c r="U8" s="33"/>
       <c r="W8" s="7" t="s">
@@ -1582,7 +1582,7 @@
       </c>
       <c r="AA8" s="9">
         <f t="shared" ref="AA8" si="9">(Z8-$AC$1)/365*12</f>
-        <v>46.257534246575347</v>
+        <v>46.224657534246575</v>
       </c>
       <c r="AB8" s="7"/>
     </row>
@@ -1600,7 +1600,7 @@
       </c>
       <c r="F9" s="9">
         <f>(E9-$AC$1)/365*12</f>
-        <v>18.805479452054794</v>
+        <v>18.772602739726025</v>
       </c>
       <c r="G9" s="33"/>
       <c r="H9" s="27"/>
@@ -1616,7 +1616,7 @@
       </c>
       <c r="M9" s="9">
         <f t="shared" ref="M9" si="10">(L9-$AC$1)/365*12</f>
-        <v>21.271232876712329</v>
+        <v>21.238356164383561</v>
       </c>
       <c r="N9" s="33"/>
       <c r="P9" s="7" t="s">
@@ -1631,7 +1631,7 @@
       </c>
       <c r="T9" s="9">
         <f t="shared" si="8"/>
-        <v>20.153424657534249</v>
+        <v>20.12054794520548</v>
       </c>
       <c r="U9" s="33"/>
       <c r="W9" s="46" t="s">
@@ -1658,7 +1658,7 @@
       </c>
       <c r="F10" s="9">
         <f>(E10-$AC$1)/365*12</f>
-        <v>19.890410958904109</v>
+        <v>19.857534246575344</v>
       </c>
       <c r="G10" s="33"/>
       <c r="I10" s="46" t="s">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="T10" s="9">
         <f t="shared" si="8"/>
-        <v>24.197260273972603</v>
+        <v>24.164383561643838</v>
       </c>
       <c r="U10" s="33"/>
       <c r="AB10" s="7"/>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="F11" s="9">
         <f>(E11-$AC$1)/365*12</f>
-        <v>21.238356164383561</v>
+        <v>21.205479452054796</v>
       </c>
       <c r="G11" s="33"/>
       <c r="K11" s="7"/>
@@ -1732,7 +1732,7 @@
       </c>
       <c r="AA11" s="9">
         <f t="shared" ref="AA11:AA12" si="11">(Z11-$AC$1)/365*12</f>
-        <v>43.232876712328768</v>
+        <v>43.2</v>
       </c>
       <c r="AB11" s="7"/>
     </row>
@@ -1764,7 +1764,7 @@
       </c>
       <c r="M12" s="9">
         <f>(L12-$AC$1)/365*12</f>
-        <v>20.81095890410959</v>
+        <v>20.778082191780822</v>
       </c>
       <c r="N12" s="33"/>
       <c r="U12" s="33"/>
@@ -1780,7 +1780,7 @@
       </c>
       <c r="AA12" s="9">
         <f t="shared" si="11"/>
-        <v>44.252054794520546</v>
+        <v>44.219178082191782</v>
       </c>
       <c r="AB12" s="7"/>
     </row>
@@ -1801,7 +1801,7 @@
       </c>
       <c r="M13" s="9">
         <f>(L13-$AC$1)/365*12</f>
-        <v>21.698630136986299</v>
+        <v>21.665753424657535</v>
       </c>
       <c r="N13" s="33"/>
       <c r="O13" s="6" t="s">
@@ -1821,7 +1821,7 @@
       </c>
       <c r="T13" s="9">
         <f t="shared" ref="T13:T14" si="12">(S13-$AC$1)/365*12</f>
-        <v>17.128767123287673</v>
+        <v>17.095890410958901</v>
       </c>
       <c r="U13" s="33"/>
       <c r="W13" s="46" t="s">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="M14" s="9">
         <f>(L14-$AC$1)/365*12</f>
-        <v>22.389041095890413</v>
+        <v>22.356164383561641</v>
       </c>
       <c r="N14" s="33"/>
       <c r="O14" s="27"/>
@@ -1879,7 +1879,7 @@
       </c>
       <c r="T14" s="9">
         <f t="shared" si="12"/>
-        <v>21.139726027397259</v>
+        <v>21.106849315068494</v>
       </c>
       <c r="U14" s="33"/>
       <c r="AB14" s="7"/>
@@ -1897,7 +1897,7 @@
       </c>
       <c r="F15" s="9">
         <f>(E15-$AC$1)/365*12</f>
-        <v>18.772602739726025</v>
+        <v>18.739726027397261</v>
       </c>
       <c r="G15" s="33"/>
       <c r="I15" s="46" t="s">
@@ -1935,7 +1935,7 @@
       </c>
       <c r="AA15" s="9">
         <f t="shared" ref="AA15" si="13">(Z15-$AC$1)/365*12</f>
-        <v>43.232876712328768</v>
+        <v>43.2</v>
       </c>
       <c r="AB15" s="7"/>
     </row>
@@ -1952,7 +1952,7 @@
       </c>
       <c r="F16" s="9">
         <f t="shared" ref="F16:F17" si="14">(E16-$AC$1)/365*12</f>
-        <v>19.890410958904109</v>
+        <v>19.857534246575344</v>
       </c>
       <c r="G16" s="33"/>
       <c r="K16" s="7"/>
@@ -1973,7 +1973,7 @@
       </c>
       <c r="AA16" s="9">
         <f t="shared" ref="AA16:AA17" si="15">(Z16-$AC$1)/365*12</f>
-        <v>44.252054794520546</v>
+        <v>44.219178082191782</v>
       </c>
       <c r="AB16" s="8"/>
     </row>
@@ -1990,7 +1990,7 @@
       </c>
       <c r="F17" s="9">
         <f t="shared" si="14"/>
-        <v>20.876712328767123</v>
+        <v>20.843835616438355</v>
       </c>
       <c r="G17" s="33"/>
       <c r="H17" s="6" t="s">
@@ -2010,7 +2010,7 @@
       </c>
       <c r="M17" s="9">
         <f t="shared" ref="M17:M18" si="16">(L17-$AC$1)/365*12</f>
-        <v>20.778082191780822</v>
+        <v>20.745205479452054</v>
       </c>
       <c r="N17" s="33"/>
       <c r="O17" s="6" t="s">
@@ -2030,7 +2030,7 @@
       </c>
       <c r="T17" s="9">
         <f t="shared" ref="T17" si="17">(S17-$AC$1)/365*12</f>
-        <v>17.128767123287673</v>
+        <v>17.095890410958901</v>
       </c>
       <c r="U17" s="33"/>
       <c r="V17" s="6"/>
@@ -2048,7 +2048,7 @@
       </c>
       <c r="AA17" s="9">
         <f t="shared" si="15"/>
-        <v>46.257534246575347</v>
+        <v>46.224657534246575</v>
       </c>
       <c r="AB17" s="7"/>
     </row>
@@ -2076,7 +2076,7 @@
       </c>
       <c r="M18" s="9">
         <f t="shared" si="16"/>
-        <v>21.271232876712329</v>
+        <v>21.238356164383561</v>
       </c>
       <c r="N18" s="33"/>
       <c r="P18" s="7" t="s">
@@ -2093,7 +2093,7 @@
       </c>
       <c r="T18" s="9">
         <f t="shared" ref="T18" si="18">(S18-$AC$1)/365*12</f>
-        <v>21.139726027397259</v>
+        <v>21.106849315068494</v>
       </c>
       <c r="U18" s="33"/>
       <c r="W18" s="46" t="s">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="F20" s="9">
         <f>(E20-$AC$1)/365*12</f>
-        <v>17.095890410958901</v>
+        <v>17.063013698630137</v>
       </c>
       <c r="G20" s="33"/>
       <c r="K20" s="7"/>
@@ -2178,7 +2178,7 @@
       </c>
       <c r="AA20" s="9">
         <f>(Z20-$AC$1)/365*12</f>
-        <v>43.232876712328768</v>
+        <v>43.2</v>
       </c>
       <c r="AB20" s="7"/>
     </row>
@@ -2195,7 +2195,7 @@
       </c>
       <c r="F21" s="9">
         <f t="shared" ref="F21" si="19">(E21-$AC$1)/365*12</f>
-        <v>19.890410958904109</v>
+        <v>19.857534246575344</v>
       </c>
       <c r="G21" s="33"/>
       <c r="H21" s="6" t="s">
@@ -2215,7 +2215,7 @@
       </c>
       <c r="M21" s="9">
         <f t="shared" ref="M21" si="20">(L21-$AC$1)/365*12</f>
-        <v>20.153424657534249</v>
+        <v>20.12054794520548</v>
       </c>
       <c r="N21" s="33"/>
       <c r="O21" s="6" t="s">
@@ -2235,7 +2235,7 @@
       </c>
       <c r="T21" s="9">
         <f t="shared" ref="T21:T22" si="21">(S21-$AC$1)/365*12</f>
-        <v>20.153424657534249</v>
+        <v>20.12054794520548</v>
       </c>
       <c r="U21" s="33"/>
       <c r="W21" s="46" t="s">
@@ -2271,7 +2271,7 @@
       </c>
       <c r="M22" s="9">
         <f t="shared" ref="M22:M23" si="22">(L22-$AC$1)/365*12</f>
-        <v>20.153424657534249</v>
+        <v>20.12054794520548</v>
       </c>
       <c r="N22" s="33"/>
       <c r="P22" s="7" t="s">
@@ -2286,7 +2286,7 @@
       </c>
       <c r="T22" s="9">
         <f t="shared" si="21"/>
-        <v>20.153424657534249</v>
+        <v>20.12054794520548</v>
       </c>
       <c r="U22" s="33"/>
       <c r="AB22" s="7"/>
@@ -2310,7 +2310,7 @@
       </c>
       <c r="M23" s="9">
         <f t="shared" si="22"/>
-        <v>22.158904109589042</v>
+        <v>22.126027397260273</v>
       </c>
       <c r="N23" s="33"/>
       <c r="P23" s="46" t="s">
@@ -2339,7 +2339,7 @@
       </c>
       <c r="AA23" s="9">
         <f t="shared" ref="AA23" si="23">(Z23-$AC$1)/365*12</f>
-        <v>43.232876712328768</v>
+        <v>43.2</v>
       </c>
       <c r="AB23" s="7"/>
     </row>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="F24" s="9">
         <f>(E24-$AC$1)/365*12</f>
-        <v>16.832876712328769</v>
+        <v>16.799999999999997</v>
       </c>
       <c r="G24" s="33"/>
       <c r="I24" s="46" t="s">
@@ -2398,7 +2398,7 @@
       </c>
       <c r="F25" s="9">
         <f>(E25-$AC$1)/365*12</f>
-        <v>20.515068493150686</v>
+        <v>20.482191780821918</v>
       </c>
       <c r="G25" s="33"/>
       <c r="K25" s="7"/>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="T25" s="9">
         <f t="shared" ref="T25:T27" si="24">(S25-$AC$1)/365*12</f>
-        <v>17.128767123287673</v>
+        <v>17.095890410958901</v>
       </c>
       <c r="U25" s="33"/>
       <c r="AB25" s="7"/>
@@ -2456,7 +2456,7 @@
       </c>
       <c r="M26" s="9">
         <f t="shared" ref="M26:M27" si="25">(L26-$AC$1)/365*12</f>
-        <v>20.153424657534249</v>
+        <v>20.12054794520548</v>
       </c>
       <c r="N26" s="33"/>
       <c r="P26" s="7" t="s">
@@ -2473,7 +2473,7 @@
       </c>
       <c r="T26" s="9">
         <f t="shared" si="24"/>
-        <v>17.128767123287673</v>
+        <v>17.095890410958901</v>
       </c>
       <c r="U26" s="33"/>
       <c r="V26" s="52" t="s">
@@ -2493,7 +2493,7 @@
       </c>
       <c r="AA26" s="9">
         <f t="shared" ref="AA26:AA27" si="26">(Z26-$AC$1)/365*12</f>
-        <v>36.230136986301368</v>
+        <v>36.197260273972603</v>
       </c>
       <c r="AB26" s="7"/>
     </row>
@@ -2514,7 +2514,7 @@
       </c>
       <c r="M27" s="9">
         <f t="shared" si="25"/>
-        <v>22.158904109589042</v>
+        <v>22.126027397260273</v>
       </c>
       <c r="N27" s="33"/>
       <c r="P27" s="7" t="s">
@@ -2531,7 +2531,7 @@
       </c>
       <c r="T27" s="9">
         <f t="shared" si="24"/>
-        <v>22.158904109589042</v>
+        <v>22.126027397260273</v>
       </c>
       <c r="U27" s="33"/>
       <c r="V27" s="52"/>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="AA27" s="9">
         <f t="shared" si="26"/>
-        <v>46.257534246575347</v>
+        <v>46.224657534246575</v>
       </c>
       <c r="AB27" s="7"/>
     </row>
@@ -2571,7 +2571,7 @@
       </c>
       <c r="F28" s="9">
         <f>(E28-$AC$1)/365*12</f>
-        <v>16.865753424657534</v>
+        <v>16.832876712328769</v>
       </c>
       <c r="G28" s="33"/>
       <c r="I28" s="46" t="s">
@@ -2616,7 +2616,7 @@
       </c>
       <c r="F29" s="9">
         <f>(E29-$AC$1)/365*12</f>
-        <v>17.523287671232879</v>
+        <v>17.490410958904111</v>
       </c>
       <c r="G29" s="33"/>
       <c r="K29" s="7"/>
@@ -2652,7 +2652,7 @@
       </c>
       <c r="M30" s="16">
         <f t="shared" ref="M30" si="27">(L30-$AC$1)/365*12</f>
-        <v>-4.9315068493150687</v>
+        <v>-4.9643835616438361</v>
       </c>
       <c r="N30" s="33"/>
       <c r="O30" s="6" t="s">
@@ -2672,7 +2672,7 @@
       </c>
       <c r="T30" s="9">
         <f t="shared" ref="T30:T31" si="28">(S30-$AC$1)/365*12</f>
-        <v>22.158904109589042</v>
+        <v>22.126027397260273</v>
       </c>
       <c r="U30" s="33"/>
       <c r="V30" s="6" t="s">
@@ -2692,7 +2692,7 @@
       </c>
       <c r="AA30" s="9">
         <f t="shared" ref="AA30:AA31" si="29">(Z30-$AC$1)/365*12</f>
-        <v>21.139726027397259</v>
+        <v>21.106849315068494</v>
       </c>
     </row>
     <row r="31" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2722,7 +2722,7 @@
       </c>
       <c r="T31" s="9">
         <f t="shared" si="28"/>
-        <v>22.158904109589042</v>
+        <v>22.126027397260273</v>
       </c>
       <c r="U31" s="33"/>
       <c r="W31" s="7" t="s">
@@ -2737,7 +2737,7 @@
       </c>
       <c r="AA31" s="9">
         <f t="shared" si="29"/>
-        <v>21.139726027397259</v>
+        <v>21.106849315068494</v>
       </c>
       <c r="AB31" s="7"/>
     </row>
@@ -2759,7 +2759,7 @@
       </c>
       <c r="F32" s="9">
         <f>(E32-$AC$1)/365*12</f>
-        <v>17.523287671232879</v>
+        <v>17.490410958904111</v>
       </c>
       <c r="G32" s="33"/>
       <c r="K32" s="7"/>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="F33" s="9">
         <f>(E33-$AC$1)/365*12</f>
-        <v>20.843835616438355</v>
+        <v>20.81095890410959</v>
       </c>
       <c r="G33" s="33"/>
       <c r="H33" s="17" t="s">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="M33" s="9">
         <f t="shared" ref="M33:M34" si="30">(L33-$AC$1)/365*12</f>
-        <v>20.613698630136987</v>
+        <v>20.580821917808219</v>
       </c>
       <c r="N33" s="33"/>
       <c r="U33" s="33"/>
@@ -2846,7 +2846,7 @@
       </c>
       <c r="M34" s="9">
         <f t="shared" si="30"/>
-        <v>20.613698630136987</v>
+        <v>20.580821917808219</v>
       </c>
       <c r="N34" s="33"/>
       <c r="O34" s="6" t="s">
@@ -2866,7 +2866,7 @@
       </c>
       <c r="T34" s="9">
         <f>(S34-$AC$1)/365*12</f>
-        <v>11.112328767123287</v>
+        <v>11.079452054794521</v>
       </c>
       <c r="U34" s="33"/>
       <c r="V34" s="6" t="s">
@@ -2886,7 +2886,7 @@
       </c>
       <c r="AA34" s="26">
         <f t="shared" ref="AA34" si="31">(Z34-$AC$1)/365*12</f>
-        <v>21.139726027397259</v>
+        <v>21.106849315068494</v>
       </c>
       <c r="AB34" s="7"/>
     </row>
@@ -2917,7 +2917,7 @@
       </c>
       <c r="T35" s="9">
         <f>(S35-$AC$1)/365*12</f>
-        <v>11.112328767123287</v>
+        <v>11.079452054794521</v>
       </c>
       <c r="U35" s="33"/>
       <c r="V35" s="6"/>
@@ -2952,7 +2952,7 @@
       </c>
       <c r="F36" s="9">
         <f>(E36-$AC$1)/365*12</f>
-        <v>19.134246575342466</v>
+        <v>19.101369863013698</v>
       </c>
       <c r="G36" s="33"/>
       <c r="K36" s="7"/>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="F37" s="9">
         <f>(E37-$AC$1)/365*12</f>
-        <v>20.153424657534249</v>
+        <v>20.12054794520548</v>
       </c>
       <c r="G37" s="33"/>
       <c r="H37" s="6" t="s">
@@ -3011,7 +3011,7 @@
       </c>
       <c r="M37" s="9">
         <f t="shared" ref="M37:M38" si="32">(L37-$AC$1)/365*12</f>
-        <v>20.613698630136987</v>
+        <v>20.580821917808219</v>
       </c>
       <c r="N37" s="33"/>
       <c r="P37" s="13"/>
@@ -3034,7 +3034,7 @@
       </c>
       <c r="F38" s="9">
         <f>(E38-$AC$1)/365*12</f>
-        <v>22.158904109589042</v>
+        <v>22.126027397260273</v>
       </c>
       <c r="G38" s="33"/>
       <c r="I38" s="7">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="M38" s="9">
         <f t="shared" si="32"/>
-        <v>20.613698630136987</v>
+        <v>20.580821917808219</v>
       </c>
       <c r="N38" s="33"/>
       <c r="O38" s="6" t="s">
@@ -3069,7 +3069,7 @@
       </c>
       <c r="T38" s="9">
         <f>(S38-$AC$1)/365*12</f>
-        <v>17.128767123287673</v>
+        <v>17.095890410958901</v>
       </c>
       <c r="U38" s="33"/>
       <c r="V38" s="6" t="s">
@@ -3087,7 +3087,7 @@
       </c>
       <c r="AA38" s="9">
         <f t="shared" ref="AA38" si="33">(Z38-$AC$1)/365*12</f>
-        <v>10.126027397260273</v>
+        <v>10.093150684931507</v>
       </c>
       <c r="AB38" s="7"/>
     </row>
@@ -3124,7 +3124,7 @@
       </c>
       <c r="T39" s="9">
         <f>(S39-$AC$1)/365*12</f>
-        <v>17.128767123287673</v>
+        <v>17.095890410958901</v>
       </c>
       <c r="U39" s="33"/>
       <c r="W39" s="46" t="s">
@@ -3161,7 +3161,7 @@
       </c>
       <c r="T40" s="9">
         <f>(S40-$AC$1)/365*12</f>
-        <v>22.158904109589042</v>
+        <v>22.126027397260273</v>
       </c>
       <c r="U40" s="34"/>
       <c r="AB40" s="7"/>
@@ -3184,7 +3184,7 @@
       </c>
       <c r="F41" s="9">
         <f>(E41-$AC$1)/365*12</f>
-        <v>19.134246575342466</v>
+        <v>19.101369863013698</v>
       </c>
       <c r="G41" s="33"/>
       <c r="H41" s="6" t="s">
@@ -3204,7 +3204,7 @@
       </c>
       <c r="M41" s="9">
         <f t="shared" ref="M41:M42" si="34">(L41-$AC$1)/365*12</f>
-        <v>17.063013698630137</v>
+        <v>17.030136986301368</v>
       </c>
       <c r="N41" s="33"/>
       <c r="P41" s="46" t="s">
@@ -3232,7 +3232,7 @@
       </c>
       <c r="F42" s="9">
         <f>(E42-$AC$1)/365*12</f>
-        <v>20.153424657534249</v>
+        <v>20.12054794520548</v>
       </c>
       <c r="G42" s="33"/>
       <c r="H42" s="27"/>
@@ -3248,7 +3248,7 @@
       </c>
       <c r="M42" s="9">
         <f t="shared" si="34"/>
-        <v>17.063013698630137</v>
+        <v>17.030136986301368</v>
       </c>
       <c r="N42" s="33"/>
       <c r="U42" s="24"/>
@@ -3312,7 +3312,7 @@
       </c>
       <c r="F45" s="9">
         <f t="shared" ref="F45:F46" si="35">(E45-$AC$1)/365*12</f>
-        <v>20.153424657534249</v>
+        <v>20.12054794520548</v>
       </c>
       <c r="G45" s="33"/>
       <c r="H45" s="6" t="s">
@@ -3332,7 +3332,7 @@
       </c>
       <c r="M45" s="9">
         <f t="shared" ref="M45:M46" si="36">(L45-$AC$1)/365*12</f>
-        <v>17.063013698630137</v>
+        <v>17.030136986301368</v>
       </c>
       <c r="N45" s="33"/>
       <c r="O45" s="6" t="s">
@@ -3360,7 +3360,7 @@
       </c>
       <c r="F46" s="9">
         <f t="shared" si="35"/>
-        <v>22.158904109589042</v>
+        <v>22.126027397260273</v>
       </c>
       <c r="G46" s="33"/>
       <c r="I46" s="7">
@@ -3375,7 +3375,7 @@
       </c>
       <c r="M46" s="9">
         <f t="shared" si="36"/>
-        <v>20.547945205479451</v>
+        <v>20.515068493150686</v>
       </c>
       <c r="N46" s="33"/>
       <c r="U46" s="24"/>
@@ -3435,7 +3435,7 @@
       </c>
       <c r="F49" s="9">
         <f t="shared" ref="F49:F50" si="37">(E49-$AC$1)/365*12</f>
-        <v>19.134246575342466</v>
+        <v>19.101369863013698</v>
       </c>
       <c r="G49" s="33"/>
       <c r="I49" s="11"/>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="F50" s="9">
         <f t="shared" si="37"/>
-        <v>20.153424657534249</v>
+        <v>20.12054794520548</v>
       </c>
       <c r="G50" s="33"/>
       <c r="I50" s="39"/>
@@ -3519,7 +3519,7 @@
       </c>
       <c r="F53" s="16">
         <f>(E53-$AC$1)/365*12</f>
-        <v>-4.9315068493150687</v>
+        <v>-4.9643835616438361</v>
       </c>
       <c r="G53" s="33"/>
       <c r="K53" s="7"/>
@@ -4562,7 +4562,7 @@
     <row r="282" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="283" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="3m+/sAiyTu18zbqFO8q4Cx1g8/pxO1BAFE3y/E5w6Ky70OZDEEXKDIuVB/99KYenwOKq5XsJwLYewU8OtOuj3w==" saltValue="oTtqUHozhy0RIDQsm5OFXQ==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" deleteColumns="0" deleteRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="95L7QmuvYaUtSthXtNxsnKMYJFF5kqgYchCbnCX2fYGwRgTDf/0kDfTQF4FnOK5CJ046N/FD1ZcN4V0u8fOm9w==" saltValue="CM301zdGMq/RSSSdcorVnA==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="44">
     <mergeCell ref="X24:Y24"/>
     <mergeCell ref="V26:V27"/>

</xml_diff>

<commit_message>
Update lot codes - 2025-01-28 11:54:33
</commit_message>
<xml_diff>
--- a/LotCode.xlsx
+++ b/LotCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf.sharepoint.com/sites/production-warehouse/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7133" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2817158D-9936-4510-B75C-504B8EA41158}"/>
+  <xr:revisionPtr revIDLastSave="7137" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3047D4B3-5527-4EDA-9455-2A9E63DAB8C2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$AA$61</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -346,9 +345,6 @@
     <t>PRSS2414</t>
   </si>
   <si>
-    <t>1024CC206</t>
-  </si>
-  <si>
     <t>1124FH308</t>
   </si>
   <si>
@@ -377,6 +373,9 @@
   </si>
   <si>
     <t>1.21.25</t>
+  </si>
+  <si>
+    <t>1024S206</t>
   </si>
 </sst>
 </file>
@@ -747,11 +746,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1096,8 +1095,8 @@
   <dimension ref="A1:AE283"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC2" sqref="AC2"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC36" sqref="AC36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,19 +1218,19 @@
     </row>
     <row r="2" spans="1:31" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G2" s="32"/>
       <c r="H2" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N2" s="32"/>
       <c r="O2" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="U2" s="32"/>
       <c r="V2" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AB2" s="8"/>
       <c r="AE2" s="18"/>
@@ -1410,7 +1409,7 @@
       <c r="N5" s="33"/>
       <c r="O5" s="27"/>
       <c r="P5" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q5" s="7">
         <v>195</v>
@@ -1671,7 +1670,7 @@
       <c r="K10" s="50"/>
       <c r="N10" s="33"/>
       <c r="P10" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q10" s="7">
         <v>173</v>
@@ -1716,7 +1715,7 @@
       <c r="R11" s="50"/>
       <c r="U11" s="33"/>
       <c r="V11" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="W11" s="7" t="s">
         <v>15</v>
@@ -2185,7 +2184,7 @@
     <row r="21" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="27"/>
       <c r="B21" s="44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C21" s="7">
         <v>149</v>
@@ -2297,7 +2296,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="33"/>
       <c r="I23" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J23" s="7">
         <v>86</v>
@@ -2476,7 +2475,7 @@
         <v>17.095890410958901</v>
       </c>
       <c r="U26" s="33"/>
-      <c r="V26" s="52" t="s">
+      <c r="V26" s="51" t="s">
         <v>78</v>
       </c>
       <c r="W26" s="7" t="s">
@@ -2503,7 +2502,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="33"/>
       <c r="I27" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J27" s="7">
         <v>75</v>
@@ -2534,7 +2533,7 @@
         <v>22.126027397260273</v>
       </c>
       <c r="U27" s="33"/>
-      <c r="V27" s="52"/>
+      <c r="V27" s="51"/>
       <c r="W27" s="7" t="s">
         <v>91</v>
       </c>
@@ -2873,7 +2872,7 @@
         <v>39</v>
       </c>
       <c r="W34" s="11" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="X34" s="11">
         <v>7</v>
@@ -2922,7 +2921,7 @@
       <c r="U35" s="33"/>
       <c r="V35" s="6"/>
       <c r="W35" s="11" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="X35" s="11">
         <v>73</v>
@@ -3023,7 +3022,7 @@
     </row>
     <row r="38" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C38" s="40">
         <v>85</v>
@@ -3347,7 +3346,7 @@
     <row r="46" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
       <c r="B46" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C46" s="11">
         <v>55</v>
@@ -3467,8 +3466,8 @@
       </c>
       <c r="G50" s="33"/>
       <c r="I50" s="39"/>
-      <c r="J50" s="51"/>
-      <c r="K50" s="51"/>
+      <c r="J50" s="52"/>
+      <c r="K50" s="52"/>
       <c r="L50" s="24"/>
       <c r="M50" s="24"/>
       <c r="N50" s="24"/>
@@ -4562,37 +4561,8 @@
     <row r="282" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="283" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="95L7QmuvYaUtSthXtNxsnKMYJFF5kqgYchCbnCX2fYGwRgTDf/0kDfTQF4FnOK5CJ046N/FD1ZcN4V0u8fOm9w==" saltValue="CM301zdGMq/RSSSdcorVnA==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" deleteColumns="0" deleteRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="IRERHQb2wZFLERXF8rb2y0YWpmBLXl8oTaMA7JYja/VGMEwuqcGF/ZkAFjc+8wS+10fgvnEuAHNDnim7CRjVfA==" saltValue="j363xL+t5UEaQA6DziEa0A==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="44">
-    <mergeCell ref="X24:Y24"/>
-    <mergeCell ref="V26:V27"/>
-    <mergeCell ref="X32:Y32"/>
-    <mergeCell ref="X28:Y28"/>
-    <mergeCell ref="X39:Y39"/>
-    <mergeCell ref="X36:Y36"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="X9:Y9"/>
-    <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="X18:Y18"/>
-    <mergeCell ref="X21:Y21"/>
-    <mergeCell ref="Q41:R41"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="J19:K19"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="C47:D47"/>
     <mergeCell ref="C54:D54"/>
@@ -4608,6 +4578,35 @@
     <mergeCell ref="J31:K31"/>
     <mergeCell ref="J35:K35"/>
     <mergeCell ref="J39:K39"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="Q41:R41"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="X9:Y9"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="X18:Y18"/>
+    <mergeCell ref="X21:Y21"/>
+    <mergeCell ref="X24:Y24"/>
+    <mergeCell ref="V26:V27"/>
+    <mergeCell ref="X32:Y32"/>
+    <mergeCell ref="X28:Y28"/>
+    <mergeCell ref="X39:Y39"/>
+    <mergeCell ref="X36:Y36"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4625,15 +4624,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e752113-b2fb-4b78-ae69-b10b93a6ace4">
@@ -4642,6 +4632,15 @@
     <TaxCatchAll xmlns="a2a82fc2-af7c-43c6-84e4-151c3b8f78f4" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4886,20 +4885,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64C959BB-4F03-4A27-81AC-6DE1AA020D13}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E564C7A4-BCA4-4794-8A6C-B04A14263787}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="4e752113-b2fb-4b78-ae69-b10b93a6ace4"/>
     <ds:schemaRef ds:uri="a2a82fc2-af7c-43c6-84e4-151c3b8f78f4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64C959BB-4F03-4A27-81AC-6DE1AA020D13}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update lot codes - 2025-01-28 12:11:21
</commit_message>
<xml_diff>
--- a/LotCode.xlsx
+++ b/LotCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf.sharepoint.com/sites/production-warehouse/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7137" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3047D4B3-5527-4EDA-9455-2A9E63DAB8C2}"/>
+  <xr:revisionPtr revIDLastSave="7140" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AA55172-BE88-4692-9370-50287B9D76D7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
   </bookViews>
@@ -1096,7 +1096,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC36" sqref="AC36"/>
+      <selection pane="bottomLeft" activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,7 +1212,7 @@
         <v>6</v>
       </c>
       <c r="AC1" s="20">
-        <v>45679</v>
+        <v>45684</v>
       </c>
       <c r="AE1" s="5"/>
     </row>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="F3" s="9">
         <f t="shared" ref="F3:F5" si="0">(E3-$AC$1)/365*12</f>
-        <v>20.547945205479451</v>
+        <v>20.383561643835616</v>
       </c>
       <c r="G3" s="33"/>
       <c r="H3" s="6" t="s">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="M3" s="9">
         <f t="shared" ref="M3:M4" si="1">(L3-$AC$1)/365*12</f>
-        <v>13.643835616438357</v>
+        <v>13.479452054794521</v>
       </c>
       <c r="N3" s="33"/>
       <c r="O3" s="6" t="s">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="T3" s="9">
         <f t="shared" ref="T3:T5" si="2">(S3-$AC$1)/365*12</f>
-        <v>20.12054794520548</v>
+        <v>19.956164383561642</v>
       </c>
       <c r="U3" s="33"/>
       <c r="V3" s="6" t="s">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="AA3" s="9">
         <f t="shared" ref="AA3" si="3">(Z3-$AC$1)/365*12</f>
-        <v>43.2</v>
+        <v>43.035616438356165</v>
       </c>
       <c r="AB3" s="12"/>
     </row>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="F4" s="9">
         <f t="shared" si="0"/>
-        <v>21.172602739726027</v>
+        <v>21.008219178082193</v>
       </c>
       <c r="G4" s="33"/>
       <c r="I4" s="7">
@@ -1345,7 +1345,7 @@
       </c>
       <c r="M4" s="9">
         <f t="shared" si="1"/>
-        <v>20.745205479452054</v>
+        <v>20.580821917808219</v>
       </c>
       <c r="N4" s="33"/>
       <c r="O4" s="27"/>
@@ -1361,7 +1361,7 @@
       </c>
       <c r="T4" s="9">
         <f t="shared" si="2"/>
-        <v>20.12054794520548</v>
+        <v>19.956164383561642</v>
       </c>
       <c r="U4" s="33"/>
       <c r="W4" s="7" t="s">
@@ -1378,7 +1378,7 @@
       </c>
       <c r="AA4" s="9">
         <f t="shared" ref="AA4" si="4">(Z4-$AC$1)/365*12</f>
-        <v>44.219178082191782</v>
+        <v>44.054794520547944</v>
       </c>
       <c r="AB4" s="7"/>
     </row>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="F5" s="9">
         <f t="shared" si="0"/>
-        <v>21.172602739726027</v>
+        <v>21.008219178082193</v>
       </c>
       <c r="G5" s="33"/>
       <c r="I5" s="46" t="s">
@@ -1422,7 +1422,7 @@
       </c>
       <c r="T5" s="9">
         <f t="shared" si="2"/>
-        <v>24.164383561643838</v>
+        <v>24</v>
       </c>
       <c r="U5" s="33"/>
       <c r="W5" s="46" t="s">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="M7" s="9">
         <f t="shared" ref="M7:M8" si="5">(L7-$AC$1)/365*12</f>
-        <v>16.635616438356166</v>
+        <v>16.471232876712328</v>
       </c>
       <c r="N7" s="33"/>
       <c r="U7" s="33"/>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="AA7" s="9">
         <f t="shared" ref="AA7" si="6">(Z7-$AC$1)/365*12</f>
-        <v>43.2</v>
+        <v>43.035616438356165</v>
       </c>
       <c r="AB7" s="7"/>
     </row>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="F8" s="9">
         <f t="shared" ref="F8" si="7">(E8-$AC$1)/365*12</f>
-        <v>18.772602739726025</v>
+        <v>18.608219178082194</v>
       </c>
       <c r="G8" s="33"/>
       <c r="H8" s="27"/>
@@ -1544,7 +1544,7 @@
       </c>
       <c r="M8" s="9">
         <f t="shared" si="5"/>
-        <v>20.745205479452054</v>
+        <v>20.580821917808219</v>
       </c>
       <c r="N8" s="33"/>
       <c r="O8" s="6" t="s">
@@ -1564,7 +1564,7 @@
       </c>
       <c r="T8" s="9">
         <f t="shared" ref="T8:T10" si="8">(S8-$AC$1)/365*12</f>
-        <v>20.12054794520548</v>
+        <v>19.956164383561642</v>
       </c>
       <c r="U8" s="33"/>
       <c r="W8" s="7" t="s">
@@ -1581,7 +1581,7 @@
       </c>
       <c r="AA8" s="9">
         <f t="shared" ref="AA8" si="9">(Z8-$AC$1)/365*12</f>
-        <v>46.224657534246575</v>
+        <v>46.060273972602737</v>
       </c>
       <c r="AB8" s="7"/>
     </row>
@@ -1599,7 +1599,7 @@
       </c>
       <c r="F9" s="9">
         <f>(E9-$AC$1)/365*12</f>
-        <v>18.772602739726025</v>
+        <v>18.608219178082194</v>
       </c>
       <c r="G9" s="33"/>
       <c r="H9" s="27"/>
@@ -1615,7 +1615,7 @@
       </c>
       <c r="M9" s="9">
         <f t="shared" ref="M9" si="10">(L9-$AC$1)/365*12</f>
-        <v>21.238356164383561</v>
+        <v>21.073972602739726</v>
       </c>
       <c r="N9" s="33"/>
       <c r="P9" s="7" t="s">
@@ -1630,7 +1630,7 @@
       </c>
       <c r="T9" s="9">
         <f t="shared" si="8"/>
-        <v>20.12054794520548</v>
+        <v>19.956164383561642</v>
       </c>
       <c r="U9" s="33"/>
       <c r="W9" s="46" t="s">
@@ -1657,7 +1657,7 @@
       </c>
       <c r="F10" s="9">
         <f>(E10-$AC$1)/365*12</f>
-        <v>19.857534246575344</v>
+        <v>19.693150684931506</v>
       </c>
       <c r="G10" s="33"/>
       <c r="I10" s="46" t="s">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="T10" s="9">
         <f t="shared" si="8"/>
-        <v>24.164383561643838</v>
+        <v>24</v>
       </c>
       <c r="U10" s="33"/>
       <c r="AB10" s="7"/>
@@ -1700,7 +1700,7 @@
       </c>
       <c r="F11" s="9">
         <f>(E11-$AC$1)/365*12</f>
-        <v>21.205479452054796</v>
+        <v>21.041095890410958</v>
       </c>
       <c r="G11" s="33"/>
       <c r="K11" s="7"/>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="AA11" s="9">
         <f t="shared" ref="AA11:AA12" si="11">(Z11-$AC$1)/365*12</f>
-        <v>43.2</v>
+        <v>43.035616438356165</v>
       </c>
       <c r="AB11" s="7"/>
     </row>
@@ -1763,7 +1763,7 @@
       </c>
       <c r="M12" s="9">
         <f>(L12-$AC$1)/365*12</f>
-        <v>20.778082191780822</v>
+        <v>20.613698630136987</v>
       </c>
       <c r="N12" s="33"/>
       <c r="U12" s="33"/>
@@ -1779,7 +1779,7 @@
       </c>
       <c r="AA12" s="9">
         <f t="shared" si="11"/>
-        <v>44.219178082191782</v>
+        <v>44.054794520547944</v>
       </c>
       <c r="AB12" s="7"/>
     </row>
@@ -1800,7 +1800,7 @@
       </c>
       <c r="M13" s="9">
         <f>(L13-$AC$1)/365*12</f>
-        <v>21.665753424657535</v>
+        <v>21.5013698630137</v>
       </c>
       <c r="N13" s="33"/>
       <c r="O13" s="6" t="s">
@@ -1820,7 +1820,7 @@
       </c>
       <c r="T13" s="9">
         <f t="shared" ref="T13:T14" si="12">(S13-$AC$1)/365*12</f>
-        <v>17.095890410958901</v>
+        <v>16.93150684931507</v>
       </c>
       <c r="U13" s="33"/>
       <c r="W13" s="46" t="s">
@@ -1860,7 +1860,7 @@
       </c>
       <c r="M14" s="9">
         <f>(L14-$AC$1)/365*12</f>
-        <v>22.356164383561641</v>
+        <v>22.19178082191781</v>
       </c>
       <c r="N14" s="33"/>
       <c r="O14" s="27"/>
@@ -1878,7 +1878,7 @@
       </c>
       <c r="T14" s="9">
         <f t="shared" si="12"/>
-        <v>21.106849315068494</v>
+        <v>20.942465753424656</v>
       </c>
       <c r="U14" s="33"/>
       <c r="AB14" s="7"/>
@@ -1896,7 +1896,7 @@
       </c>
       <c r="F15" s="9">
         <f>(E15-$AC$1)/365*12</f>
-        <v>18.739726027397261</v>
+        <v>18.575342465753423</v>
       </c>
       <c r="G15" s="33"/>
       <c r="I15" s="46" t="s">
@@ -1934,7 +1934,7 @@
       </c>
       <c r="AA15" s="9">
         <f t="shared" ref="AA15" si="13">(Z15-$AC$1)/365*12</f>
-        <v>43.2</v>
+        <v>43.035616438356165</v>
       </c>
       <c r="AB15" s="7"/>
     </row>
@@ -1951,7 +1951,7 @@
       </c>
       <c r="F16" s="9">
         <f t="shared" ref="F16:F17" si="14">(E16-$AC$1)/365*12</f>
-        <v>19.857534246575344</v>
+        <v>19.693150684931506</v>
       </c>
       <c r="G16" s="33"/>
       <c r="K16" s="7"/>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="AA16" s="9">
         <f t="shared" ref="AA16:AA17" si="15">(Z16-$AC$1)/365*12</f>
-        <v>44.219178082191782</v>
+        <v>44.054794520547944</v>
       </c>
       <c r="AB16" s="8"/>
     </row>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="F17" s="9">
         <f t="shared" si="14"/>
-        <v>20.843835616438355</v>
+        <v>20.67945205479452</v>
       </c>
       <c r="G17" s="33"/>
       <c r="H17" s="6" t="s">
@@ -2009,7 +2009,7 @@
       </c>
       <c r="M17" s="9">
         <f t="shared" ref="M17:M18" si="16">(L17-$AC$1)/365*12</f>
-        <v>20.745205479452054</v>
+        <v>20.580821917808219</v>
       </c>
       <c r="N17" s="33"/>
       <c r="O17" s="6" t="s">
@@ -2029,7 +2029,7 @@
       </c>
       <c r="T17" s="9">
         <f t="shared" ref="T17" si="17">(S17-$AC$1)/365*12</f>
-        <v>17.095890410958901</v>
+        <v>16.93150684931507</v>
       </c>
       <c r="U17" s="33"/>
       <c r="V17" s="6"/>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="AA17" s="9">
         <f t="shared" si="15"/>
-        <v>46.224657534246575</v>
+        <v>46.060273972602737</v>
       </c>
       <c r="AB17" s="7"/>
     </row>
@@ -2075,7 +2075,7 @@
       </c>
       <c r="M18" s="9">
         <f t="shared" si="16"/>
-        <v>21.238356164383561</v>
+        <v>21.073972602739726</v>
       </c>
       <c r="N18" s="33"/>
       <c r="P18" s="7" t="s">
@@ -2092,7 +2092,7 @@
       </c>
       <c r="T18" s="9">
         <f t="shared" ref="T18" si="18">(S18-$AC$1)/365*12</f>
-        <v>21.106849315068494</v>
+        <v>20.942465753424656</v>
       </c>
       <c r="U18" s="33"/>
       <c r="W18" s="46" t="s">
@@ -2150,7 +2150,7 @@
       </c>
       <c r="F20" s="9">
         <f>(E20-$AC$1)/365*12</f>
-        <v>17.063013698630137</v>
+        <v>16.898630136986302</v>
       </c>
       <c r="G20" s="33"/>
       <c r="K20" s="7"/>
@@ -2177,7 +2177,7 @@
       </c>
       <c r="AA20" s="9">
         <f>(Z20-$AC$1)/365*12</f>
-        <v>43.2</v>
+        <v>43.035616438356165</v>
       </c>
       <c r="AB20" s="7"/>
     </row>
@@ -2194,7 +2194,7 @@
       </c>
       <c r="F21" s="9">
         <f t="shared" ref="F21" si="19">(E21-$AC$1)/365*12</f>
-        <v>19.857534246575344</v>
+        <v>19.693150684931506</v>
       </c>
       <c r="G21" s="33"/>
       <c r="H21" s="6" t="s">
@@ -2214,7 +2214,7 @@
       </c>
       <c r="M21" s="9">
         <f t="shared" ref="M21" si="20">(L21-$AC$1)/365*12</f>
-        <v>20.12054794520548</v>
+        <v>19.956164383561642</v>
       </c>
       <c r="N21" s="33"/>
       <c r="O21" s="6" t="s">
@@ -2234,7 +2234,7 @@
       </c>
       <c r="T21" s="9">
         <f t="shared" ref="T21:T22" si="21">(S21-$AC$1)/365*12</f>
-        <v>20.12054794520548</v>
+        <v>19.956164383561642</v>
       </c>
       <c r="U21" s="33"/>
       <c r="W21" s="46" t="s">
@@ -2270,7 +2270,7 @@
       </c>
       <c r="M22" s="9">
         <f t="shared" ref="M22:M23" si="22">(L22-$AC$1)/365*12</f>
-        <v>20.12054794520548</v>
+        <v>19.956164383561642</v>
       </c>
       <c r="N22" s="33"/>
       <c r="P22" s="7" t="s">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="T22" s="9">
         <f t="shared" si="21"/>
-        <v>20.12054794520548</v>
+        <v>19.956164383561642</v>
       </c>
       <c r="U22" s="33"/>
       <c r="AB22" s="7"/>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="M23" s="9">
         <f t="shared" si="22"/>
-        <v>22.126027397260273</v>
+        <v>21.961643835616439</v>
       </c>
       <c r="N23" s="33"/>
       <c r="P23" s="46" t="s">
@@ -2338,7 +2338,7 @@
       </c>
       <c r="AA23" s="9">
         <f t="shared" ref="AA23" si="23">(Z23-$AC$1)/365*12</f>
-        <v>43.2</v>
+        <v>43.035616438356165</v>
       </c>
       <c r="AB23" s="7"/>
     </row>
@@ -2360,7 +2360,7 @@
       </c>
       <c r="F24" s="9">
         <f>(E24-$AC$1)/365*12</f>
-        <v>16.799999999999997</v>
+        <v>16.635616438356166</v>
       </c>
       <c r="G24" s="33"/>
       <c r="I24" s="46" t="s">
@@ -2397,7 +2397,7 @@
       </c>
       <c r="F25" s="9">
         <f>(E25-$AC$1)/365*12</f>
-        <v>20.482191780821918</v>
+        <v>20.317808219178083</v>
       </c>
       <c r="G25" s="33"/>
       <c r="K25" s="7"/>
@@ -2422,7 +2422,7 @@
       </c>
       <c r="T25" s="9">
         <f t="shared" ref="T25:T27" si="24">(S25-$AC$1)/365*12</f>
-        <v>17.095890410958901</v>
+        <v>16.93150684931507</v>
       </c>
       <c r="U25" s="33"/>
       <c r="AB25" s="7"/>
@@ -2455,7 +2455,7 @@
       </c>
       <c r="M26" s="9">
         <f t="shared" ref="M26:M27" si="25">(L26-$AC$1)/365*12</f>
-        <v>20.12054794520548</v>
+        <v>19.956164383561642</v>
       </c>
       <c r="N26" s="33"/>
       <c r="P26" s="7" t="s">
@@ -2472,7 +2472,7 @@
       </c>
       <c r="T26" s="9">
         <f t="shared" si="24"/>
-        <v>17.095890410958901</v>
+        <v>16.93150684931507</v>
       </c>
       <c r="U26" s="33"/>
       <c r="V26" s="51" t="s">
@@ -2492,7 +2492,7 @@
       </c>
       <c r="AA26" s="9">
         <f t="shared" ref="AA26:AA27" si="26">(Z26-$AC$1)/365*12</f>
-        <v>36.197260273972603</v>
+        <v>36.032876712328772</v>
       </c>
       <c r="AB26" s="7"/>
     </row>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="M27" s="9">
         <f t="shared" si="25"/>
-        <v>22.126027397260273</v>
+        <v>21.961643835616439</v>
       </c>
       <c r="N27" s="33"/>
       <c r="P27" s="7" t="s">
@@ -2530,7 +2530,7 @@
       </c>
       <c r="T27" s="9">
         <f t="shared" si="24"/>
-        <v>22.126027397260273</v>
+        <v>21.961643835616439</v>
       </c>
       <c r="U27" s="33"/>
       <c r="V27" s="51"/>
@@ -2548,7 +2548,7 @@
       </c>
       <c r="AA27" s="9">
         <f t="shared" si="26"/>
-        <v>46.224657534246575</v>
+        <v>46.060273972602737</v>
       </c>
       <c r="AB27" s="7"/>
     </row>
@@ -2570,7 +2570,7 @@
       </c>
       <c r="F28" s="9">
         <f>(E28-$AC$1)/365*12</f>
-        <v>16.832876712328769</v>
+        <v>16.668493150684931</v>
       </c>
       <c r="G28" s="33"/>
       <c r="I28" s="46" t="s">
@@ -2615,7 +2615,7 @@
       </c>
       <c r="F29" s="9">
         <f>(E29-$AC$1)/365*12</f>
-        <v>17.490410958904111</v>
+        <v>17.326027397260273</v>
       </c>
       <c r="G29" s="33"/>
       <c r="K29" s="7"/>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="M30" s="16">
         <f t="shared" ref="M30" si="27">(L30-$AC$1)/365*12</f>
-        <v>-4.9643835616438361</v>
+        <v>-5.1287671232876715</v>
       </c>
       <c r="N30" s="33"/>
       <c r="O30" s="6" t="s">
@@ -2671,7 +2671,7 @@
       </c>
       <c r="T30" s="9">
         <f t="shared" ref="T30:T31" si="28">(S30-$AC$1)/365*12</f>
-        <v>22.126027397260273</v>
+        <v>21.961643835616439</v>
       </c>
       <c r="U30" s="33"/>
       <c r="V30" s="6" t="s">
@@ -2691,7 +2691,7 @@
       </c>
       <c r="AA30" s="9">
         <f t="shared" ref="AA30:AA31" si="29">(Z30-$AC$1)/365*12</f>
-        <v>21.106849315068494</v>
+        <v>20.942465753424656</v>
       </c>
     </row>
     <row r="31" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2721,7 +2721,7 @@
       </c>
       <c r="T31" s="9">
         <f t="shared" si="28"/>
-        <v>22.126027397260273</v>
+        <v>21.961643835616439</v>
       </c>
       <c r="U31" s="33"/>
       <c r="W31" s="7" t="s">
@@ -2736,7 +2736,7 @@
       </c>
       <c r="AA31" s="9">
         <f t="shared" si="29"/>
-        <v>21.106849315068494</v>
+        <v>20.942465753424656</v>
       </c>
       <c r="AB31" s="7"/>
     </row>
@@ -2758,7 +2758,7 @@
       </c>
       <c r="F32" s="9">
         <f>(E32-$AC$1)/365*12</f>
-        <v>17.490410958904111</v>
+        <v>17.326027397260273</v>
       </c>
       <c r="G32" s="33"/>
       <c r="K32" s="7"/>
@@ -2796,7 +2796,7 @@
       </c>
       <c r="F33" s="9">
         <f>(E33-$AC$1)/365*12</f>
-        <v>20.81095890410959</v>
+        <v>20.646575342465752</v>
       </c>
       <c r="G33" s="33"/>
       <c r="H33" s="17" t="s">
@@ -2816,7 +2816,7 @@
       </c>
       <c r="M33" s="9">
         <f t="shared" ref="M33:M34" si="30">(L33-$AC$1)/365*12</f>
-        <v>20.580821917808219</v>
+        <v>20.416438356164385</v>
       </c>
       <c r="N33" s="33"/>
       <c r="U33" s="33"/>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="M34" s="9">
         <f t="shared" si="30"/>
-        <v>20.580821917808219</v>
+        <v>20.416438356164385</v>
       </c>
       <c r="N34" s="33"/>
       <c r="O34" s="6" t="s">
@@ -2865,7 +2865,7 @@
       </c>
       <c r="T34" s="9">
         <f>(S34-$AC$1)/365*12</f>
-        <v>11.079452054794521</v>
+        <v>10.915068493150685</v>
       </c>
       <c r="U34" s="33"/>
       <c r="V34" s="6" t="s">
@@ -2885,7 +2885,7 @@
       </c>
       <c r="AA34" s="26">
         <f t="shared" ref="AA34" si="31">(Z34-$AC$1)/365*12</f>
-        <v>21.106849315068494</v>
+        <v>20.942465753424656</v>
       </c>
       <c r="AB34" s="7"/>
     </row>
@@ -2916,7 +2916,7 @@
       </c>
       <c r="T35" s="9">
         <f>(S35-$AC$1)/365*12</f>
-        <v>11.079452054794521</v>
+        <v>10.915068493150685</v>
       </c>
       <c r="U35" s="33"/>
       <c r="V35" s="6"/>
@@ -2951,7 +2951,7 @@
       </c>
       <c r="F36" s="9">
         <f>(E36-$AC$1)/365*12</f>
-        <v>19.101369863013698</v>
+        <v>18.936986301369863</v>
       </c>
       <c r="G36" s="33"/>
       <c r="K36" s="7"/>
@@ -2990,7 +2990,7 @@
       </c>
       <c r="F37" s="9">
         <f>(E37-$AC$1)/365*12</f>
-        <v>20.12054794520548</v>
+        <v>19.956164383561642</v>
       </c>
       <c r="G37" s="33"/>
       <c r="H37" s="6" t="s">
@@ -3010,7 +3010,7 @@
       </c>
       <c r="M37" s="9">
         <f t="shared" ref="M37:M38" si="32">(L37-$AC$1)/365*12</f>
-        <v>20.580821917808219</v>
+        <v>20.416438356164385</v>
       </c>
       <c r="N37" s="33"/>
       <c r="P37" s="13"/>
@@ -3033,7 +3033,7 @@
       </c>
       <c r="F38" s="9">
         <f>(E38-$AC$1)/365*12</f>
-        <v>22.126027397260273</v>
+        <v>21.961643835616439</v>
       </c>
       <c r="G38" s="33"/>
       <c r="I38" s="7">
@@ -3048,7 +3048,7 @@
       </c>
       <c r="M38" s="9">
         <f t="shared" si="32"/>
-        <v>20.580821917808219</v>
+        <v>20.416438356164385</v>
       </c>
       <c r="N38" s="33"/>
       <c r="O38" s="6" t="s">
@@ -3068,7 +3068,7 @@
       </c>
       <c r="T38" s="9">
         <f>(S38-$AC$1)/365*12</f>
-        <v>17.095890410958901</v>
+        <v>16.93150684931507</v>
       </c>
       <c r="U38" s="33"/>
       <c r="V38" s="6" t="s">
@@ -3086,7 +3086,7 @@
       </c>
       <c r="AA38" s="9">
         <f t="shared" ref="AA38" si="33">(Z38-$AC$1)/365*12</f>
-        <v>10.093150684931507</v>
+        <v>9.9287671232876722</v>
       </c>
       <c r="AB38" s="7"/>
     </row>
@@ -3123,7 +3123,7 @@
       </c>
       <c r="T39" s="9">
         <f>(S39-$AC$1)/365*12</f>
-        <v>17.095890410958901</v>
+        <v>16.93150684931507</v>
       </c>
       <c r="U39" s="33"/>
       <c r="W39" s="46" t="s">
@@ -3160,7 +3160,7 @@
       </c>
       <c r="T40" s="9">
         <f>(S40-$AC$1)/365*12</f>
-        <v>22.126027397260273</v>
+        <v>21.961643835616439</v>
       </c>
       <c r="U40" s="34"/>
       <c r="AB40" s="7"/>
@@ -3183,7 +3183,7 @@
       </c>
       <c r="F41" s="9">
         <f>(E41-$AC$1)/365*12</f>
-        <v>19.101369863013698</v>
+        <v>18.936986301369863</v>
       </c>
       <c r="G41" s="33"/>
       <c r="H41" s="6" t="s">
@@ -3203,7 +3203,7 @@
       </c>
       <c r="M41" s="9">
         <f t="shared" ref="M41:M42" si="34">(L41-$AC$1)/365*12</f>
-        <v>17.030136986301368</v>
+        <v>16.865753424657534</v>
       </c>
       <c r="N41" s="33"/>
       <c r="P41" s="46" t="s">
@@ -3231,7 +3231,7 @@
       </c>
       <c r="F42" s="9">
         <f>(E42-$AC$1)/365*12</f>
-        <v>20.12054794520548</v>
+        <v>19.956164383561642</v>
       </c>
       <c r="G42" s="33"/>
       <c r="H42" s="27"/>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="M42" s="9">
         <f t="shared" si="34"/>
-        <v>17.030136986301368</v>
+        <v>16.865753424657534</v>
       </c>
       <c r="N42" s="33"/>
       <c r="U42" s="24"/>
@@ -3311,7 +3311,7 @@
       </c>
       <c r="F45" s="9">
         <f t="shared" ref="F45:F46" si="35">(E45-$AC$1)/365*12</f>
-        <v>20.12054794520548</v>
+        <v>19.956164383561642</v>
       </c>
       <c r="G45" s="33"/>
       <c r="H45" s="6" t="s">
@@ -3331,7 +3331,7 @@
       </c>
       <c r="M45" s="9">
         <f t="shared" ref="M45:M46" si="36">(L45-$AC$1)/365*12</f>
-        <v>17.030136986301368</v>
+        <v>16.865753424657534</v>
       </c>
       <c r="N45" s="33"/>
       <c r="O45" s="6" t="s">
@@ -3359,7 +3359,7 @@
       </c>
       <c r="F46" s="9">
         <f t="shared" si="35"/>
-        <v>22.126027397260273</v>
+        <v>21.961643835616439</v>
       </c>
       <c r="G46" s="33"/>
       <c r="I46" s="7">
@@ -3374,7 +3374,7 @@
       </c>
       <c r="M46" s="9">
         <f t="shared" si="36"/>
-        <v>20.515068493150686</v>
+        <v>20.350684931506848</v>
       </c>
       <c r="N46" s="33"/>
       <c r="U46" s="24"/>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="F49" s="9">
         <f t="shared" ref="F49:F50" si="37">(E49-$AC$1)/365*12</f>
-        <v>19.101369863013698</v>
+        <v>18.936986301369863</v>
       </c>
       <c r="G49" s="33"/>
       <c r="I49" s="11"/>
@@ -3462,7 +3462,7 @@
       </c>
       <c r="F50" s="9">
         <f t="shared" si="37"/>
-        <v>20.12054794520548</v>
+        <v>19.956164383561642</v>
       </c>
       <c r="G50" s="33"/>
       <c r="I50" s="39"/>
@@ -3518,7 +3518,7 @@
       </c>
       <c r="F53" s="16">
         <f>(E53-$AC$1)/365*12</f>
-        <v>-4.9643835616438361</v>
+        <v>-5.1287671232876715</v>
       </c>
       <c r="G53" s="33"/>
       <c r="K53" s="7"/>
@@ -4561,7 +4561,7 @@
     <row r="282" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="283" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="IRERHQb2wZFLERXF8rb2y0YWpmBLXl8oTaMA7JYja/VGMEwuqcGF/ZkAFjc+8wS+10fgvnEuAHNDnim7CRjVfA==" saltValue="j363xL+t5UEaQA6DziEa0A==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" deleteColumns="0" deleteRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="hgUFn575gqca0prUo1kzidQgsek8GSKkwOaoB0KUCdxEzuLhA4OEV/jcGIx2oPHvXyzS8wkCblhHr48ywSU39w==" saltValue="nE8R7BaEmtFYW8RZfIRObA==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="44">
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="C47:D47"/>

</xml_diff>

<commit_message>
Update lot codes - 2025-01-29 08:16:02
</commit_message>
<xml_diff>
--- a/LotCode.xlsx
+++ b/LotCode.xlsx
@@ -8,9 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf.sharepoint.com/sites/production-warehouse/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7140" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AA55172-BE88-4692-9370-50287B9D76D7}"/>
+  <xr:revisionPtr revIDLastSave="7155" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5F2CE1C-246A-4A34-9B24-EBC8CA5D5B14}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="a/VZ8kgdZMyU/a42HcB04O8OBNrnh4WxCIPRCv9GqcObOgYeM9oYcSfQqndR/nnirMykfzLaq88Ahwir6HajhQ==" workbookSaltValue="jsEDzk1n/+JkLoe+dWrmxg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
+    <workbookView minimized="1" xWindow="3645" yWindow="1935" windowWidth="21660" windowHeight="11265" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="105">
   <si>
     <t>SKU</t>
   </si>
@@ -162,9 +163,6 @@
     <t>0822EJ2401</t>
   </si>
   <si>
-    <t>PRIDSG0031</t>
-  </si>
-  <si>
     <t>OMEGA-ALG</t>
   </si>
   <si>
@@ -342,9 +340,6 @@
     <t>161797</t>
   </si>
   <si>
-    <t>PRSS2414</t>
-  </si>
-  <si>
     <t>1124FH308</t>
   </si>
   <si>
@@ -376,6 +371,12 @@
   </si>
   <si>
     <t>1024S206</t>
+  </si>
+  <si>
+    <t>1.29.25</t>
+  </si>
+  <si>
+    <t>PRSS2411-4</t>
   </si>
 </sst>
 </file>
@@ -1094,9 +1095,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4D02CE-C7F3-446F-985C-950AF7BFACB9}">
   <dimension ref="A1:AE283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC2" sqref="AC2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC16" sqref="AC16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,32 +1213,32 @@
         <v>6</v>
       </c>
       <c r="AC1" s="20">
-        <v>45684</v>
+        <v>45686</v>
       </c>
       <c r="AE1" s="5"/>
     </row>
     <row r="2" spans="1:31" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="42" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G2" s="32"/>
       <c r="H2" s="23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N2" s="32"/>
       <c r="O2" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="U2" s="32"/>
       <c r="V2" s="42" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="AB2" s="8"/>
       <c r="AE2" s="18"/>
     </row>
     <row r="3" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="40">
         <v>159368</v>
@@ -1253,11 +1254,11 @@
       </c>
       <c r="F3" s="9">
         <f t="shared" ref="F3:F5" si="0">(E3-$AC$1)/365*12</f>
-        <v>20.383561643835616</v>
+        <v>20.317808219178083</v>
       </c>
       <c r="G3" s="33"/>
       <c r="H3" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I3" s="7">
         <v>155511</v>
@@ -1273,7 +1274,7 @@
       </c>
       <c r="M3" s="9">
         <f t="shared" ref="M3:M4" si="1">(L3-$AC$1)/365*12</f>
-        <v>13.479452054794521</v>
+        <v>13.413698630136988</v>
       </c>
       <c r="N3" s="33"/>
       <c r="O3" s="6" t="s">
@@ -1293,11 +1294,11 @@
       </c>
       <c r="T3" s="9">
         <f t="shared" ref="T3:T5" si="2">(S3-$AC$1)/365*12</f>
-        <v>19.956164383561642</v>
+        <v>19.890410958904109</v>
       </c>
       <c r="U3" s="33"/>
       <c r="V3" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="W3" s="7" t="s">
         <v>8</v>
@@ -1313,7 +1314,7 @@
       </c>
       <c r="AA3" s="9">
         <f t="shared" ref="AA3" si="3">(Z3-$AC$1)/365*12</f>
-        <v>43.035616438356165</v>
+        <v>42.969863013698628</v>
       </c>
       <c r="AB3" s="12"/>
     </row>
@@ -1330,7 +1331,7 @@
       </c>
       <c r="F4" s="9">
         <f t="shared" si="0"/>
-        <v>21.008219178082193</v>
+        <v>20.942465753424656</v>
       </c>
       <c r="G4" s="33"/>
       <c r="I4" s="7">
@@ -1345,7 +1346,7 @@
       </c>
       <c r="M4" s="9">
         <f t="shared" si="1"/>
-        <v>20.580821917808219</v>
+        <v>20.515068493150686</v>
       </c>
       <c r="N4" s="33"/>
       <c r="O4" s="27"/>
@@ -1361,14 +1362,14 @@
       </c>
       <c r="T4" s="9">
         <f t="shared" si="2"/>
-        <v>19.956164383561642</v>
+        <v>19.890410958904109</v>
       </c>
       <c r="U4" s="33"/>
       <c r="W4" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="X4" s="15">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="Y4" s="7">
         <v>1</v>
@@ -1378,7 +1379,7 @@
       </c>
       <c r="AA4" s="9">
         <f t="shared" ref="AA4" si="4">(Z4-$AC$1)/365*12</f>
-        <v>44.054794520547944</v>
+        <v>43.989041095890407</v>
       </c>
       <c r="AB4" s="7"/>
     </row>
@@ -1395,7 +1396,7 @@
       </c>
       <c r="F5" s="9">
         <f t="shared" si="0"/>
-        <v>21.008219178082193</v>
+        <v>20.942465753424656</v>
       </c>
       <c r="G5" s="33"/>
       <c r="I5" s="46" t="s">
@@ -1409,7 +1410,7 @@
       <c r="N5" s="33"/>
       <c r="O5" s="27"/>
       <c r="P5" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Q5" s="7">
         <v>195</v>
@@ -1422,7 +1423,7 @@
       </c>
       <c r="T5" s="9">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>23.934246575342467</v>
       </c>
       <c r="U5" s="33"/>
       <c r="W5" s="46" t="s">
@@ -1430,7 +1431,7 @@
       </c>
       <c r="X5" s="49">
         <f>SUM(X3:X4)*6+Y3+Y4</f>
-        <v>1096</v>
+        <v>1102</v>
       </c>
       <c r="Y5" s="50"/>
       <c r="AB5" s="7"/>
@@ -1469,7 +1470,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="33"/>
       <c r="H7" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I7" s="7">
         <v>156645</v>
@@ -1485,12 +1486,12 @@
       </c>
       <c r="M7" s="9">
         <f t="shared" ref="M7:M8" si="5">(L7-$AC$1)/365*12</f>
-        <v>16.471232876712328</v>
+        <v>16.405479452054795</v>
       </c>
       <c r="N7" s="33"/>
       <c r="U7" s="33"/>
       <c r="V7" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="W7" s="7" t="s">
         <v>13</v>
@@ -1506,13 +1507,13 @@
       </c>
       <c r="AA7" s="9">
         <f t="shared" ref="AA7" si="6">(Z7-$AC$1)/365*12</f>
-        <v>43.035616438356165</v>
+        <v>42.969863013698628</v>
       </c>
       <c r="AB7" s="7"/>
     </row>
     <row r="8" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="7">
         <v>158583</v>
@@ -1528,7 +1529,7 @@
       </c>
       <c r="F8" s="9">
         <f t="shared" ref="F8" si="7">(E8-$AC$1)/365*12</f>
-        <v>18.608219178082194</v>
+        <v>18.542465753424658</v>
       </c>
       <c r="G8" s="33"/>
       <c r="H8" s="27"/>
@@ -1544,14 +1545,14 @@
       </c>
       <c r="M8" s="9">
         <f t="shared" si="5"/>
-        <v>20.580821917808219</v>
+        <v>20.515068493150686</v>
       </c>
       <c r="N8" s="33"/>
       <c r="O8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q8" s="7">
         <v>9</v>
@@ -1564,14 +1565,14 @@
       </c>
       <c r="T8" s="9">
         <f t="shared" ref="T8:T10" si="8">(S8-$AC$1)/365*12</f>
-        <v>19.956164383561642</v>
+        <v>19.890410958904109</v>
       </c>
       <c r="U8" s="33"/>
       <c r="W8" s="7" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="X8" s="7">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="Y8" s="7">
         <v>2</v>
@@ -1581,7 +1582,7 @@
       </c>
       <c r="AA8" s="9">
         <f t="shared" ref="AA8" si="9">(Z8-$AC$1)/365*12</f>
-        <v>46.060273972602737</v>
+        <v>45.994520547945207</v>
       </c>
       <c r="AB8" s="7"/>
     </row>
@@ -1599,7 +1600,7 @@
       </c>
       <c r="F9" s="9">
         <f>(E9-$AC$1)/365*12</f>
-        <v>18.608219178082194</v>
+        <v>18.542465753424658</v>
       </c>
       <c r="G9" s="33"/>
       <c r="H9" s="27"/>
@@ -1615,11 +1616,11 @@
       </c>
       <c r="M9" s="9">
         <f t="shared" ref="M9" si="10">(L9-$AC$1)/365*12</f>
-        <v>21.073972602739726</v>
+        <v>21.008219178082193</v>
       </c>
       <c r="N9" s="33"/>
       <c r="P9" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q9" s="7">
         <v>29</v>
@@ -1630,7 +1631,7 @@
       </c>
       <c r="T9" s="9">
         <f t="shared" si="8"/>
-        <v>19.956164383561642</v>
+        <v>19.890410958904109</v>
       </c>
       <c r="U9" s="33"/>
       <c r="W9" s="46" t="s">
@@ -1638,7 +1639,7 @@
       </c>
       <c r="X9" s="49">
         <f>SUM(X7:X8)*6+Y7+Y8</f>
-        <v>522</v>
+        <v>444</v>
       </c>
       <c r="Y9" s="50"/>
       <c r="AB9" s="7"/>
@@ -1657,7 +1658,7 @@
       </c>
       <c r="F10" s="9">
         <f>(E10-$AC$1)/365*12</f>
-        <v>19.693150684931506</v>
+        <v>19.627397260273973</v>
       </c>
       <c r="G10" s="33"/>
       <c r="I10" s="46" t="s">
@@ -1670,7 +1671,7 @@
       <c r="K10" s="50"/>
       <c r="N10" s="33"/>
       <c r="P10" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="Q10" s="7">
         <v>173</v>
@@ -1681,7 +1682,7 @@
       </c>
       <c r="T10" s="9">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>23.934246575342467</v>
       </c>
       <c r="U10" s="33"/>
       <c r="AB10" s="7"/>
@@ -1700,7 +1701,7 @@
       </c>
       <c r="F11" s="9">
         <f>(E11-$AC$1)/365*12</f>
-        <v>21.041095890410958</v>
+        <v>20.975342465753425</v>
       </c>
       <c r="G11" s="33"/>
       <c r="K11" s="7"/>
@@ -1715,7 +1716,7 @@
       <c r="R11" s="50"/>
       <c r="U11" s="33"/>
       <c r="V11" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="W11" s="7" t="s">
         <v>15</v>
@@ -1731,7 +1732,7 @@
       </c>
       <c r="AA11" s="9">
         <f t="shared" ref="AA11:AA12" si="11">(Z11-$AC$1)/365*12</f>
-        <v>43.035616438356165</v>
+        <v>42.969863013698628</v>
       </c>
       <c r="AB11" s="7"/>
     </row>
@@ -1747,7 +1748,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="33"/>
       <c r="H12" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I12" s="7">
         <v>163239</v>
@@ -1763,15 +1764,15 @@
       </c>
       <c r="M12" s="9">
         <f>(L12-$AC$1)/365*12</f>
-        <v>20.613698630136987</v>
+        <v>20.547945205479451</v>
       </c>
       <c r="N12" s="33"/>
       <c r="U12" s="33"/>
       <c r="W12" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="X12" s="7">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="Y12" s="7"/>
       <c r="Z12" s="14">
@@ -1779,7 +1780,7 @@
       </c>
       <c r="AA12" s="9">
         <f t="shared" si="11"/>
-        <v>44.054794520547944</v>
+        <v>43.989041095890407</v>
       </c>
       <c r="AB12" s="7"/>
     </row>
@@ -1800,7 +1801,7 @@
       </c>
       <c r="M13" s="9">
         <f>(L13-$AC$1)/365*12</f>
-        <v>21.5013698630137</v>
+        <v>21.435616438356163</v>
       </c>
       <c r="N13" s="33"/>
       <c r="O13" s="6" t="s">
@@ -1820,7 +1821,7 @@
       </c>
       <c r="T13" s="9">
         <f t="shared" ref="T13:T14" si="12">(S13-$AC$1)/365*12</f>
-        <v>16.93150684931507</v>
+        <v>16.865753424657534</v>
       </c>
       <c r="U13" s="33"/>
       <c r="W13" s="46" t="s">
@@ -1828,14 +1829,14 @@
       </c>
       <c r="X13" s="49">
         <f>SUM(X11:X12)*6+Y11+Y12</f>
-        <v>1086</v>
+        <v>1230</v>
       </c>
       <c r="Y13" s="50"/>
       <c r="AB13" s="7"/>
     </row>
     <row r="14" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="35">
         <v>158221</v>
@@ -1860,12 +1861,12 @@
       </c>
       <c r="M14" s="9">
         <f>(L14-$AC$1)/365*12</f>
-        <v>22.19178082191781</v>
+        <v>22.126027397260273</v>
       </c>
       <c r="N14" s="33"/>
       <c r="O14" s="27"/>
       <c r="P14" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q14" s="7">
         <v>120</v>
@@ -1878,7 +1879,7 @@
       </c>
       <c r="T14" s="9">
         <f t="shared" si="12"/>
-        <v>20.942465753424656</v>
+        <v>20.876712328767123</v>
       </c>
       <c r="U14" s="33"/>
       <c r="AB14" s="7"/>
@@ -1896,7 +1897,7 @@
       </c>
       <c r="F15" s="9">
         <f>(E15-$AC$1)/365*12</f>
-        <v>18.575342465753423</v>
+        <v>18.509589041095889</v>
       </c>
       <c r="G15" s="33"/>
       <c r="I15" s="46" t="s">
@@ -1918,7 +1919,7 @@
       <c r="R15" s="50"/>
       <c r="U15" s="33"/>
       <c r="V15" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W15" s="7" t="s">
         <v>18</v>
@@ -1934,7 +1935,7 @@
       </c>
       <c r="AA15" s="9">
         <f t="shared" ref="AA15" si="13">(Z15-$AC$1)/365*12</f>
-        <v>43.035616438356165</v>
+        <v>42.969863013698628</v>
       </c>
       <c r="AB15" s="7"/>
     </row>
@@ -1951,7 +1952,7 @@
       </c>
       <c r="F16" s="9">
         <f t="shared" ref="F16:F17" si="14">(E16-$AC$1)/365*12</f>
-        <v>19.693150684931506</v>
+        <v>19.627397260273973</v>
       </c>
       <c r="G16" s="33"/>
       <c r="K16" s="7"/>
@@ -1959,7 +1960,7 @@
       <c r="U16" s="33"/>
       <c r="V16" s="6"/>
       <c r="W16" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="X16" s="7">
         <v>15</v>
@@ -1972,7 +1973,7 @@
       </c>
       <c r="AA16" s="9">
         <f t="shared" ref="AA16:AA17" si="15">(Z16-$AC$1)/365*12</f>
-        <v>44.054794520547944</v>
+        <v>43.989041095890407</v>
       </c>
       <c r="AB16" s="8"/>
     </row>
@@ -1989,11 +1990,11 @@
       </c>
       <c r="F17" s="9">
         <f t="shared" si="14"/>
-        <v>20.67945205479452</v>
+        <v>20.613698630136987</v>
       </c>
       <c r="G17" s="33"/>
       <c r="H17" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I17" s="7">
         <v>163238</v>
@@ -2009,14 +2010,14 @@
       </c>
       <c r="M17" s="9">
         <f t="shared" ref="M17:M18" si="16">(L17-$AC$1)/365*12</f>
-        <v>20.580821917808219</v>
+        <v>20.515068493150686</v>
       </c>
       <c r="N17" s="33"/>
       <c r="O17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="P17" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q17" s="7">
         <v>9</v>
@@ -2029,15 +2030,15 @@
       </c>
       <c r="T17" s="9">
         <f t="shared" ref="T17" si="17">(S17-$AC$1)/365*12</f>
-        <v>16.93150684931507</v>
+        <v>16.865753424657534</v>
       </c>
       <c r="U17" s="33"/>
       <c r="V17" s="6"/>
       <c r="W17" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="X17" s="7">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="Y17" s="7">
         <v>2</v>
@@ -2047,7 +2048,7 @@
       </c>
       <c r="AA17" s="9">
         <f t="shared" si="15"/>
-        <v>46.060273972602737</v>
+        <v>45.994520547945207</v>
       </c>
       <c r="AB17" s="7"/>
     </row>
@@ -2075,11 +2076,11 @@
       </c>
       <c r="M18" s="9">
         <f t="shared" si="16"/>
-        <v>21.073972602739726</v>
+        <v>21.008219178082193</v>
       </c>
       <c r="N18" s="33"/>
       <c r="P18" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q18" s="7">
         <v>36</v>
@@ -2092,7 +2093,7 @@
       </c>
       <c r="T18" s="9">
         <f t="shared" ref="T18" si="18">(S18-$AC$1)/365*12</f>
-        <v>20.942465753424656</v>
+        <v>20.876712328767123</v>
       </c>
       <c r="U18" s="33"/>
       <c r="W18" s="46" t="s">
@@ -2100,7 +2101,7 @@
       </c>
       <c r="X18" s="49">
         <f>SUM(X15:X17)*6+Y15+Y16</f>
-        <v>685</v>
+        <v>625</v>
       </c>
       <c r="Y18" s="50"/>
       <c r="AB18" s="7"/>
@@ -2134,10 +2135,10 @@
     </row>
     <row r="20" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="11">
         <v>6</v>
@@ -2150,7 +2151,7 @@
       </c>
       <c r="F20" s="9">
         <f>(E20-$AC$1)/365*12</f>
-        <v>16.898630136986302</v>
+        <v>16.832876712328769</v>
       </c>
       <c r="G20" s="33"/>
       <c r="K20" s="7"/>
@@ -2177,14 +2178,14 @@
       </c>
       <c r="AA20" s="9">
         <f>(Z20-$AC$1)/365*12</f>
-        <v>43.035616438356165</v>
+        <v>42.969863013698628</v>
       </c>
       <c r="AB20" s="7"/>
     </row>
     <row r="21" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="27"/>
       <c r="B21" s="44" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C21" s="7">
         <v>149</v>
@@ -2194,7 +2195,7 @@
       </c>
       <c r="F21" s="9">
         <f t="shared" ref="F21" si="19">(E21-$AC$1)/365*12</f>
-        <v>19.693150684931506</v>
+        <v>19.627397260273973</v>
       </c>
       <c r="G21" s="33"/>
       <c r="H21" s="6" t="s">
@@ -2214,14 +2215,14 @@
       </c>
       <c r="M21" s="9">
         <f t="shared" ref="M21" si="20">(L21-$AC$1)/365*12</f>
-        <v>19.956164383561642</v>
+        <v>19.890410958904109</v>
       </c>
       <c r="N21" s="33"/>
       <c r="O21" s="6" t="s">
         <v>21</v>
       </c>
       <c r="P21" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q21" s="7">
         <v>9</v>
@@ -2234,7 +2235,7 @@
       </c>
       <c r="T21" s="9">
         <f t="shared" ref="T21:T22" si="21">(S21-$AC$1)/365*12</f>
-        <v>19.956164383561642</v>
+        <v>19.890410958904109</v>
       </c>
       <c r="U21" s="33"/>
       <c r="W21" s="46" t="s">
@@ -2270,11 +2271,11 @@
       </c>
       <c r="M22" s="9">
         <f t="shared" ref="M22:M23" si="22">(L22-$AC$1)/365*12</f>
-        <v>19.956164383561642</v>
+        <v>19.890410958904109</v>
       </c>
       <c r="N22" s="33"/>
       <c r="P22" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q22" s="7">
         <v>52</v>
@@ -2285,7 +2286,7 @@
       </c>
       <c r="T22" s="9">
         <f t="shared" si="21"/>
-        <v>19.956164383561642</v>
+        <v>19.890410958904109</v>
       </c>
       <c r="U22" s="33"/>
       <c r="AB22" s="7"/>
@@ -2296,7 +2297,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="33"/>
       <c r="I23" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J23" s="7">
         <v>86</v>
@@ -2309,7 +2310,7 @@
       </c>
       <c r="M23" s="9">
         <f t="shared" si="22"/>
-        <v>21.961643835616439</v>
+        <v>21.895890410958906</v>
       </c>
       <c r="N23" s="33"/>
       <c r="P23" s="46" t="s">
@@ -2322,7 +2323,7 @@
       <c r="R23" s="50"/>
       <c r="U23" s="33"/>
       <c r="V23" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W23" s="7" t="s">
         <v>29</v>
@@ -2338,13 +2339,13 @@
       </c>
       <c r="AA23" s="9">
         <f t="shared" ref="AA23" si="23">(Z23-$AC$1)/365*12</f>
-        <v>43.035616438356165</v>
+        <v>42.969863013698628</v>
       </c>
       <c r="AB23" s="7"/>
     </row>
     <row r="24" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" s="45">
         <v>158238</v>
@@ -2360,7 +2361,7 @@
       </c>
       <c r="F24" s="9">
         <f>(E24-$AC$1)/365*12</f>
-        <v>16.635616438356166</v>
+        <v>16.56986301369863</v>
       </c>
       <c r="G24" s="33"/>
       <c r="I24" s="46" t="s">
@@ -2397,7 +2398,7 @@
       </c>
       <c r="F25" s="9">
         <f>(E25-$AC$1)/365*12</f>
-        <v>20.317808219178083</v>
+        <v>20.252054794520546</v>
       </c>
       <c r="G25" s="33"/>
       <c r="K25" s="7"/>
@@ -2422,7 +2423,7 @@
       </c>
       <c r="T25" s="9">
         <f t="shared" ref="T25:T27" si="24">(S25-$AC$1)/365*12</f>
-        <v>16.93150684931507</v>
+        <v>16.865753424657534</v>
       </c>
       <c r="U25" s="33"/>
       <c r="AB25" s="7"/>
@@ -2455,7 +2456,7 @@
       </c>
       <c r="M26" s="9">
         <f t="shared" ref="M26:M27" si="25">(L26-$AC$1)/365*12</f>
-        <v>19.956164383561642</v>
+        <v>19.890410958904109</v>
       </c>
       <c r="N26" s="33"/>
       <c r="P26" s="7" t="s">
@@ -2472,27 +2473,27 @@
       </c>
       <c r="T26" s="9">
         <f t="shared" si="24"/>
-        <v>16.93150684931507</v>
+        <v>16.865753424657534</v>
       </c>
       <c r="U26" s="33"/>
       <c r="V26" s="51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="W26" s="7" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="X26" s="7">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="Y26" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z26" s="14">
-        <v>46780</v>
+        <v>47085</v>
       </c>
       <c r="AA26" s="9">
-        <f t="shared" ref="AA26:AA27" si="26">(Z26-$AC$1)/365*12</f>
-        <v>36.032876712328772</v>
+        <f t="shared" ref="AA26" si="26">(Z26-$AC$1)/365*12</f>
+        <v>45.994520547945207</v>
       </c>
       <c r="AB26" s="7"/>
     </row>
@@ -2502,7 +2503,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="33"/>
       <c r="I27" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J27" s="7">
         <v>75</v>
@@ -2513,11 +2514,11 @@
       </c>
       <c r="M27" s="9">
         <f t="shared" si="25"/>
-        <v>21.961643835616439</v>
+        <v>21.895890410958906</v>
       </c>
       <c r="N27" s="33"/>
       <c r="P27" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q27" s="7">
         <v>50</v>
@@ -2530,31 +2531,20 @@
       </c>
       <c r="T27" s="9">
         <f t="shared" si="24"/>
-        <v>21.961643835616439</v>
+        <v>21.895890410958906</v>
       </c>
       <c r="U27" s="33"/>
       <c r="V27" s="51"/>
-      <c r="W27" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="X27" s="7">
-        <v>43</v>
-      </c>
-      <c r="Y27" s="7">
-        <v>2</v>
-      </c>
-      <c r="Z27" s="14">
-        <v>47085</v>
-      </c>
-      <c r="AA27" s="9">
-        <f t="shared" si="26"/>
-        <v>46.060273972602737</v>
-      </c>
+      <c r="W27" s="7"/>
+      <c r="X27" s="7"/>
+      <c r="Y27" s="7"/>
+      <c r="Z27" s="14"/>
+      <c r="AA27" s="9"/>
       <c r="AB27" s="7"/>
     </row>
     <row r="28" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" s="44">
         <v>158234</v>
@@ -2570,7 +2560,7 @@
       </c>
       <c r="F28" s="9">
         <f>(E28-$AC$1)/365*12</f>
-        <v>16.668493150684931</v>
+        <v>16.602739726027398</v>
       </c>
       <c r="G28" s="33"/>
       <c r="I28" s="46" t="s">
@@ -2597,14 +2587,14 @@
       </c>
       <c r="X28" s="49">
         <f>SUM(X26:X27)*4+Y26+Y27</f>
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Y28" s="50"/>
       <c r="AB28" s="7"/>
     </row>
     <row r="29" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29" s="7">
         <v>94</v>
@@ -2615,7 +2605,7 @@
       </c>
       <c r="F29" s="9">
         <f>(E29-$AC$1)/365*12</f>
-        <v>17.326027397260273</v>
+        <v>17.260273972602739</v>
       </c>
       <c r="G29" s="33"/>
       <c r="K29" s="7"/>
@@ -2651,14 +2641,14 @@
       </c>
       <c r="M30" s="16">
         <f t="shared" ref="M30" si="27">(L30-$AC$1)/365*12</f>
-        <v>-5.1287671232876715</v>
+        <v>-5.1945205479452055</v>
       </c>
       <c r="N30" s="33"/>
       <c r="O30" s="6" t="s">
         <v>30</v>
       </c>
       <c r="P30" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q30" s="7">
         <v>9</v>
@@ -2671,14 +2661,14 @@
       </c>
       <c r="T30" s="9">
         <f t="shared" ref="T30:T31" si="28">(S30-$AC$1)/365*12</f>
-        <v>21.961643835616439</v>
+        <v>21.895890410958906</v>
       </c>
       <c r="U30" s="33"/>
       <c r="V30" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W30" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="X30" s="7">
         <v>8</v>
@@ -2691,7 +2681,7 @@
       </c>
       <c r="AA30" s="9">
         <f t="shared" ref="AA30:AA31" si="29">(Z30-$AC$1)/365*12</f>
-        <v>20.942465753424656</v>
+        <v>20.876712328767123</v>
       </c>
     </row>
     <row r="31" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2710,7 +2700,7 @@
       <c r="N31" s="33"/>
       <c r="O31" s="6"/>
       <c r="P31" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q31" s="7">
         <v>11</v>
@@ -2721,14 +2711,14 @@
       </c>
       <c r="T31" s="9">
         <f t="shared" si="28"/>
-        <v>21.961643835616439</v>
+        <v>21.895890410958906</v>
       </c>
       <c r="U31" s="33"/>
       <c r="W31" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="X31" s="7">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="Y31" s="7"/>
       <c r="Z31" s="14">
@@ -2736,16 +2726,16 @@
       </c>
       <c r="AA31" s="9">
         <f t="shared" si="29"/>
-        <v>20.942465753424656</v>
+        <v>20.876712328767123</v>
       </c>
       <c r="AB31" s="7"/>
     </row>
     <row r="32" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32" s="44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C32" s="7">
         <v>4</v>
@@ -2758,7 +2748,7 @@
       </c>
       <c r="F32" s="9">
         <f>(E32-$AC$1)/365*12</f>
-        <v>17.326027397260273</v>
+        <v>17.260273972602739</v>
       </c>
       <c r="G32" s="33"/>
       <c r="K32" s="7"/>
@@ -2777,7 +2767,7 @@
       </c>
       <c r="X32" s="49">
         <f>SUM(X30:X31)*30+Y30</f>
-        <v>1577</v>
+        <v>1187</v>
       </c>
       <c r="Y32" s="50"/>
       <c r="AB32" s="7"/>
@@ -2785,7 +2775,7 @@
     <row r="33" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="27"/>
       <c r="B33" s="44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C33" s="7">
         <v>108</v>
@@ -2796,11 +2786,11 @@
       </c>
       <c r="F33" s="9">
         <f>(E33-$AC$1)/365*12</f>
-        <v>20.646575342465752</v>
+        <v>20.580821917808219</v>
       </c>
       <c r="G33" s="33"/>
       <c r="H33" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I33" s="7">
         <v>162839</v>
@@ -2816,7 +2806,7 @@
       </c>
       <c r="M33" s="9">
         <f t="shared" ref="M33:M34" si="30">(L33-$AC$1)/365*12</f>
-        <v>20.416438356164385</v>
+        <v>20.350684931506848</v>
       </c>
       <c r="N33" s="33"/>
       <c r="U33" s="33"/>
@@ -2845,14 +2835,14 @@
       </c>
       <c r="M34" s="9">
         <f t="shared" si="30"/>
-        <v>20.416438356164385</v>
+        <v>20.350684931506848</v>
       </c>
       <c r="N34" s="33"/>
       <c r="O34" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P34" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="P34" s="7" t="s">
-        <v>35</v>
       </c>
       <c r="Q34" s="7">
         <v>9</v>
@@ -2865,14 +2855,14 @@
       </c>
       <c r="T34" s="9">
         <f>(S34-$AC$1)/365*12</f>
-        <v>10.915068493150685</v>
+        <v>10.84931506849315</v>
       </c>
       <c r="U34" s="33"/>
       <c r="V34" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="W34" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="X34" s="11">
         <v>7</v>
@@ -2885,7 +2875,7 @@
       </c>
       <c r="AA34" s="26">
         <f t="shared" ref="AA34" si="31">(Z34-$AC$1)/365*12</f>
-        <v>20.942465753424656</v>
+        <v>20.876712328767123</v>
       </c>
       <c r="AB34" s="7"/>
     </row>
@@ -2905,7 +2895,7 @@
       <c r="N35" s="33"/>
       <c r="O35" s="6"/>
       <c r="P35" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q35" s="7">
         <v>18</v>
@@ -2916,15 +2906,15 @@
       </c>
       <c r="T35" s="9">
         <f>(S35-$AC$1)/365*12</f>
-        <v>10.915068493150685</v>
+        <v>10.84931506849315</v>
       </c>
       <c r="U35" s="33"/>
       <c r="V35" s="6"/>
       <c r="W35" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="X35" s="11">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="Y35" s="24"/>
       <c r="Z35" s="25">
@@ -2935,10 +2925,10 @@
     </row>
     <row r="36" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B36" s="44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C36" s="11">
         <v>1</v>
@@ -2951,7 +2941,7 @@
       </c>
       <c r="F36" s="9">
         <f>(E36-$AC$1)/365*12</f>
-        <v>18.936986301369863</v>
+        <v>18.871232876712327</v>
       </c>
       <c r="G36" s="33"/>
       <c r="K36" s="7"/>
@@ -2972,14 +2962,14 @@
       </c>
       <c r="X36" s="49">
         <f>SUM(X34:X35)*18+Y34</f>
-        <v>1451</v>
+        <v>1307</v>
       </c>
       <c r="Y36" s="50"/>
       <c r="AB36" s="7"/>
     </row>
     <row r="37" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C37" s="40">
         <v>23</v>
@@ -2990,11 +2980,11 @@
       </c>
       <c r="F37" s="9">
         <f>(E37-$AC$1)/365*12</f>
-        <v>19.956164383561642</v>
+        <v>19.890410958904109</v>
       </c>
       <c r="G37" s="33"/>
       <c r="H37" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I37" s="7">
         <v>161789</v>
@@ -3010,7 +3000,7 @@
       </c>
       <c r="M37" s="9">
         <f t="shared" ref="M37:M38" si="32">(L37-$AC$1)/365*12</f>
-        <v>20.416438356164385</v>
+        <v>20.350684931506848</v>
       </c>
       <c r="N37" s="33"/>
       <c r="P37" s="13"/>
@@ -3022,7 +3012,7 @@
     </row>
     <row r="38" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="44" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C38" s="40">
         <v>85</v>
@@ -3033,7 +3023,7 @@
       </c>
       <c r="F38" s="9">
         <f>(E38-$AC$1)/365*12</f>
-        <v>21.961643835616439</v>
+        <v>21.895890410958906</v>
       </c>
       <c r="G38" s="33"/>
       <c r="I38" s="7">
@@ -3048,14 +3038,14 @@
       </c>
       <c r="M38" s="9">
         <f t="shared" si="32"/>
-        <v>20.416438356164385</v>
+        <v>20.350684931506848</v>
       </c>
       <c r="N38" s="33"/>
       <c r="O38" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P38" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="P38" s="7" t="s">
-        <v>38</v>
       </c>
       <c r="Q38" s="7">
         <v>6</v>
@@ -3068,14 +3058,14 @@
       </c>
       <c r="T38" s="9">
         <f>(S38-$AC$1)/365*12</f>
-        <v>16.93150684931507</v>
+        <v>16.865753424657534</v>
       </c>
       <c r="U38" s="33"/>
       <c r="V38" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W38" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X38" s="7"/>
       <c r="Y38" s="7">
@@ -3086,7 +3076,7 @@
       </c>
       <c r="AA38" s="9">
         <f t="shared" ref="AA38" si="33">(Z38-$AC$1)/365*12</f>
-        <v>9.9287671232876722</v>
+        <v>9.8630136986301373</v>
       </c>
       <c r="AB38" s="7"/>
     </row>
@@ -3112,7 +3102,7 @@
       <c r="N39" s="33"/>
       <c r="O39" s="24"/>
       <c r="P39" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q39" s="7">
         <v>33</v>
@@ -3123,7 +3113,7 @@
       </c>
       <c r="T39" s="9">
         <f>(S39-$AC$1)/365*12</f>
-        <v>16.93150684931507</v>
+        <v>16.865753424657534</v>
       </c>
       <c r="U39" s="33"/>
       <c r="W39" s="46" t="s">
@@ -3147,7 +3137,7 @@
       <c r="N40" s="33"/>
       <c r="O40" s="24"/>
       <c r="P40" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q40" s="7">
         <v>69</v>
@@ -3160,17 +3150,17 @@
       </c>
       <c r="T40" s="9">
         <f>(S40-$AC$1)/365*12</f>
-        <v>21.961643835616439</v>
+        <v>21.895890410958906</v>
       </c>
       <c r="U40" s="34"/>
       <c r="AB40" s="7"/>
     </row>
     <row r="41" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="44" t="s">
         <v>44</v>
-      </c>
-      <c r="B41" s="44" t="s">
-        <v>45</v>
       </c>
       <c r="C41" s="7">
         <v>1</v>
@@ -3183,11 +3173,11 @@
       </c>
       <c r="F41" s="9">
         <f>(E41-$AC$1)/365*12</f>
-        <v>18.936986301369863</v>
+        <v>18.871232876712327</v>
       </c>
       <c r="G41" s="33"/>
       <c r="H41" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I41" s="7">
         <v>156642</v>
@@ -3203,7 +3193,7 @@
       </c>
       <c r="M41" s="9">
         <f t="shared" ref="M41:M42" si="34">(L41-$AC$1)/365*12</f>
-        <v>16.865753424657534</v>
+        <v>16.799999999999997</v>
       </c>
       <c r="N41" s="33"/>
       <c r="P41" s="46" t="s">
@@ -3220,7 +3210,7 @@
     <row r="42" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="6"/>
       <c r="B42" s="44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C42" s="7">
         <v>62</v>
@@ -3231,7 +3221,7 @@
       </c>
       <c r="F42" s="9">
         <f>(E42-$AC$1)/365*12</f>
-        <v>19.956164383561642</v>
+        <v>19.890410958904109</v>
       </c>
       <c r="G42" s="33"/>
       <c r="H42" s="27"/>
@@ -3247,7 +3237,7 @@
       </c>
       <c r="M42" s="9">
         <f t="shared" si="34"/>
-        <v>16.865753424657534</v>
+        <v>16.799999999999997</v>
       </c>
       <c r="N42" s="33"/>
       <c r="U42" s="24"/>
@@ -3274,7 +3264,7 @@
       <c r="K43" s="50"/>
       <c r="N43" s="33"/>
       <c r="O43" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P43" s="7">
         <v>3</v>
@@ -3295,10 +3285,10 @@
     </row>
     <row r="45" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B45" s="44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C45" s="7">
         <v>0</v>
@@ -3311,11 +3301,11 @@
       </c>
       <c r="F45" s="9">
         <f t="shared" ref="F45:F46" si="35">(E45-$AC$1)/365*12</f>
-        <v>19.956164383561642</v>
+        <v>19.890410958904109</v>
       </c>
       <c r="G45" s="33"/>
       <c r="H45" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I45" s="7">
         <v>156641</v>
@@ -3331,11 +3321,11 @@
       </c>
       <c r="M45" s="9">
         <f t="shared" ref="M45:M46" si="36">(L45-$AC$1)/365*12</f>
-        <v>16.865753424657534</v>
+        <v>16.799999999999997</v>
       </c>
       <c r="N45" s="33"/>
       <c r="O45" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P45" s="7">
         <v>49</v>
@@ -3346,7 +3336,7 @@
     <row r="46" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
       <c r="B46" s="44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C46" s="11">
         <v>55</v>
@@ -3359,7 +3349,7 @@
       </c>
       <c r="F46" s="9">
         <f t="shared" si="35"/>
-        <v>21.961643835616439</v>
+        <v>21.895890410958906</v>
       </c>
       <c r="G46" s="33"/>
       <c r="I46" s="7">
@@ -3374,7 +3364,7 @@
       </c>
       <c r="M46" s="9">
         <f t="shared" si="36"/>
-        <v>20.350684931506848</v>
+        <v>20.284931506849315</v>
       </c>
       <c r="N46" s="33"/>
       <c r="U46" s="24"/>
@@ -3418,10 +3408,10 @@
     </row>
     <row r="49" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B49" s="43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C49" s="7">
         <v>7</v>
@@ -3434,7 +3424,7 @@
       </c>
       <c r="F49" s="9">
         <f t="shared" ref="F49:F50" si="37">(E49-$AC$1)/365*12</f>
-        <v>18.936986301369863</v>
+        <v>18.871232876712327</v>
       </c>
       <c r="G49" s="33"/>
       <c r="I49" s="11"/>
@@ -3449,7 +3439,7 @@
     <row r="50" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6"/>
       <c r="B50" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C50" s="7">
         <v>53</v>
@@ -3462,7 +3452,7 @@
       </c>
       <c r="F50" s="9">
         <f t="shared" si="37"/>
-        <v>19.956164383561642</v>
+        <v>19.890410958904109</v>
       </c>
       <c r="G50" s="33"/>
       <c r="I50" s="39"/>
@@ -3502,10 +3492,10 @@
     </row>
     <row r="53" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53" s="44" t="s">
         <v>47</v>
-      </c>
-      <c r="B53" s="44" t="s">
-        <v>48</v>
       </c>
       <c r="C53" s="7">
         <v>10</v>
@@ -3518,7 +3508,7 @@
       </c>
       <c r="F53" s="16">
         <f>(E53-$AC$1)/365*12</f>
-        <v>-5.1287671232876715</v>
+        <v>-5.1945205479452055</v>
       </c>
       <c r="G53" s="33"/>
       <c r="K53" s="7"/>
@@ -4561,7 +4551,7 @@
     <row r="282" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="283" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="hgUFn575gqca0prUo1kzidQgsek8GSKkwOaoB0KUCdxEzuLhA4OEV/jcGIx2oPHvXyzS8wkCblhHr48ywSU39w==" saltValue="nE8R7BaEmtFYW8RZfIRObA==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" deleteColumns="0" deleteRows="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="44">
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="C47:D47"/>

</xml_diff>

<commit_message>
Update lot codes - 2025-01-29 15:44:27
</commit_message>
<xml_diff>
--- a/LotCode.xlsx
+++ b/LotCode.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf.sharepoint.com/sites/production-warehouse/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7155" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5F2CE1C-246A-4A34-9B24-EBC8CA5D5B14}"/>
+  <xr:revisionPtr revIDLastSave="7182" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A41A2C5-8F75-43B6-AAD7-4E80742776BB}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="a/VZ8kgdZMyU/a42HcB04O8OBNrnh4WxCIPRCv9GqcObOgYeM9oYcSfQqndR/nnirMykfzLaq88Ahwir6HajhQ==" workbookSaltValue="jsEDzk1n/+JkLoe+dWrmxg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3645" yWindow="1935" windowWidth="21660" windowHeight="11265" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="103">
   <si>
     <t>SKU</t>
   </si>
@@ -88,9 +88,6 @@
     <t>100-DR-HO</t>
   </si>
   <si>
-    <t>PRID10042</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
   </si>
   <si>
     <t>750-DR-HO</t>
-  </si>
-  <si>
-    <t>PRC0043</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -1095,9 +1089,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4D02CE-C7F3-446F-985C-950AF7BFACB9}">
   <dimension ref="A1:AE283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC16" sqref="AC16"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W21" sqref="W21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,26 +1213,26 @@
     </row>
     <row r="2" spans="1:31" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="42" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G2" s="32"/>
       <c r="H2" s="23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="N2" s="32"/>
       <c r="O2" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="U2" s="32"/>
       <c r="V2" s="42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="AB2" s="8"/>
       <c r="AE2" s="18"/>
     </row>
     <row r="3" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" s="40">
         <v>159368</v>
@@ -1258,7 +1252,7 @@
       </c>
       <c r="G3" s="33"/>
       <c r="H3" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I3" s="7">
         <v>155511</v>
@@ -1281,7 +1275,7 @@
         <v>7</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q3" s="12">
         <v>9</v>
@@ -1298,23 +1292,23 @@
       </c>
       <c r="U3" s="33"/>
       <c r="V3" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="W3" s="7" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="X3" s="7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="Y3" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Z3" s="14">
-        <v>46993</v>
+        <v>47024</v>
       </c>
       <c r="AA3" s="9">
         <f t="shared" ref="AA3" si="3">(Z3-$AC$1)/365*12</f>
-        <v>42.969863013698628</v>
+        <v>43.989041095890407</v>
       </c>
       <c r="AB3" s="12"/>
     </row>
@@ -1351,7 +1345,7 @@
       <c r="N4" s="33"/>
       <c r="O4" s="27"/>
       <c r="P4" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q4" s="7">
         <v>55</v>
@@ -1366,7 +1360,7 @@
       </c>
       <c r="U4" s="33"/>
       <c r="W4" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="X4" s="15">
         <v>177</v>
@@ -1400,7 +1394,7 @@
       </c>
       <c r="G5" s="33"/>
       <c r="I5" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J5" s="49">
         <f>SUM(J3:J4)*40+K3</f>
@@ -1410,7 +1404,7 @@
       <c r="N5" s="33"/>
       <c r="O5" s="27"/>
       <c r="P5" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="Q5" s="7">
         <v>195</v>
@@ -1427,18 +1421,18 @@
       </c>
       <c r="U5" s="33"/>
       <c r="W5" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="X5" s="49">
         <f>SUM(X3:X4)*6+Y3+Y4</f>
-        <v>1102</v>
+        <v>1122</v>
       </c>
       <c r="Y5" s="50"/>
       <c r="AB5" s="7"/>
     </row>
     <row r="6" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="49">
         <f>SUM(C3:C5)*40+D3</f>
@@ -1450,7 +1444,7 @@
       <c r="K6" s="7"/>
       <c r="N6" s="33"/>
       <c r="P6" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q6" s="49">
         <f>SUM(Q3:Q5)*30+R3+R5</f>
@@ -1459,7 +1453,7 @@
       <c r="R6" s="50"/>
       <c r="U6" s="33"/>
       <c r="V6" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AB6" s="7"/>
     </row>
@@ -1470,7 +1464,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="33"/>
       <c r="H7" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I7" s="7">
         <v>156645</v>
@@ -1491,16 +1485,16 @@
       <c r="N7" s="33"/>
       <c r="U7" s="33"/>
       <c r="V7" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="W7" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="X7" s="15">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="Y7" s="15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Z7" s="14">
         <v>46993</v>
@@ -1513,7 +1507,7 @@
     </row>
     <row r="8" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B8" s="7">
         <v>158583</v>
@@ -1549,10 +1543,10 @@
       </c>
       <c r="N8" s="33"/>
       <c r="O8" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q8" s="7">
         <v>9</v>
@@ -1569,7 +1563,7 @@
       </c>
       <c r="U8" s="33"/>
       <c r="W8" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="X8" s="7">
         <v>54</v>
@@ -1620,7 +1614,7 @@
       </c>
       <c r="N9" s="33"/>
       <c r="P9" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q9" s="7">
         <v>29</v>
@@ -1635,11 +1629,11 @@
       </c>
       <c r="U9" s="33"/>
       <c r="W9" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="X9" s="49">
         <f>SUM(X7:X8)*6+Y7+Y8</f>
-        <v>444</v>
+        <v>412</v>
       </c>
       <c r="Y9" s="50"/>
       <c r="AB9" s="7"/>
@@ -1662,7 +1656,7 @@
       </c>
       <c r="G10" s="33"/>
       <c r="I10" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J10" s="49">
         <f>SUM(J7:J9)*24+K7</f>
@@ -1671,7 +1665,7 @@
       <c r="K10" s="50"/>
       <c r="N10" s="33"/>
       <c r="P10" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Q10" s="7">
         <v>173</v>
@@ -1707,7 +1701,7 @@
       <c r="K11" s="7"/>
       <c r="N11" s="33"/>
       <c r="P11" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q11" s="49">
         <f>SUM(Q8:Q10)*30+R8</f>
@@ -1716,16 +1710,16 @@
       <c r="R11" s="50"/>
       <c r="U11" s="33"/>
       <c r="V11" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="W11" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X11" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Y11" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z11" s="14">
         <v>46993</v>
@@ -1738,7 +1732,7 @@
     </row>
     <row r="12" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="49">
         <f>SUM(C8:C11)*24+D8</f>
@@ -1748,7 +1742,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="33"/>
       <c r="H12" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I12" s="7">
         <v>163239</v>
@@ -1769,10 +1763,10 @@
       <c r="N12" s="33"/>
       <c r="U12" s="33"/>
       <c r="W12" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="X12" s="7">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="Y12" s="7"/>
       <c r="Z12" s="14">
@@ -1805,10 +1799,10 @@
       </c>
       <c r="N13" s="33"/>
       <c r="O13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q13" s="7">
         <v>9</v>
@@ -1825,18 +1819,18 @@
       </c>
       <c r="U13" s="33"/>
       <c r="W13" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="X13" s="49">
         <f>SUM(X11:X12)*6+Y11+Y12</f>
-        <v>1230</v>
+        <v>1240</v>
       </c>
       <c r="Y13" s="50"/>
       <c r="AB13" s="7"/>
     </row>
     <row r="14" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B14" s="35">
         <v>158221</v>
@@ -1866,7 +1860,7 @@
       <c r="N14" s="33"/>
       <c r="O14" s="27"/>
       <c r="P14" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q14" s="7">
         <v>120</v>
@@ -1901,7 +1895,7 @@
       </c>
       <c r="G15" s="33"/>
       <c r="I15" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J15" s="49">
         <f>SUM(J12:J13)*24+K12</f>
@@ -1910,7 +1904,7 @@
       <c r="K15" s="50"/>
       <c r="N15" s="33"/>
       <c r="P15" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q15" s="49">
         <f>SUM(Q13:Q14)*30+R13+R14</f>
@@ -1919,27 +1913,27 @@
       <c r="R15" s="50"/>
       <c r="U15" s="33"/>
       <c r="V15" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="W15" s="7" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="X15" s="7">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="Y15" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z15" s="14">
-        <v>46993</v>
+        <v>47024</v>
       </c>
       <c r="AA15" s="9">
-        <f t="shared" ref="AA15" si="13">(Z15-$AC$1)/365*12</f>
-        <v>42.969863013698628</v>
+        <f t="shared" ref="AA15:AA16" si="13">(Z15-$AC$1)/365*12</f>
+        <v>43.989041095890407</v>
       </c>
       <c r="AB15" s="7"/>
     </row>
-    <row r="16" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="35">
         <v>159366</v>
       </c>
@@ -1960,20 +1954,20 @@
       <c r="U16" s="33"/>
       <c r="V16" s="6"/>
       <c r="W16" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="X16" s="7">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="Y16" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z16" s="14">
-        <v>47024</v>
+        <v>47085</v>
       </c>
       <c r="AA16" s="9">
-        <f t="shared" ref="AA16:AA17" si="15">(Z16-$AC$1)/365*12</f>
-        <v>43.989041095890407</v>
+        <f t="shared" si="13"/>
+        <v>45.994520547945207</v>
       </c>
       <c r="AB16" s="8"/>
     </row>
@@ -1994,7 +1988,7 @@
       </c>
       <c r="G17" s="33"/>
       <c r="H17" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I17" s="7">
         <v>163238</v>
@@ -2009,15 +2003,15 @@
         <v>46310</v>
       </c>
       <c r="M17" s="9">
-        <f t="shared" ref="M17:M18" si="16">(L17-$AC$1)/365*12</f>
+        <f t="shared" ref="M17:M18" si="15">(L17-$AC$1)/365*12</f>
         <v>20.515068493150686</v>
       </c>
       <c r="N17" s="33"/>
       <c r="O17" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P17" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Q17" s="7">
         <v>9</v>
@@ -2029,32 +2023,23 @@
         <v>46199</v>
       </c>
       <c r="T17" s="9">
-        <f t="shared" ref="T17" si="17">(S17-$AC$1)/365*12</f>
+        <f t="shared" ref="T17" si="16">(S17-$AC$1)/365*12</f>
         <v>16.865753424657534</v>
       </c>
       <c r="U17" s="33"/>
-      <c r="V17" s="6"/>
-      <c r="W17" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="X17" s="7">
-        <v>73</v>
-      </c>
-      <c r="Y17" s="7">
-        <v>2</v>
-      </c>
-      <c r="Z17" s="14">
-        <v>47085</v>
-      </c>
-      <c r="AA17" s="9">
-        <f t="shared" si="15"/>
-        <v>45.994520547945207</v>
-      </c>
+      <c r="W17" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="X17" s="49">
+        <f>SUM(X15:X16)*6+Y15+Y16</f>
+        <v>517</v>
+      </c>
+      <c r="Y17" s="50"/>
       <c r="AB17" s="7"/>
     </row>
     <row r="18" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18" s="49">
         <f>SUM(C14:C17)*24+D14</f>
@@ -2075,12 +2060,12 @@
         <v>46325</v>
       </c>
       <c r="M18" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>21.008219178082193</v>
       </c>
       <c r="N18" s="33"/>
       <c r="P18" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q18" s="7">
         <v>36</v>
@@ -2092,18 +2077,10 @@
         <v>46321</v>
       </c>
       <c r="T18" s="9">
-        <f t="shared" ref="T18" si="18">(S18-$AC$1)/365*12</f>
+        <f t="shared" ref="T18" si="17">(S18-$AC$1)/365*12</f>
         <v>20.876712328767123</v>
       </c>
       <c r="U18" s="33"/>
-      <c r="W18" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="X18" s="49">
-        <f>SUM(X15:X17)*6+Y15+Y16</f>
-        <v>625</v>
-      </c>
-      <c r="Y18" s="50"/>
       <c r="AB18" s="7"/>
     </row>
     <row r="19" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2112,7 +2089,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="33"/>
       <c r="I19" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J19" s="49">
         <f>SUM(J17:J18)*12+K17</f>
@@ -2123,7 +2100,7 @@
       <c r="M19" s="7"/>
       <c r="N19" s="33"/>
       <c r="P19" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q19" s="49">
         <f>SUM(Q17:Q18)*30+R17+R18</f>
@@ -2131,14 +2108,33 @@
       </c>
       <c r="R19" s="50"/>
       <c r="U19" s="33"/>
+      <c r="V19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="W19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="X19" s="7">
+        <v>5</v>
+      </c>
+      <c r="Y19" s="7">
+        <v>118</v>
+      </c>
+      <c r="Z19" s="14">
+        <v>46993</v>
+      </c>
+      <c r="AA19" s="9">
+        <f>(Z19-$AC$1)/365*12</f>
+        <v>42.969863013698628</v>
+      </c>
       <c r="AB19" s="7"/>
     </row>
     <row r="20" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B20" s="44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C20" s="11">
         <v>6</v>
@@ -2158,34 +2154,23 @@
       <c r="N20" s="33"/>
       <c r="P20" s="13"/>
       <c r="Q20" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="U20" s="33"/>
-      <c r="V20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="W20" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="X20" s="7">
-        <v>6</v>
-      </c>
-      <c r="Y20" s="7">
-        <v>39</v>
-      </c>
-      <c r="Z20" s="14">
-        <v>46993</v>
-      </c>
-      <c r="AA20" s="9">
-        <f>(Z20-$AC$1)/365*12</f>
-        <v>42.969863013698628</v>
-      </c>
+      <c r="W20" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="X20" s="49">
+        <f>SUM(X19*200)+Y19</f>
+        <v>1118</v>
+      </c>
+      <c r="Y20" s="50"/>
       <c r="AB20" s="7"/>
     </row>
     <row r="21" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="27"/>
       <c r="B21" s="44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C21" s="7">
         <v>149</v>
@@ -2194,15 +2179,15 @@
         <v>46283</v>
       </c>
       <c r="F21" s="9">
-        <f t="shared" ref="F21" si="19">(E21-$AC$1)/365*12</f>
+        <f t="shared" ref="F21" si="18">(E21-$AC$1)/365*12</f>
         <v>19.627397260273973</v>
       </c>
       <c r="G21" s="33"/>
       <c r="H21" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J21" s="7">
         <v>4</v>
@@ -2214,15 +2199,15 @@
         <v>46291</v>
       </c>
       <c r="M21" s="9">
-        <f t="shared" ref="M21" si="20">(L21-$AC$1)/365*12</f>
+        <f t="shared" ref="M21" si="19">(L21-$AC$1)/365*12</f>
         <v>19.890410958904109</v>
       </c>
       <c r="N21" s="33"/>
       <c r="O21" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P21" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Q21" s="7">
         <v>9</v>
@@ -2234,23 +2219,15 @@
         <v>46291</v>
       </c>
       <c r="T21" s="9">
-        <f t="shared" ref="T21:T22" si="21">(S21-$AC$1)/365*12</f>
+        <f t="shared" ref="T21:T22" si="20">(S21-$AC$1)/365*12</f>
         <v>19.890410958904109</v>
       </c>
       <c r="U21" s="33"/>
-      <c r="W21" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="X21" s="49">
-        <f>SUM(X20*200)+Y20</f>
-        <v>1239</v>
-      </c>
-      <c r="Y21" s="50"/>
       <c r="AB21" s="7"/>
     </row>
     <row r="22" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" s="49">
         <f>SUM(C20:C21)*12+D20</f>
@@ -2260,7 +2237,7 @@
       <c r="F22" s="7"/>
       <c r="G22" s="33"/>
       <c r="I22" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J22" s="7">
         <v>16</v>
@@ -2270,12 +2247,12 @@
         <v>46291</v>
       </c>
       <c r="M22" s="9">
-        <f t="shared" ref="M22:M23" si="22">(L22-$AC$1)/365*12</f>
+        <f t="shared" ref="M22:M23" si="21">(L22-$AC$1)/365*12</f>
         <v>19.890410958904109</v>
       </c>
       <c r="N22" s="33"/>
       <c r="P22" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Q22" s="7">
         <v>52</v>
@@ -2285,10 +2262,29 @@
         <v>46291</v>
       </c>
       <c r="T22" s="9">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>19.890410958904109</v>
       </c>
       <c r="U22" s="33"/>
+      <c r="V22" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="W22" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="X22" s="7">
+        <v>3</v>
+      </c>
+      <c r="Y22" s="7">
+        <v>180</v>
+      </c>
+      <c r="Z22" s="14">
+        <v>46993</v>
+      </c>
+      <c r="AA22" s="9">
+        <f t="shared" ref="AA22" si="22">(Z22-$AC$1)/365*12</f>
+        <v>42.969863013698628</v>
+      </c>
       <c r="AB22" s="7"/>
     </row>
     <row r="23" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2297,7 +2293,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="33"/>
       <c r="I23" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J23" s="7">
         <v>86</v>
@@ -2309,12 +2305,12 @@
         <v>46352</v>
       </c>
       <c r="M23" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>21.895890410958906</v>
       </c>
       <c r="N23" s="33"/>
       <c r="P23" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q23" s="49">
         <f>SUM(Q21:Q22)*30+R21</f>
@@ -2322,30 +2318,19 @@
       </c>
       <c r="R23" s="50"/>
       <c r="U23" s="33"/>
-      <c r="V23" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="W23" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="X23" s="7">
-        <v>4</v>
-      </c>
-      <c r="Y23" s="7">
-        <v>92</v>
-      </c>
-      <c r="Z23" s="14">
-        <v>46993</v>
-      </c>
-      <c r="AA23" s="9">
-        <f t="shared" ref="AA23" si="23">(Z23-$AC$1)/365*12</f>
-        <v>42.969863013698628</v>
-      </c>
+      <c r="W23" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="X23" s="49">
+        <f>SUM(X22*200)+Y22</f>
+        <v>780</v>
+      </c>
+      <c r="Y23" s="50"/>
       <c r="AB23" s="7"/>
     </row>
     <row r="24" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B24" s="45">
         <v>158238</v>
@@ -2365,7 +2350,7 @@
       </c>
       <c r="G24" s="33"/>
       <c r="I24" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J24" s="49">
         <f>SUM(J21:J23)*30+K21+K23</f>
@@ -2374,14 +2359,6 @@
       <c r="K24" s="50"/>
       <c r="N24" s="33"/>
       <c r="U24" s="33"/>
-      <c r="W24" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="X24" s="49">
-        <f>SUM(X23*200)+Y23</f>
-        <v>892</v>
-      </c>
-      <c r="Y24" s="50"/>
       <c r="AB24" s="7"/>
     </row>
     <row r="25" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2403,14 +2380,14 @@
       <c r="G25" s="33"/>
       <c r="K25" s="7"/>
       <c r="M25" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N25" s="33"/>
       <c r="O25" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q25" s="7">
         <v>9</v>
@@ -2422,15 +2399,34 @@
         <v>46199</v>
       </c>
       <c r="T25" s="9">
-        <f t="shared" ref="T25:T27" si="24">(S25-$AC$1)/365*12</f>
+        <f t="shared" ref="T25:T27" si="23">(S25-$AC$1)/365*12</f>
         <v>16.865753424657534</v>
       </c>
       <c r="U25" s="33"/>
+      <c r="V25" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="W25" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="X25" s="7">
+        <v>43</v>
+      </c>
+      <c r="Y25" s="7">
+        <v>2</v>
+      </c>
+      <c r="Z25" s="14">
+        <v>47085</v>
+      </c>
+      <c r="AA25" s="9">
+        <f t="shared" ref="AA25" si="24">(Z25-$AC$1)/365*12</f>
+        <v>45.994520547945207</v>
+      </c>
       <c r="AB25" s="7"/>
     </row>
     <row r="26" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C26" s="49">
         <f>SUM(C24:C25)*40+D24+D25</f>
@@ -2440,10 +2436,10 @@
       <c r="F26" s="7"/>
       <c r="G26" s="33"/>
       <c r="H26" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J26" s="7">
         <v>2</v>
@@ -2460,7 +2456,7 @@
       </c>
       <c r="N26" s="33"/>
       <c r="P26" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q26" s="7">
         <v>20</v>
@@ -2472,29 +2468,16 @@
         <v>46199</v>
       </c>
       <c r="T26" s="9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>16.865753424657534</v>
       </c>
       <c r="U26" s="33"/>
-      <c r="V26" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="W26" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="X26" s="7">
-        <v>43</v>
-      </c>
-      <c r="Y26" s="7">
-        <v>2</v>
-      </c>
-      <c r="Z26" s="14">
-        <v>47085</v>
-      </c>
-      <c r="AA26" s="9">
-        <f t="shared" ref="AA26" si="26">(Z26-$AC$1)/365*12</f>
-        <v>45.994520547945207</v>
-      </c>
+      <c r="V26" s="51"/>
+      <c r="W26" s="7"/>
+      <c r="X26" s="7"/>
+      <c r="Y26" s="7"/>
+      <c r="Z26" s="14"/>
+      <c r="AA26" s="9"/>
       <c r="AB26" s="7"/>
     </row>
     <row r="27" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2503,7 +2486,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="33"/>
       <c r="I27" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J27" s="7">
         <v>75</v>
@@ -2518,7 +2501,7 @@
       </c>
       <c r="N27" s="33"/>
       <c r="P27" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q27" s="7">
         <v>50</v>
@@ -2530,21 +2513,24 @@
         <v>46352</v>
       </c>
       <c r="T27" s="9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>21.895890410958906</v>
       </c>
       <c r="U27" s="33"/>
-      <c r="V27" s="51"/>
-      <c r="W27" s="7"/>
-      <c r="X27" s="7"/>
-      <c r="Y27" s="7"/>
-      <c r="Z27" s="14"/>
-      <c r="AA27" s="9"/>
+      <c r="V27" s="48"/>
+      <c r="W27" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="X27" s="49">
+        <f>SUM(X25:X26)*4+Y25+Y26</f>
+        <v>174</v>
+      </c>
+      <c r="Y27" s="50"/>
       <c r="AB27" s="7"/>
     </row>
     <row r="28" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B28" s="44">
         <v>158234</v>
@@ -2564,7 +2550,7 @@
       </c>
       <c r="G28" s="33"/>
       <c r="I28" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J28" s="49">
         <f>SUM(J26:J27)*30+K26</f>
@@ -2573,7 +2559,7 @@
       <c r="K28" s="50"/>
       <c r="N28" s="33"/>
       <c r="P28" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q28" s="49">
         <f>SUM(Q25:Q27)*30+R25+R26+R27</f>
@@ -2581,20 +2567,11 @@
       </c>
       <c r="R28" s="50"/>
       <c r="U28" s="33"/>
-      <c r="V28" s="48"/>
-      <c r="W28" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="X28" s="49">
-        <f>SUM(X26:X27)*4+Y26+Y27</f>
-        <v>174</v>
-      </c>
-      <c r="Y28" s="50"/>
       <c r="AB28" s="7"/>
     </row>
     <row r="29" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="44" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C29" s="7">
         <v>94</v>
@@ -2611,11 +2588,30 @@
       <c r="K29" s="7"/>
       <c r="N29" s="33"/>
       <c r="U29" s="33"/>
+      <c r="V29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="W29" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="X29" s="7">
+        <v>10</v>
+      </c>
+      <c r="Y29" s="7">
+        <v>10</v>
+      </c>
+      <c r="Z29" s="14">
+        <v>46321</v>
+      </c>
+      <c r="AA29" s="9">
+        <f t="shared" ref="AA29:AA30" si="26">(Z29-$AC$1)/365*12</f>
+        <v>20.876712328767123</v>
+      </c>
       <c r="AB29" s="8"/>
     </row>
     <row r="30" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C30" s="49">
         <f>SUM(C28:C29)*24+D28</f>
@@ -2625,10 +2621,10 @@
       <c r="F30" s="7"/>
       <c r="G30" s="33"/>
       <c r="H30" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J30" s="7">
         <v>7</v>
@@ -2645,10 +2641,10 @@
       </c>
       <c r="N30" s="33"/>
       <c r="O30" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P30" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q30" s="7">
         <v>9</v>
@@ -2664,23 +2660,18 @@
         <v>21.895890410958906</v>
       </c>
       <c r="U30" s="33"/>
-      <c r="V30" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="W30" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="X30" s="7">
-        <v>8</v>
-      </c>
-      <c r="Y30" s="7">
-        <v>17</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="Y30" s="7"/>
       <c r="Z30" s="14">
         <v>46321</v>
       </c>
       <c r="AA30" s="9">
-        <f t="shared" ref="AA30:AA31" si="29">(Z30-$AC$1)/365*12</f>
+        <f t="shared" si="26"/>
         <v>20.876712328767123</v>
       </c>
     </row>
@@ -2690,7 +2681,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="33"/>
       <c r="I31" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J31" s="49">
         <f>SUM(J30)*30+K30</f>
@@ -2700,7 +2691,7 @@
       <c r="N31" s="33"/>
       <c r="O31" s="6"/>
       <c r="P31" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q31" s="7">
         <v>11</v>
@@ -2714,28 +2705,22 @@
         <v>21.895890410958906</v>
       </c>
       <c r="U31" s="33"/>
-      <c r="W31" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="X31" s="7">
-        <v>31</v>
-      </c>
-      <c r="Y31" s="7"/>
-      <c r="Z31" s="14">
-        <v>46321</v>
-      </c>
-      <c r="AA31" s="9">
-        <f t="shared" si="29"/>
-        <v>20.876712328767123</v>
-      </c>
+      <c r="W31" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="X31" s="49">
+        <f>SUM(X29:X30)*30+Y29</f>
+        <v>1270</v>
+      </c>
+      <c r="Y31" s="50"/>
       <c r="AB31" s="7"/>
     </row>
     <row r="32" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B32" s="44" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C32" s="7">
         <v>4</v>
@@ -2754,7 +2739,7 @@
       <c r="K32" s="7"/>
       <c r="N32" s="33"/>
       <c r="P32" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q32" s="49">
         <f>SUM(Q30:Q31)*30+R30</f>
@@ -2762,20 +2747,12 @@
       </c>
       <c r="R32" s="50"/>
       <c r="U32" s="33"/>
-      <c r="W32" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="X32" s="49">
-        <f>SUM(X30:X31)*30+Y30</f>
-        <v>1187</v>
-      </c>
-      <c r="Y32" s="50"/>
       <c r="AB32" s="7"/>
     </row>
     <row r="33" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="27"/>
       <c r="B33" s="44" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C33" s="7">
         <v>108</v>
@@ -2790,7 +2767,7 @@
       </c>
       <c r="G33" s="33"/>
       <c r="H33" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I33" s="7">
         <v>162839</v>
@@ -2805,16 +2782,35 @@
         <v>46305</v>
       </c>
       <c r="M33" s="9">
-        <f t="shared" ref="M33:M34" si="30">(L33-$AC$1)/365*12</f>
+        <f t="shared" ref="M33:M34" si="29">(L33-$AC$1)/365*12</f>
         <v>20.350684931506848</v>
       </c>
       <c r="N33" s="33"/>
       <c r="U33" s="33"/>
+      <c r="V33" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="W33" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="X33" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="24">
+        <v>5</v>
+      </c>
+      <c r="Z33" s="25">
+        <v>46321</v>
+      </c>
+      <c r="AA33" s="26">
+        <f t="shared" ref="AA33" si="30">(Z33-$AC$1)/365*12</f>
+        <v>20.876712328767123</v>
+      </c>
       <c r="AB33" s="7"/>
     </row>
     <row r="34" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C34" s="49">
         <f>SUM(C32:C33)*24+D32</f>
@@ -2834,15 +2830,15 @@
         <v>46305</v>
       </c>
       <c r="M34" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>20.350684931506848</v>
       </c>
       <c r="N34" s="33"/>
       <c r="O34" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P34" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Q34" s="7">
         <v>9</v>
@@ -2858,25 +2854,18 @@
         <v>10.84931506849315</v>
       </c>
       <c r="U34" s="33"/>
-      <c r="V34" s="6" t="s">
-        <v>38</v>
-      </c>
+      <c r="V34" s="6"/>
       <c r="W34" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="X34" s="11">
-        <v>7</v>
-      </c>
-      <c r="Y34" s="24">
-        <v>11</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="Y34" s="24"/>
       <c r="Z34" s="25">
         <v>46321</v>
       </c>
-      <c r="AA34" s="26">
-        <f t="shared" ref="AA34" si="31">(Z34-$AC$1)/365*12</f>
-        <v>20.876712328767123</v>
-      </c>
+      <c r="AA34" s="26"/>
       <c r="AB34" s="7"/>
     </row>
     <row r="35" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2885,7 +2874,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="33"/>
       <c r="I35" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J35" s="49">
         <f>SUM(J33:J34)*24+K33</f>
@@ -2895,7 +2884,7 @@
       <c r="N35" s="33"/>
       <c r="O35" s="6"/>
       <c r="P35" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Q35" s="7">
         <v>18</v>
@@ -2909,26 +2898,22 @@
         <v>10.84931506849315</v>
       </c>
       <c r="U35" s="33"/>
-      <c r="V35" s="6"/>
-      <c r="W35" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="X35" s="11">
-        <v>65</v>
-      </c>
-      <c r="Y35" s="24"/>
-      <c r="Z35" s="25">
-        <v>46321</v>
-      </c>
-      <c r="AA35" s="26"/>
+      <c r="W35" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="X35" s="49">
+        <f>SUM(X33:X34)*18+Y33</f>
+        <v>1175</v>
+      </c>
+      <c r="Y35" s="50"/>
       <c r="AB35" s="7"/>
     </row>
     <row r="36" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B36" s="44" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C36" s="11">
         <v>1</v>
@@ -2947,7 +2932,7 @@
       <c r="K36" s="7"/>
       <c r="N36" s="33"/>
       <c r="P36" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q36" s="49">
         <f>SUM(Q34:Q35)*30+R34</f>
@@ -2957,19 +2942,11 @@
       <c r="S36" s="7"/>
       <c r="T36" s="7"/>
       <c r="U36" s="33"/>
-      <c r="W36" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="X36" s="49">
-        <f>SUM(X34:X35)*18+Y34</f>
-        <v>1307</v>
-      </c>
-      <c r="Y36" s="50"/>
       <c r="AB36" s="7"/>
     </row>
-    <row r="37" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="44" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C37" s="40">
         <v>23</v>
@@ -2984,7 +2961,7 @@
       </c>
       <c r="G37" s="33"/>
       <c r="H37" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I37" s="7">
         <v>161789</v>
@@ -2999,7 +2976,7 @@
         <v>46305</v>
       </c>
       <c r="M37" s="9">
-        <f t="shared" ref="M37:M38" si="32">(L37-$AC$1)/365*12</f>
+        <f t="shared" ref="M37:M38" si="31">(L37-$AC$1)/365*12</f>
         <v>20.350684931506848</v>
       </c>
       <c r="N37" s="33"/>
@@ -3008,11 +2985,28 @@
       <c r="S37" s="7"/>
       <c r="T37" s="7"/>
       <c r="U37" s="33"/>
+      <c r="V37" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="W37" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="X37" s="7"/>
+      <c r="Y37" s="7">
+        <v>2</v>
+      </c>
+      <c r="Z37" s="14">
+        <v>45986</v>
+      </c>
+      <c r="AA37" s="9">
+        <f t="shared" ref="AA37" si="32">(Z37-$AC$1)/365*12</f>
+        <v>9.8630136986301373</v>
+      </c>
       <c r="AB37" s="7"/>
     </row>
     <row r="38" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="44" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C38" s="40">
         <v>85</v>
@@ -3037,15 +3031,15 @@
         <v>46305</v>
       </c>
       <c r="M38" s="9">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>20.350684931506848</v>
       </c>
       <c r="N38" s="33"/>
       <c r="O38" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P38" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="Q38" s="7">
         <v>6</v>
@@ -3061,28 +3055,19 @@
         <v>16.865753424657534</v>
       </c>
       <c r="U38" s="33"/>
-      <c r="V38" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="W38" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="X38" s="7"/>
-      <c r="Y38" s="7">
+      <c r="W38" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="X38" s="49">
+        <f>SUM(X37:X37)*18+Y37</f>
         <v>2</v>
       </c>
-      <c r="Z38" s="14">
-        <v>45986</v>
-      </c>
-      <c r="AA38" s="9">
-        <f t="shared" ref="AA38" si="33">(Z38-$AC$1)/365*12</f>
-        <v>9.8630136986301373</v>
-      </c>
+      <c r="Y38" s="50"/>
       <c r="AB38" s="7"/>
     </row>
     <row r="39" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C39" s="49">
         <f>SUM(C36:C38)*30+D36</f>
@@ -3092,7 +3077,7 @@
       <c r="F39" s="7"/>
       <c r="G39" s="33"/>
       <c r="I39" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J39" s="49">
         <f>SUM(J37:J38)*24+K37</f>
@@ -3102,7 +3087,7 @@
       <c r="N39" s="33"/>
       <c r="O39" s="24"/>
       <c r="P39" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="Q39" s="7">
         <v>33</v>
@@ -3116,14 +3101,6 @@
         <v>16.865753424657534</v>
       </c>
       <c r="U39" s="33"/>
-      <c r="W39" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="X39" s="49">
-        <f>SUM(X38:X38)*18+Y38</f>
-        <v>2</v>
-      </c>
-      <c r="Y39" s="50"/>
       <c r="AB39" s="7"/>
     </row>
     <row r="40" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3137,7 +3114,7 @@
       <c r="N40" s="33"/>
       <c r="O40" s="24"/>
       <c r="P40" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q40" s="7">
         <v>69</v>
@@ -3157,10 +3134,10 @@
     </row>
     <row r="41" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B41" s="44" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C41" s="7">
         <v>1</v>
@@ -3177,7 +3154,7 @@
       </c>
       <c r="G41" s="33"/>
       <c r="H41" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I41" s="7">
         <v>156642</v>
@@ -3192,12 +3169,12 @@
         <v>46197</v>
       </c>
       <c r="M41" s="9">
-        <f t="shared" ref="M41:M42" si="34">(L41-$AC$1)/365*12</f>
+        <f t="shared" ref="M41:M42" si="33">(L41-$AC$1)/365*12</f>
         <v>16.799999999999997</v>
       </c>
       <c r="N41" s="33"/>
       <c r="P41" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q41" s="49">
         <f>SUM(Q38:Q40)*30+R38+R40</f>
@@ -3210,7 +3187,7 @@
     <row r="42" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="6"/>
       <c r="B42" s="44" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C42" s="7">
         <v>62</v>
@@ -3236,7 +3213,7 @@
         <v>46197</v>
       </c>
       <c r="M42" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>16.799999999999997</v>
       </c>
       <c r="N42" s="33"/>
@@ -3245,7 +3222,7 @@
     </row>
     <row r="43" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B43" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C43" s="49">
         <f>SUM(C41:C42)*30+D41</f>
@@ -3255,7 +3232,7 @@
       <c r="F43" s="7"/>
       <c r="G43" s="33"/>
       <c r="I43" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J43" s="49">
         <f>SUM(J41:J42)*24+K41</f>
@@ -3264,7 +3241,7 @@
       <c r="K43" s="50"/>
       <c r="N43" s="33"/>
       <c r="O43" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="P43" s="7">
         <v>3</v>
@@ -3285,10 +3262,10 @@
     </row>
     <row r="45" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B45" s="44" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C45" s="7">
         <v>0</v>
@@ -3300,12 +3277,12 @@
         <v>46291</v>
       </c>
       <c r="F45" s="9">
-        <f t="shared" ref="F45:F46" si="35">(E45-$AC$1)/365*12</f>
+        <f t="shared" ref="F45:F46" si="34">(E45-$AC$1)/365*12</f>
         <v>19.890410958904109</v>
       </c>
       <c r="G45" s="33"/>
       <c r="H45" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I45" s="7">
         <v>156641</v>
@@ -3320,12 +3297,12 @@
         <v>46197</v>
       </c>
       <c r="M45" s="9">
-        <f t="shared" ref="M45:M46" si="36">(L45-$AC$1)/365*12</f>
+        <f t="shared" ref="M45:M46" si="35">(L45-$AC$1)/365*12</f>
         <v>16.799999999999997</v>
       </c>
       <c r="N45" s="33"/>
       <c r="O45" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P45" s="7">
         <v>49</v>
@@ -3336,7 +3313,7 @@
     <row r="46" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
       <c r="B46" s="44" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C46" s="11">
         <v>55</v>
@@ -3348,7 +3325,7 @@
         <v>46352</v>
       </c>
       <c r="F46" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>21.895890410958906</v>
       </c>
       <c r="G46" s="33"/>
@@ -3363,7 +3340,7 @@
         <v>46303</v>
       </c>
       <c r="M46" s="9">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>20.284931506849315</v>
       </c>
       <c r="N46" s="33"/>
@@ -3372,7 +3349,7 @@
     </row>
     <row r="47" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B47" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C47" s="49">
         <f>SUM(C45:C46)*30+D45</f>
@@ -3383,7 +3360,7 @@
       <c r="G47" s="33"/>
       <c r="H47" s="36"/>
       <c r="I47" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J47" s="49">
         <f>SUM(J45:J46)*24+K45</f>
@@ -3408,10 +3385,10 @@
     </row>
     <row r="49" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B49" s="43" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C49" s="7">
         <v>7</v>
@@ -3423,7 +3400,7 @@
         <v>46260</v>
       </c>
       <c r="F49" s="9">
-        <f t="shared" ref="F49:F50" si="37">(E49-$AC$1)/365*12</f>
+        <f t="shared" ref="F49:F50" si="36">(E49-$AC$1)/365*12</f>
         <v>18.871232876712327</v>
       </c>
       <c r="G49" s="33"/>
@@ -3439,7 +3416,7 @@
     <row r="50" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6"/>
       <c r="B50" s="43" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C50" s="7">
         <v>53</v>
@@ -3451,7 +3428,7 @@
         <v>46291</v>
       </c>
       <c r="F50" s="9">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>19.890410958904109</v>
       </c>
       <c r="G50" s="33"/>
@@ -3466,7 +3443,7 @@
     </row>
     <row r="51" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C51" s="49" cm="1">
         <f t="array" ref="C51">SUM(C49:C50*40)+D49+D50</f>
@@ -3492,10 +3469,10 @@
     </row>
     <row r="53" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B53" s="44" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C53" s="7">
         <v>10</v>
@@ -3518,7 +3495,7 @@
     </row>
     <row r="54" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B54" s="47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C54" s="49">
         <f>SUM(C53)*30+D53</f>
@@ -4416,6 +4393,12 @@
       <c r="R190"/>
       <c r="S190"/>
       <c r="T190"/>
+      <c r="V190"/>
+      <c r="W190"/>
+      <c r="X190"/>
+      <c r="Y190"/>
+      <c r="Z190"/>
+      <c r="AA190"/>
       <c r="AB190" s="4"/>
     </row>
     <row r="191" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
@@ -4589,14 +4572,14 @@
     <mergeCell ref="X5:Y5"/>
     <mergeCell ref="X9:Y9"/>
     <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="X18:Y18"/>
-    <mergeCell ref="X21:Y21"/>
-    <mergeCell ref="X24:Y24"/>
-    <mergeCell ref="V26:V27"/>
-    <mergeCell ref="X32:Y32"/>
-    <mergeCell ref="X28:Y28"/>
-    <mergeCell ref="X39:Y39"/>
-    <mergeCell ref="X36:Y36"/>
+    <mergeCell ref="X17:Y17"/>
+    <mergeCell ref="X20:Y20"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="V25:V26"/>
+    <mergeCell ref="X31:Y31"/>
+    <mergeCell ref="X27:Y27"/>
+    <mergeCell ref="X38:Y38"/>
+    <mergeCell ref="X35:Y35"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update lot codes - 2025-02-01 17:26:55
</commit_message>
<xml_diff>
--- a/LotCode.xlsx
+++ b/LotCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf.sharepoint.com/sites/production-warehouse/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7182" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A41A2C5-8F75-43B6-AAD7-4E80742776BB}"/>
+  <xr:revisionPtr revIDLastSave="7269" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39A3E9BF-8CDA-4E2F-BE0E-03911E557E92}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="a/VZ8kgdZMyU/a42HcB04O8OBNrnh4WxCIPRCv9GqcObOgYeM9oYcSfQqndR/nnirMykfzLaq88Ahwir6HajhQ==" workbookSaltValue="jsEDzk1n/+JkLoe+dWrmxg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="104">
   <si>
     <t>SKU</t>
   </si>
@@ -229,9 +229,6 @@
     <t>158236</t>
   </si>
   <si>
-    <t>158226</t>
-  </si>
-  <si>
     <t>TS-EDI-STRESS-PB</t>
   </si>
   <si>
@@ -352,9 +349,6 @@
     <t>1124FS313</t>
   </si>
   <si>
-    <t>1.17.25</t>
-  </si>
-  <si>
     <t>1124T119</t>
   </si>
   <si>
@@ -371,6 +365,15 @@
   </si>
   <si>
     <t>PRSS2411-4</t>
+  </si>
+  <si>
+    <t>161796</t>
+  </si>
+  <si>
+    <t>158237</t>
+  </si>
+  <si>
+    <t>1.31.25</t>
   </si>
 </sst>
 </file>
@@ -613,7 +616,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -741,10 +744,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1089,9 +1095,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4D02CE-C7F3-446F-985C-950AF7BFACB9}">
   <dimension ref="A1:AE283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W21" sqref="W21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,32 +1213,32 @@
         <v>6</v>
       </c>
       <c r="AC1" s="20">
-        <v>45686</v>
+        <v>45688</v>
       </c>
       <c r="AE1" s="5"/>
     </row>
     <row r="2" spans="1:31" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="42" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="G2" s="32"/>
       <c r="H2" s="23" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="N2" s="32"/>
       <c r="O2" s="23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="U2" s="32"/>
       <c r="V2" s="42" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AB2" s="8"/>
       <c r="AE2" s="18"/>
     </row>
     <row r="3" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="40">
         <v>159368</v>
@@ -1248,17 +1254,17 @@
       </c>
       <c r="F3" s="9">
         <f t="shared" ref="F3:F5" si="0">(E3-$AC$1)/365*12</f>
-        <v>20.317808219178083</v>
+        <v>20.252054794520546</v>
       </c>
       <c r="G3" s="33"/>
       <c r="H3" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I3" s="7">
-        <v>155511</v>
+        <v>62</v>
+      </c>
+      <c r="I3" s="53">
+        <v>158587</v>
       </c>
       <c r="J3" s="7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K3" s="7">
         <v>9</v>
@@ -1268,7 +1274,7 @@
       </c>
       <c r="M3" s="9">
         <f t="shared" ref="M3:M4" si="1">(L3-$AC$1)/365*12</f>
-        <v>13.413698630136988</v>
+        <v>13.347945205479453</v>
       </c>
       <c r="N3" s="33"/>
       <c r="O3" s="6" t="s">
@@ -1288,14 +1294,14 @@
       </c>
       <c r="T3" s="9">
         <f t="shared" ref="T3:T5" si="2">(S3-$AC$1)/365*12</f>
-        <v>19.890410958904109</v>
+        <v>19.824657534246576</v>
       </c>
       <c r="U3" s="33"/>
       <c r="V3" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="W3" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="X3" s="7">
         <v>9</v>
@@ -1308,7 +1314,7 @@
       </c>
       <c r="AA3" s="9">
         <f t="shared" ref="AA3" si="3">(Z3-$AC$1)/365*12</f>
-        <v>43.989041095890407</v>
+        <v>43.923287671232877</v>
       </c>
       <c r="AB3" s="12"/>
     </row>
@@ -1325,7 +1331,7 @@
       </c>
       <c r="F4" s="9">
         <f t="shared" si="0"/>
-        <v>20.942465753424656</v>
+        <v>20.876712328767123</v>
       </c>
       <c r="G4" s="33"/>
       <c r="I4" s="7">
@@ -1340,7 +1346,7 @@
       </c>
       <c r="M4" s="9">
         <f t="shared" si="1"/>
-        <v>20.515068493150686</v>
+        <v>20.449315068493153</v>
       </c>
       <c r="N4" s="33"/>
       <c r="O4" s="27"/>
@@ -1356,11 +1362,11 @@
       </c>
       <c r="T4" s="9">
         <f t="shared" si="2"/>
-        <v>19.890410958904109</v>
+        <v>19.824657534246576</v>
       </c>
       <c r="U4" s="33"/>
       <c r="W4" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="X4" s="15">
         <v>177</v>
@@ -1373,7 +1379,7 @@
       </c>
       <c r="AA4" s="9">
         <f t="shared" ref="AA4" si="4">(Z4-$AC$1)/365*12</f>
-        <v>43.989041095890407</v>
+        <v>43.923287671232877</v>
       </c>
       <c r="AB4" s="7"/>
     </row>
@@ -1382,7 +1388,7 @@
         <v>162840</v>
       </c>
       <c r="C5" s="40">
-        <v>155</v>
+        <v>110</v>
       </c>
       <c r="D5" s="40"/>
       <c r="E5" s="41">
@@ -1390,7 +1396,7 @@
       </c>
       <c r="F5" s="9">
         <f t="shared" si="0"/>
-        <v>20.942465753424656</v>
+        <v>20.876712328767123</v>
       </c>
       <c r="G5" s="33"/>
       <c r="I5" s="46" t="s">
@@ -1398,13 +1404,13 @@
       </c>
       <c r="J5" s="49">
         <f>SUM(J3:J4)*40+K3</f>
-        <v>4369</v>
+        <v>4329</v>
       </c>
       <c r="K5" s="50"/>
       <c r="N5" s="33"/>
       <c r="O5" s="27"/>
       <c r="P5" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="Q5" s="7">
         <v>195</v>
@@ -1417,7 +1423,7 @@
       </c>
       <c r="T5" s="9">
         <f t="shared" si="2"/>
-        <v>23.934246575342467</v>
+        <v>23.868493150684934</v>
       </c>
       <c r="U5" s="33"/>
       <c r="W5" s="46" t="s">
@@ -1436,7 +1442,7 @@
       </c>
       <c r="C6" s="49">
         <f>SUM(C3:C5)*40+D3</f>
-        <v>8268</v>
+        <v>6468</v>
       </c>
       <c r="D6" s="50"/>
       <c r="F6" s="7"/>
@@ -1464,28 +1470,28 @@
       <c r="F7" s="7"/>
       <c r="G7" s="33"/>
       <c r="H7" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I7" s="7">
-        <v>156645</v>
+        <v>163237</v>
       </c>
       <c r="J7" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K7" s="7">
         <v>10</v>
       </c>
       <c r="L7" s="8">
-        <v>46185</v>
+        <v>46310</v>
       </c>
       <c r="M7" s="9">
         <f t="shared" ref="M7:M8" si="5">(L7-$AC$1)/365*12</f>
-        <v>16.405479452054795</v>
+        <v>20.449315068493153</v>
       </c>
       <c r="N7" s="33"/>
       <c r="U7" s="33"/>
       <c r="V7" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="W7" s="7" t="s">
         <v>12</v>
@@ -1501,19 +1507,19 @@
       </c>
       <c r="AA7" s="9">
         <f t="shared" ref="AA7" si="6">(Z7-$AC$1)/365*12</f>
-        <v>42.969863013698628</v>
+        <v>42.904109589041099</v>
       </c>
       <c r="AB7" s="7"/>
     </row>
     <row r="8" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="7">
         <v>158583</v>
       </c>
       <c r="C8" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" s="7">
         <v>8</v>
@@ -1523,23 +1529,23 @@
       </c>
       <c r="F8" s="9">
         <f t="shared" ref="F8" si="7">(E8-$AC$1)/365*12</f>
-        <v>18.542465753424658</v>
+        <v>18.476712328767121</v>
       </c>
       <c r="G8" s="33"/>
       <c r="H8" s="27"/>
       <c r="I8" s="7">
-        <v>163237</v>
+        <v>161791</v>
       </c>
       <c r="J8" s="7">
-        <v>73</v>
+        <v>148</v>
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="8">
-        <v>46310</v>
+        <v>46325</v>
       </c>
       <c r="M8" s="9">
         <f t="shared" si="5"/>
-        <v>20.515068493150686</v>
+        <v>20.942465753424656</v>
       </c>
       <c r="N8" s="33"/>
       <c r="O8" s="6" t="s">
@@ -1559,11 +1565,11 @@
       </c>
       <c r="T8" s="9">
         <f t="shared" ref="T8:T10" si="8">(S8-$AC$1)/365*12</f>
-        <v>19.890410958904109</v>
+        <v>19.824657534246576</v>
       </c>
       <c r="U8" s="33"/>
       <c r="W8" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="X8" s="7">
         <v>54</v>
@@ -1576,42 +1582,35 @@
       </c>
       <c r="AA8" s="9">
         <f t="shared" ref="AA8" si="9">(Z8-$AC$1)/365*12</f>
-        <v>45.994520547945207</v>
+        <v>45.92876712328767</v>
       </c>
       <c r="AB8" s="7"/>
     </row>
     <row r="9" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="27"/>
       <c r="B9" s="7">
-        <v>158583</v>
+        <v>159367</v>
       </c>
       <c r="C9" s="11">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="8">
-        <v>46250</v>
+        <v>46283</v>
       </c>
       <c r="F9" s="9">
         <f>(E9-$AC$1)/365*12</f>
-        <v>18.542465753424658</v>
+        <v>19.56164383561644</v>
       </c>
       <c r="G9" s="33"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="7">
-        <v>161791</v>
-      </c>
-      <c r="J9" s="7">
-        <v>80</v>
-      </c>
-      <c r="K9" s="7"/>
-      <c r="L9" s="8">
-        <v>46325</v>
-      </c>
-      <c r="M9" s="9">
-        <f t="shared" ref="M9" si="10">(L9-$AC$1)/365*12</f>
-        <v>21.008219178082193</v>
-      </c>
+      <c r="I9" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="49">
+        <f>SUM(J7:J8)*24+K7</f>
+        <v>3634</v>
+      </c>
+      <c r="K9" s="50"/>
       <c r="N9" s="33"/>
       <c r="P9" s="7" t="s">
         <v>49</v>
@@ -1625,7 +1624,7 @@
       </c>
       <c r="T9" s="9">
         <f t="shared" si="8"/>
-        <v>19.890410958904109</v>
+        <v>19.824657534246576</v>
       </c>
       <c r="U9" s="33"/>
       <c r="W9" s="46" t="s">
@@ -1641,31 +1640,24 @@
     <row r="10" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="27"/>
       <c r="B10" s="7">
-        <v>159367</v>
+        <v>161794</v>
       </c>
       <c r="C10" s="11">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="8">
-        <v>46283</v>
+        <v>46324</v>
       </c>
       <c r="F10" s="9">
         <f>(E10-$AC$1)/365*12</f>
-        <v>19.627397260273973</v>
+        <v>20.909589041095892</v>
       </c>
       <c r="G10" s="33"/>
-      <c r="I10" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="49">
-        <f>SUM(J7:J9)*24+K7</f>
-        <v>3682</v>
-      </c>
-      <c r="K10" s="50"/>
+      <c r="K10" s="7"/>
       <c r="N10" s="33"/>
       <c r="P10" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Q10" s="7">
         <v>173</v>
@@ -1676,7 +1668,7 @@
       </c>
       <c r="T10" s="9">
         <f t="shared" si="8"/>
-        <v>23.934246575342467</v>
+        <v>23.868493150684934</v>
       </c>
       <c r="U10" s="33"/>
       <c r="AB10" s="7"/>
@@ -1684,21 +1676,37 @@
     <row r="11" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="27"/>
       <c r="B11" s="7">
-        <v>161794</v>
+        <v>161798</v>
       </c>
       <c r="C11" s="11">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="8">
         <v>46324</v>
       </c>
       <c r="F11" s="9">
-        <f>(E11-$AC$1)/365*12</f>
-        <v>20.975342465753425</v>
+        <f t="shared" ref="F11:F12" si="10">(E11-$AC$1)/365*12</f>
+        <v>20.909589041095892</v>
       </c>
       <c r="G11" s="33"/>
+      <c r="H11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="7">
+        <v>159369</v>
+      </c>
+      <c r="J11" s="7">
+        <v>3</v>
+      </c>
       <c r="K11" s="7"/>
+      <c r="L11" s="8">
+        <v>46338</v>
+      </c>
+      <c r="M11" s="9">
+        <f>(L11-$AC$1)/365*12</f>
+        <v>21.36986301369863</v>
+      </c>
       <c r="N11" s="33"/>
       <c r="P11" s="46" t="s">
         <v>8</v>
@@ -1710,7 +1718,7 @@
       <c r="R11" s="50"/>
       <c r="U11" s="33"/>
       <c r="V11" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="W11" s="7" t="s">
         <v>14</v>
@@ -1726,44 +1734,46 @@
       </c>
       <c r="AA11" s="9">
         <f t="shared" ref="AA11:AA12" si="11">(Z11-$AC$1)/365*12</f>
-        <v>42.969863013698628</v>
+        <v>42.904109589041099</v>
       </c>
       <c r="AB11" s="7"/>
     </row>
     <row r="12" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="49">
-        <f>SUM(C8:C11)*24+D8</f>
-        <v>5456</v>
-      </c>
-      <c r="D12" s="50"/>
-      <c r="F12" s="7"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="7">
+        <v>162036</v>
+      </c>
+      <c r="C12" s="11">
+        <v>22</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8">
+        <v>46337</v>
+      </c>
+      <c r="F12" s="9">
+        <f t="shared" si="10"/>
+        <v>21.336986301369862</v>
+      </c>
       <c r="G12" s="33"/>
-      <c r="H12" s="6" t="s">
-        <v>65</v>
-      </c>
+      <c r="H12" s="27"/>
       <c r="I12" s="7">
-        <v>163239</v>
+        <v>159369</v>
       </c>
       <c r="J12" s="7">
-        <v>0</v>
-      </c>
-      <c r="K12" s="7">
-        <v>19</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="K12" s="7"/>
       <c r="L12" s="8">
-        <v>46311</v>
+        <v>46338</v>
       </c>
       <c r="M12" s="9">
         <f>(L12-$AC$1)/365*12</f>
-        <v>20.547945205479451</v>
+        <v>21.36986301369863</v>
       </c>
       <c r="N12" s="33"/>
       <c r="U12" s="33"/>
       <c r="W12" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="X12" s="7">
         <v>202</v>
@@ -1774,28 +1784,35 @@
       </c>
       <c r="AA12" s="9">
         <f t="shared" si="11"/>
-        <v>43.989041095890407</v>
+        <v>43.923287671232877</v>
       </c>
       <c r="AB12" s="7"/>
     </row>
     <row r="13" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D13" s="7"/>
+      <c r="B13" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="49">
+        <f>SUM(C8:C12)*24+D8</f>
+        <v>5336</v>
+      </c>
+      <c r="D13" s="50"/>
       <c r="F13" s="7"/>
       <c r="G13" s="33"/>
       <c r="H13" s="27"/>
       <c r="I13" s="7">
-        <v>159369</v>
+        <v>162047</v>
       </c>
       <c r="J13" s="7">
-        <v>80</v>
+        <v>169</v>
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="8">
-        <v>46338</v>
+        <v>46359</v>
       </c>
       <c r="M13" s="9">
         <f>(L13-$AC$1)/365*12</f>
-        <v>21.435616438356163</v>
+        <v>22.06027397260274</v>
       </c>
       <c r="N13" s="33"/>
       <c r="O13" s="6" t="s">
@@ -1815,7 +1832,7 @@
       </c>
       <c r="T13" s="9">
         <f t="shared" ref="T13:T14" si="12">(S13-$AC$1)/365*12</f>
-        <v>16.865753424657534</v>
+        <v>16.799999999999997</v>
       </c>
       <c r="U13" s="33"/>
       <c r="W13" s="46" t="s">
@@ -1829,38 +1846,28 @@
       <c r="AB13" s="7"/>
     </row>
     <row r="14" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="35">
-        <v>158221</v>
-      </c>
-      <c r="C14" s="7">
-        <v>4</v>
-      </c>
       <c r="D14" s="7"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
+      <c r="F14" s="7"/>
       <c r="G14" s="33"/>
       <c r="H14" s="27"/>
       <c r="I14" s="7">
-        <v>162047</v>
+        <v>162048</v>
       </c>
       <c r="J14" s="7">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="K14" s="7"/>
       <c r="L14" s="8">
-        <v>46359</v>
+        <v>46374</v>
       </c>
       <c r="M14" s="9">
         <f>(L14-$AC$1)/365*12</f>
-        <v>22.126027397260273</v>
+        <v>22.553424657534247</v>
       </c>
       <c r="N14" s="33"/>
       <c r="O14" s="27"/>
       <c r="P14" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q14" s="7">
         <v>120</v>
@@ -1873,33 +1880,36 @@
       </c>
       <c r="T14" s="9">
         <f t="shared" si="12"/>
-        <v>20.876712328767123</v>
+        <v>20.81095890410959</v>
       </c>
       <c r="U14" s="33"/>
       <c r="AB14" s="7"/>
     </row>
     <row r="15" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="B15" s="35">
-        <v>158221</v>
-      </c>
-      <c r="C15" s="11">
-        <v>37</v>
+        <v>159366</v>
+      </c>
+      <c r="C15" s="7">
+        <v>4</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="8">
-        <v>46249</v>
+        <v>46283</v>
       </c>
       <c r="F15" s="9">
         <f>(E15-$AC$1)/365*12</f>
-        <v>18.509589041095889</v>
+        <v>19.56164383561644</v>
       </c>
       <c r="G15" s="33"/>
       <c r="I15" s="46" t="s">
         <v>8</v>
       </c>
       <c r="J15" s="49">
-        <f>SUM(J12:J13)*24+K12</f>
-        <v>1939</v>
+        <f>SUM(J11:J14)*24+K11</f>
+        <v>5520</v>
       </c>
       <c r="K15" s="50"/>
       <c r="N15" s="33"/>
@@ -1913,10 +1923,10 @@
       <c r="R15" s="50"/>
       <c r="U15" s="33"/>
       <c r="V15" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W15" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="X15" s="7">
         <v>12</v>
@@ -1929,24 +1939,24 @@
       </c>
       <c r="AA15" s="9">
         <f t="shared" ref="AA15:AA16" si="13">(Z15-$AC$1)/365*12</f>
-        <v>43.989041095890407</v>
+        <v>43.923287671232877</v>
       </c>
       <c r="AB15" s="7"/>
     </row>
     <row r="16" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="35">
-        <v>159366</v>
-      </c>
-      <c r="C16" s="11">
-        <v>19</v>
-      </c>
-      <c r="D16" s="7"/>
+        <v>158221</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="7">
+        <v>18</v>
+      </c>
       <c r="E16" s="8">
-        <v>46283</v>
+        <v>46249</v>
       </c>
       <c r="F16" s="9">
-        <f t="shared" ref="F16:F17" si="14">(E16-$AC$1)/365*12</f>
-        <v>19.627397260273973</v>
+        <f>(E16-$AC$1)/365*12</f>
+        <v>18.443835616438356</v>
       </c>
       <c r="G16" s="33"/>
       <c r="K16" s="7"/>
@@ -1954,7 +1964,7 @@
       <c r="U16" s="33"/>
       <c r="V16" s="6"/>
       <c r="W16" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="X16" s="7">
         <v>73</v>
@@ -1967,7 +1977,7 @@
       </c>
       <c r="AA16" s="9">
         <f t="shared" si="13"/>
-        <v>45.994520547945207</v>
+        <v>45.92876712328767</v>
       </c>
       <c r="AB16" s="8"/>
     </row>
@@ -1983,12 +1993,12 @@
         <v>46313</v>
       </c>
       <c r="F17" s="9">
-        <f t="shared" si="14"/>
-        <v>20.613698630136987</v>
+        <f t="shared" ref="F17" si="14">(E17-$AC$1)/365*12</f>
+        <v>20.547945205479451</v>
       </c>
       <c r="G17" s="33"/>
       <c r="H17" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I17" s="7">
         <v>163238</v>
@@ -2003,8 +2013,8 @@
         <v>46310</v>
       </c>
       <c r="M17" s="9">
-        <f t="shared" ref="M17:M18" si="15">(L17-$AC$1)/365*12</f>
-        <v>20.515068493150686</v>
+        <f t="shared" ref="M17:M19" si="15">(L17-$AC$1)/365*12</f>
+        <v>20.449315068493153</v>
       </c>
       <c r="N17" s="33"/>
       <c r="O17" s="6" t="s">
@@ -2024,7 +2034,7 @@
       </c>
       <c r="T17" s="9">
         <f t="shared" ref="T17" si="16">(S17-$AC$1)/365*12</f>
-        <v>16.865753424657534</v>
+        <v>16.799999999999997</v>
       </c>
       <c r="U17" s="33"/>
       <c r="W17" s="46" t="s">
@@ -2038,22 +2048,27 @@
       <c r="AB17" s="7"/>
     </row>
     <row r="18" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="49">
-        <f>SUM(C14:C17)*24+D14</f>
-        <v>4824</v>
-      </c>
-      <c r="D18" s="50"/>
-      <c r="F18" s="7"/>
+      <c r="B18" s="35">
+        <v>161794</v>
+      </c>
+      <c r="C18" s="11">
+        <v>69</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8">
+        <v>46324</v>
+      </c>
+      <c r="F18" s="9">
+        <f t="shared" ref="F18" si="17">(E18-$AC$1)/365*12</f>
+        <v>20.909589041095892</v>
+      </c>
       <c r="G18" s="33"/>
       <c r="H18" s="6"/>
       <c r="I18" s="7">
         <v>161792</v>
       </c>
       <c r="J18" s="7">
-        <v>188</v>
+        <v>105</v>
       </c>
       <c r="K18" s="11"/>
       <c r="L18" s="8">
@@ -2061,11 +2076,11 @@
       </c>
       <c r="M18" s="9">
         <f t="shared" si="15"/>
-        <v>21.008219178082193</v>
+        <v>20.942465753424656</v>
       </c>
       <c r="N18" s="33"/>
       <c r="P18" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q18" s="7">
         <v>36</v>
@@ -2077,27 +2092,38 @@
         <v>46321</v>
       </c>
       <c r="T18" s="9">
-        <f t="shared" ref="T18" si="17">(S18-$AC$1)/365*12</f>
-        <v>20.876712328767123</v>
+        <f t="shared" ref="T18" si="18">(S18-$AC$1)/365*12</f>
+        <v>20.81095890410959</v>
       </c>
       <c r="U18" s="33"/>
       <c r="AB18" s="7"/>
     </row>
     <row r="19" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="43"/>
-      <c r="D19" s="7"/>
+      <c r="B19" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="49">
+        <f>SUM(C15:C18)*24+D16</f>
+        <v>5154</v>
+      </c>
+      <c r="D19" s="50"/>
       <c r="F19" s="7"/>
       <c r="G19" s="33"/>
-      <c r="I19" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="J19" s="49">
-        <f>SUM(J17:J18)*12+K17</f>
-        <v>2275</v>
-      </c>
-      <c r="K19" s="50"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="7">
+        <v>162032</v>
+      </c>
+      <c r="J19" s="7">
+        <v>98</v>
+      </c>
+      <c r="K19" s="11"/>
+      <c r="L19" s="8">
+        <v>46361</v>
+      </c>
+      <c r="M19" s="9">
+        <f t="shared" si="15"/>
+        <v>22.126027397260273</v>
+      </c>
       <c r="N19" s="33"/>
       <c r="P19" s="46" t="s">
         <v>8</v>
@@ -2125,32 +2151,25 @@
       </c>
       <c r="AA19" s="9">
         <f>(Z19-$AC$1)/365*12</f>
-        <v>42.969863013698628</v>
+        <v>42.904109589041099</v>
       </c>
       <c r="AB19" s="7"/>
     </row>
     <row r="20" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="11">
-        <v>6</v>
-      </c>
-      <c r="D20" s="7">
-        <v>0</v>
-      </c>
-      <c r="E20" s="8">
-        <v>46198</v>
-      </c>
-      <c r="F20" s="9">
-        <f>(E20-$AC$1)/365*12</f>
-        <v>16.832876712328769</v>
-      </c>
+      <c r="B20" s="43"/>
+      <c r="D20" s="7"/>
+      <c r="F20" s="7"/>
       <c r="G20" s="33"/>
-      <c r="K20" s="7"/>
+      <c r="I20" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="49">
+        <f>SUM(J17:J19)*12+K17</f>
+        <v>2455</v>
+      </c>
+      <c r="K20" s="50"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
       <c r="N20" s="33"/>
       <c r="P20" s="13"/>
       <c r="Q20" s="10" t="s">
@@ -2167,41 +2186,28 @@
       <c r="Y20" s="50"/>
       <c r="AB20" s="7"/>
     </row>
-    <row r="21" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="27"/>
+    <row r="21" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="B21" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="C21" s="7">
-        <v>149</v>
+        <v>93</v>
+      </c>
+      <c r="C21" s="11">
+        <v>6</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0</v>
       </c>
       <c r="E21" s="8">
         <v>46283</v>
       </c>
       <c r="F21" s="9">
-        <f t="shared" ref="F21" si="18">(E21-$AC$1)/365*12</f>
-        <v>19.627397260273973</v>
+        <f t="shared" ref="F21" si="19">(E21-$AC$1)/365*12</f>
+        <v>19.56164383561644</v>
       </c>
       <c r="G21" s="33"/>
-      <c r="H21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J21" s="7">
-        <v>4</v>
-      </c>
-      <c r="K21" s="7">
-        <v>18</v>
-      </c>
-      <c r="L21" s="14">
-        <v>46291</v>
-      </c>
-      <c r="M21" s="9">
-        <f t="shared" ref="M21" si="19">(L21-$AC$1)/365*12</f>
-        <v>19.890410958904109</v>
-      </c>
+      <c r="K21" s="7"/>
       <c r="N21" s="33"/>
       <c r="O21" s="6" t="s">
         <v>19</v>
@@ -2220,35 +2226,45 @@
       </c>
       <c r="T21" s="9">
         <f t="shared" ref="T21:T22" si="20">(S21-$AC$1)/365*12</f>
-        <v>19.890410958904109</v>
+        <v>19.824657534246576</v>
       </c>
       <c r="U21" s="33"/>
       <c r="AB21" s="7"/>
     </row>
     <row r="22" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="49">
-        <f>SUM(C20:C21)*12+D20</f>
-        <v>1860</v>
-      </c>
-      <c r="D22" s="50"/>
-      <c r="F22" s="7"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="7">
+        <v>74</v>
+      </c>
+      <c r="E22" s="8">
+        <v>46283</v>
+      </c>
+      <c r="F22" s="9">
+        <f t="shared" ref="F22:F23" si="21">(E22-$AC$1)/365*12</f>
+        <v>19.56164383561644</v>
+      </c>
       <c r="G22" s="33"/>
+      <c r="H22" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="I22" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J22" s="7">
-        <v>16</v>
-      </c>
-      <c r="K22" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="K22" s="7">
+        <v>18</v>
+      </c>
       <c r="L22" s="14">
         <v>46291</v>
       </c>
       <c r="M22" s="9">
-        <f t="shared" ref="M22:M23" si="21">(L22-$AC$1)/365*12</f>
-        <v>19.890410958904109</v>
+        <f t="shared" ref="M22" si="22">(L22-$AC$1)/365*12</f>
+        <v>19.824657534246576</v>
       </c>
       <c r="N22" s="33"/>
       <c r="P22" s="7" t="s">
@@ -2263,11 +2279,11 @@
       </c>
       <c r="T22" s="9">
         <f t="shared" si="20"/>
-        <v>19.890410958904109</v>
+        <v>19.824657534246576</v>
       </c>
       <c r="U22" s="33"/>
       <c r="V22" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="W22" s="7" t="s">
         <v>27</v>
@@ -2282,18 +2298,29 @@
         <v>46993</v>
       </c>
       <c r="AA22" s="9">
-        <f t="shared" ref="AA22" si="22">(Z22-$AC$1)/365*12</f>
-        <v>42.969863013698628</v>
+        <f t="shared" ref="AA22" si="23">(Z22-$AC$1)/365*12</f>
+        <v>42.904109589041099</v>
       </c>
       <c r="AB22" s="7"/>
     </row>
     <row r="23" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="43"/>
-      <c r="D23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="7">
+        <v>101</v>
+      </c>
+      <c r="E23" s="8">
+        <v>46303</v>
+      </c>
+      <c r="F23" s="9">
+        <f t="shared" si="21"/>
+        <v>20.219178082191782</v>
+      </c>
       <c r="G23" s="33"/>
       <c r="I23" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J23" s="7">
         <v>86</v>
@@ -2305,8 +2332,8 @@
         <v>46352</v>
       </c>
       <c r="M23" s="9">
-        <f t="shared" si="21"/>
-        <v>21.895890410958906</v>
+        <f t="shared" ref="M23" si="24">(L23-$AC$1)/365*12</f>
+        <v>21.830136986301369</v>
       </c>
       <c r="N23" s="33"/>
       <c r="P23" s="46" t="s">
@@ -2329,54 +2356,32 @@
       <c r="AB23" s="7"/>
     </row>
     <row r="24" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="45">
-        <v>158238</v>
-      </c>
-      <c r="C24" s="7">
-        <v>0</v>
-      </c>
-      <c r="D24" s="7">
-        <v>18</v>
-      </c>
-      <c r="E24" s="8">
-        <v>46190</v>
-      </c>
-      <c r="F24" s="9">
-        <f>(E24-$AC$1)/365*12</f>
-        <v>16.56986301369863</v>
-      </c>
+      <c r="B24" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="49">
+        <f>SUM(C21:C23)*12+D21</f>
+        <v>2172</v>
+      </c>
+      <c r="D24" s="50"/>
+      <c r="F24" s="7"/>
       <c r="G24" s="33"/>
       <c r="I24" s="46" t="s">
         <v>8</v>
       </c>
       <c r="J24" s="49">
-        <f>SUM(J21:J23)*30+K21+K23</f>
-        <v>3202</v>
+        <f>SUM(J22:J23)*30+K22+K23</f>
+        <v>2722</v>
       </c>
       <c r="K24" s="50"/>
       <c r="N24" s="33"/>
       <c r="U24" s="33"/>
       <c r="AB24" s="7"/>
     </row>
-    <row r="25" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="29"/>
-      <c r="B25" s="45">
-        <v>163030</v>
-      </c>
-      <c r="C25" s="11">
-        <v>36</v>
-      </c>
+    <row r="25" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="43"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="8">
-        <v>46302</v>
-      </c>
-      <c r="F25" s="9">
-        <f>(E25-$AC$1)/365*12</f>
-        <v>20.252054794520546</v>
-      </c>
+      <c r="F25" s="7"/>
       <c r="G25" s="33"/>
       <c r="K25" s="7"/>
       <c r="M25" s="10" t="s">
@@ -2399,15 +2404,15 @@
         <v>46199</v>
       </c>
       <c r="T25" s="9">
-        <f t="shared" ref="T25:T27" si="23">(S25-$AC$1)/365*12</f>
-        <v>16.865753424657534</v>
+        <f t="shared" ref="T25:T27" si="25">(S25-$AC$1)/365*12</f>
+        <v>16.799999999999997</v>
       </c>
       <c r="U25" s="33"/>
-      <c r="V25" s="51" t="s">
-        <v>75</v>
+      <c r="V25" s="52" t="s">
+        <v>74</v>
       </c>
       <c r="W25" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="X25" s="7">
         <v>43</v>
@@ -2419,21 +2424,31 @@
         <v>47085</v>
       </c>
       <c r="AA25" s="9">
-        <f t="shared" ref="AA25" si="24">(Z25-$AC$1)/365*12</f>
-        <v>45.994520547945207</v>
+        <f t="shared" ref="AA25" si="26">(Z25-$AC$1)/365*12</f>
+        <v>45.92876712328767</v>
       </c>
       <c r="AB25" s="7"/>
     </row>
     <row r="26" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="49">
-        <f>SUM(C24:C25)*40+D24+D25</f>
-        <v>1458</v>
-      </c>
-      <c r="D26" s="50"/>
-      <c r="F26" s="7"/>
+      <c r="A26" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="45">
+        <v>158238</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0</v>
+      </c>
+      <c r="D26" s="7">
+        <v>18</v>
+      </c>
+      <c r="E26" s="8">
+        <v>46190</v>
+      </c>
+      <c r="F26" s="9">
+        <f>(E26-$AC$1)/365*12</f>
+        <v>16.504109589041093</v>
+      </c>
       <c r="G26" s="33"/>
       <c r="H26" s="6" t="s">
         <v>23</v>
@@ -2451,8 +2466,8 @@
         <v>46291</v>
       </c>
       <c r="M26" s="9">
-        <f t="shared" ref="M26:M27" si="25">(L26-$AC$1)/365*12</f>
-        <v>19.890410958904109</v>
+        <f t="shared" ref="M26:M27" si="27">(L26-$AC$1)/365*12</f>
+        <v>19.824657534246576</v>
       </c>
       <c r="N26" s="33"/>
       <c r="P26" s="7" t="s">
@@ -2468,11 +2483,11 @@
         <v>46199</v>
       </c>
       <c r="T26" s="9">
-        <f t="shared" si="23"/>
-        <v>16.865753424657534</v>
+        <f t="shared" si="25"/>
+        <v>16.799999999999997</v>
       </c>
       <c r="U26" s="33"/>
-      <c r="V26" s="51"/>
+      <c r="V26" s="52"/>
       <c r="W26" s="7"/>
       <c r="X26" s="7"/>
       <c r="Y26" s="7"/>
@@ -2481,23 +2496,35 @@
       <c r="AB26" s="7"/>
     </row>
     <row r="27" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="43"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="45">
+        <v>163030</v>
+      </c>
+      <c r="C27" s="11">
+        <v>36</v>
+      </c>
       <c r="D27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="E27" s="8">
+        <v>46302</v>
+      </c>
+      <c r="F27" s="9">
+        <f>(E27-$AC$1)/365*12</f>
+        <v>20.186301369863013</v>
+      </c>
       <c r="G27" s="33"/>
       <c r="I27" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J27" s="7">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K27" s="7"/>
       <c r="L27" s="25">
         <v>46352</v>
       </c>
       <c r="M27" s="9">
-        <f t="shared" si="25"/>
-        <v>21.895890410958906</v>
+        <f t="shared" si="27"/>
+        <v>21.830136986301369</v>
       </c>
       <c r="N27" s="33"/>
       <c r="P27" s="7" t="s">
@@ -2513,8 +2540,8 @@
         <v>46352</v>
       </c>
       <c r="T27" s="9">
-        <f t="shared" si="23"/>
-        <v>21.895890410958906</v>
+        <f t="shared" si="25"/>
+        <v>21.830136986301369</v>
       </c>
       <c r="U27" s="33"/>
       <c r="V27" s="48"/>
@@ -2529,32 +2556,22 @@
       <c r="AB27" s="7"/>
     </row>
     <row r="28" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="44">
-        <v>158234</v>
-      </c>
-      <c r="C28" s="7">
-        <v>3</v>
-      </c>
-      <c r="D28" s="7">
-        <v>0</v>
-      </c>
-      <c r="E28" s="8">
-        <v>46191</v>
-      </c>
-      <c r="F28" s="9">
-        <f>(E28-$AC$1)/365*12</f>
-        <v>16.602739726027398</v>
-      </c>
+      <c r="B28" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="49">
+        <f>SUM(C26:C27)*40+D26+D27</f>
+        <v>1458</v>
+      </c>
+      <c r="D28" s="50"/>
+      <c r="F28" s="7"/>
       <c r="G28" s="33"/>
       <c r="I28" s="46" t="s">
         <v>8</v>
       </c>
       <c r="J28" s="49">
         <f>SUM(J26:J27)*30+K26</f>
-        <v>2322</v>
+        <v>2292</v>
       </c>
       <c r="K28" s="50"/>
       <c r="N28" s="33"/>
@@ -2569,21 +2586,10 @@
       <c r="U28" s="33"/>
       <c r="AB28" s="7"/>
     </row>
-    <row r="29" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="7">
-        <v>94</v>
-      </c>
+    <row r="29" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="43"/>
       <c r="D29" s="7"/>
-      <c r="E29" s="8">
-        <v>46211</v>
-      </c>
-      <c r="F29" s="9">
-        <f>(E29-$AC$1)/365*12</f>
-        <v>17.260273972602739</v>
-      </c>
+      <c r="F29" s="7"/>
       <c r="G29" s="33"/>
       <c r="K29" s="7"/>
       <c r="N29" s="33"/>
@@ -2592,7 +2598,7 @@
         <v>33</v>
       </c>
       <c r="W29" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="X29" s="7">
         <v>10</v>
@@ -2604,21 +2610,31 @@
         <v>46321</v>
       </c>
       <c r="AA29" s="9">
-        <f t="shared" ref="AA29:AA30" si="26">(Z29-$AC$1)/365*12</f>
-        <v>20.876712328767123</v>
+        <f t="shared" ref="AA29:AA30" si="28">(Z29-$AC$1)/365*12</f>
+        <v>20.81095890410959</v>
       </c>
       <c r="AB29" s="8"/>
     </row>
     <row r="30" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="49">
-        <f>SUM(C28:C29)*24+D28</f>
-        <v>2328</v>
-      </c>
-      <c r="D30" s="50"/>
-      <c r="F30" s="7"/>
+      <c r="A30" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="44">
+        <v>158234</v>
+      </c>
+      <c r="C30" s="7">
+        <v>3</v>
+      </c>
+      <c r="D30" s="7">
+        <v>0</v>
+      </c>
+      <c r="E30" s="8">
+        <v>46191</v>
+      </c>
+      <c r="F30" s="9">
+        <f>(E30-$AC$1)/365*12</f>
+        <v>16.536986301369865</v>
+      </c>
       <c r="G30" s="33"/>
       <c r="H30" s="6" t="s">
         <v>29</v>
@@ -2636,8 +2652,8 @@
         <v>45528</v>
       </c>
       <c r="M30" s="16">
-        <f t="shared" ref="M30" si="27">(L30-$AC$1)/365*12</f>
-        <v>-5.1945205479452055</v>
+        <f t="shared" ref="M30" si="29">(L30-$AC$1)/365*12</f>
+        <v>-5.2602739726027394</v>
       </c>
       <c r="N30" s="33"/>
       <c r="O30" s="6" t="s">
@@ -2656,12 +2672,12 @@
         <v>46352</v>
       </c>
       <c r="T30" s="9">
-        <f t="shared" ref="T30:T31" si="28">(S30-$AC$1)/365*12</f>
-        <v>21.895890410958906</v>
+        <f t="shared" ref="T30:T31" si="30">(S30-$AC$1)/365*12</f>
+        <v>21.830136986301369</v>
       </c>
       <c r="U30" s="33"/>
       <c r="W30" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="X30" s="7">
         <v>32</v>
@@ -2671,14 +2687,25 @@
         <v>46321</v>
       </c>
       <c r="AA30" s="9">
-        <f t="shared" si="26"/>
-        <v>20.876712328767123</v>
+        <f t="shared" si="28"/>
+        <v>20.81095890410959</v>
       </c>
     </row>
     <row r="31" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="43"/>
+      <c r="B31" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="7">
+        <v>61</v>
+      </c>
       <c r="D31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="E31" s="8">
+        <v>46211</v>
+      </c>
+      <c r="F31" s="9">
+        <f>(E31-$AC$1)/365*12</f>
+        <v>17.194520547945206</v>
+      </c>
       <c r="G31" s="33"/>
       <c r="I31" s="46" t="s">
         <v>8</v>
@@ -2701,8 +2728,8 @@
         <v>46352</v>
       </c>
       <c r="T31" s="9">
-        <f t="shared" si="28"/>
-        <v>21.895890410958906</v>
+        <f t="shared" si="30"/>
+        <v>21.830136986301369</v>
       </c>
       <c r="U31" s="33"/>
       <c r="W31" s="46" t="s">
@@ -2716,24 +2743,19 @@
       <c r="AB31" s="7"/>
     </row>
     <row r="32" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
-        <v>62</v>
-      </c>
       <c r="B32" s="44" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="C32" s="7">
-        <v>4</v>
-      </c>
-      <c r="D32" s="7">
-        <v>6</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D32" s="7"/>
       <c r="E32" s="8">
-        <v>46211</v>
+        <v>46248</v>
       </c>
       <c r="F32" s="9">
         <f>(E32-$AC$1)/365*12</f>
-        <v>17.260273972602739</v>
+        <v>18.410958904109588</v>
       </c>
       <c r="G32" s="33"/>
       <c r="K32" s="7"/>
@@ -2750,24 +2772,18 @@
       <c r="AB32" s="7"/>
     </row>
     <row r="33" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="27"/>
-      <c r="B33" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" s="7">
-        <v>108</v>
-      </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="8">
-        <v>46312</v>
-      </c>
-      <c r="F33" s="9">
-        <f>(E33-$AC$1)/365*12</f>
-        <v>20.580821917808219</v>
-      </c>
+      <c r="B33" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="49">
+        <f>SUM(C30:C32)*24+D30</f>
+        <v>3456</v>
+      </c>
+      <c r="D33" s="50"/>
+      <c r="F33" s="7"/>
       <c r="G33" s="33"/>
       <c r="H33" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I33" s="7">
         <v>162839</v>
@@ -2782,8 +2798,8 @@
         <v>46305</v>
       </c>
       <c r="M33" s="9">
-        <f t="shared" ref="M33:M34" si="29">(L33-$AC$1)/365*12</f>
-        <v>20.350684931506848</v>
+        <f t="shared" ref="M33:M34" si="31">(L33-$AC$1)/365*12</f>
+        <v>20.284931506849315</v>
       </c>
       <c r="N33" s="33"/>
       <c r="U33" s="33"/>
@@ -2791,7 +2807,7 @@
         <v>36</v>
       </c>
       <c r="W33" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="X33" s="11">
         <v>0</v>
@@ -2803,20 +2819,14 @@
         <v>46321</v>
       </c>
       <c r="AA33" s="26">
-        <f t="shared" ref="AA33" si="30">(Z33-$AC$1)/365*12</f>
-        <v>20.876712328767123</v>
+        <f t="shared" ref="AA33" si="32">(Z33-$AC$1)/365*12</f>
+        <v>20.81095890410959</v>
       </c>
       <c r="AB33" s="7"/>
     </row>
     <row r="34" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="49">
-        <f>SUM(C32:C33)*24+D32</f>
-        <v>2694</v>
-      </c>
-      <c r="D34" s="50"/>
+      <c r="B34" s="43"/>
+      <c r="D34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="33"/>
       <c r="I34" s="7">
@@ -2830,8 +2840,8 @@
         <v>46305</v>
       </c>
       <c r="M34" s="9">
-        <f t="shared" si="29"/>
-        <v>20.350684931506848</v>
+        <f t="shared" si="31"/>
+        <v>20.284931506849315</v>
       </c>
       <c r="N34" s="33"/>
       <c r="O34" s="6" t="s">
@@ -2851,12 +2861,12 @@
       </c>
       <c r="T34" s="9">
         <f>(S34-$AC$1)/365*12</f>
-        <v>10.84931506849315</v>
+        <v>10.783561643835617</v>
       </c>
       <c r="U34" s="33"/>
       <c r="V34" s="6"/>
       <c r="W34" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="X34" s="11">
         <v>65</v>
@@ -2869,9 +2879,25 @@
       <c r="AB34" s="7"/>
     </row>
     <row r="35" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="43"/>
-      <c r="D35" s="7"/>
-      <c r="F35" s="7"/>
+      <c r="A35" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="7">
+        <v>4</v>
+      </c>
+      <c r="D35" s="7">
+        <v>6</v>
+      </c>
+      <c r="E35" s="8">
+        <v>46211</v>
+      </c>
+      <c r="F35" s="9">
+        <f>(E35-$AC$1)/365*12</f>
+        <v>17.194520547945206</v>
+      </c>
       <c r="G35" s="33"/>
       <c r="I35" s="46" t="s">
         <v>8</v>
@@ -2895,7 +2921,7 @@
       </c>
       <c r="T35" s="9">
         <f>(S35-$AC$1)/365*12</f>
-        <v>10.84931506849315</v>
+        <v>10.783561643835617</v>
       </c>
       <c r="U35" s="33"/>
       <c r="W35" s="46" t="s">
@@ -2909,24 +2935,20 @@
       <c r="AB35" s="7"/>
     </row>
     <row r="36" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="A36" s="27"/>
       <c r="B36" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="11">
-        <v>1</v>
-      </c>
-      <c r="D36" s="7">
-        <v>6</v>
-      </c>
-      <c r="E36" s="14">
-        <v>46260</v>
+        <v>88</v>
+      </c>
+      <c r="C36" s="7">
+        <v>89</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="8">
+        <v>46312</v>
       </c>
       <c r="F36" s="9">
         <f>(E36-$AC$1)/365*12</f>
-        <v>18.871232876712327</v>
+        <v>20.515068493150686</v>
       </c>
       <c r="G36" s="33"/>
       <c r="K36" s="7"/>
@@ -2945,23 +2967,18 @@
       <c r="AB36" s="7"/>
     </row>
     <row r="37" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="40">
-        <v>23</v>
-      </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="14">
-        <v>46291</v>
-      </c>
-      <c r="F37" s="9">
-        <f>(E37-$AC$1)/365*12</f>
-        <v>19.890410958904109</v>
-      </c>
+      <c r="B37" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="49">
+        <f>SUM(C35:C36)*24+D35</f>
+        <v>2238</v>
+      </c>
+      <c r="D37" s="50"/>
+      <c r="F37" s="7"/>
       <c r="G37" s="33"/>
       <c r="H37" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I37" s="7">
         <v>161789</v>
@@ -2976,8 +2993,8 @@
         <v>46305</v>
       </c>
       <c r="M37" s="9">
-        <f t="shared" ref="M37:M38" si="31">(L37-$AC$1)/365*12</f>
-        <v>20.350684931506848</v>
+        <f t="shared" ref="M37:M38" si="33">(L37-$AC$1)/365*12</f>
+        <v>20.284931506849315</v>
       </c>
       <c r="N37" s="33"/>
       <c r="P37" s="13"/>
@@ -2986,7 +3003,7 @@
       <c r="T37" s="7"/>
       <c r="U37" s="33"/>
       <c r="V37" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W37" s="7" t="s">
         <v>38</v>
@@ -2999,26 +3016,15 @@
         <v>45986</v>
       </c>
       <c r="AA37" s="9">
-        <f t="shared" ref="AA37" si="32">(Z37-$AC$1)/365*12</f>
-        <v>9.8630136986301373</v>
+        <f t="shared" ref="AA37" si="34">(Z37-$AC$1)/365*12</f>
+        <v>9.7972602739726025</v>
       </c>
       <c r="AB37" s="7"/>
     </row>
     <row r="38" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="44" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" s="40">
-        <v>85</v>
-      </c>
+      <c r="B38" s="43"/>
       <c r="D38" s="7"/>
-      <c r="E38" s="14">
-        <v>46352</v>
-      </c>
-      <c r="F38" s="9">
-        <f>(E38-$AC$1)/365*12</f>
-        <v>21.895890410958906</v>
-      </c>
+      <c r="F38" s="7"/>
       <c r="G38" s="33"/>
       <c r="I38" s="7">
         <v>161789</v>
@@ -3031,8 +3037,8 @@
         <v>46305</v>
       </c>
       <c r="M38" s="9">
-        <f t="shared" si="31"/>
-        <v>20.350684931506848</v>
+        <f t="shared" si="33"/>
+        <v>20.284931506849315</v>
       </c>
       <c r="N38" s="33"/>
       <c r="O38" s="6" t="s">
@@ -3052,7 +3058,7 @@
       </c>
       <c r="T38" s="9">
         <f>(S38-$AC$1)/365*12</f>
-        <v>16.865753424657534</v>
+        <v>16.799999999999997</v>
       </c>
       <c r="U38" s="33"/>
       <c r="W38" s="46" t="s">
@@ -3066,15 +3072,25 @@
       <c r="AB38" s="7"/>
     </row>
     <row r="39" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="49">
-        <f>SUM(C36:C38)*30+D36</f>
-        <v>3276</v>
-      </c>
-      <c r="D39" s="50"/>
-      <c r="F39" s="7"/>
+      <c r="A39" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="11">
+        <v>1</v>
+      </c>
+      <c r="D39" s="7">
+        <v>6</v>
+      </c>
+      <c r="E39" s="14">
+        <v>46260</v>
+      </c>
+      <c r="F39" s="9">
+        <f>(E39-$AC$1)/365*12</f>
+        <v>18.805479452054794</v>
+      </c>
       <c r="G39" s="33"/>
       <c r="I39" s="46" t="s">
         <v>8</v>
@@ -3098,15 +3114,26 @@
       </c>
       <c r="T39" s="9">
         <f>(S39-$AC$1)/365*12</f>
-        <v>16.865753424657534</v>
+        <v>16.799999999999997</v>
       </c>
       <c r="U39" s="33"/>
       <c r="AB39" s="7"/>
     </row>
     <row r="40" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="43"/>
+      <c r="B40" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="40">
+        <v>23</v>
+      </c>
       <c r="D40" s="7"/>
-      <c r="F40" s="7"/>
+      <c r="E40" s="14">
+        <v>46291</v>
+      </c>
+      <c r="F40" s="9">
+        <f>(E40-$AC$1)/365*12</f>
+        <v>19.824657534246576</v>
+      </c>
       <c r="G40" s="33"/>
       <c r="I40" s="13"/>
       <c r="J40" s="30"/>
@@ -3114,7 +3141,7 @@
       <c r="N40" s="33"/>
       <c r="O40" s="24"/>
       <c r="P40" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q40" s="7">
         <v>69</v>
@@ -3127,34 +3154,29 @@
       </c>
       <c r="T40" s="9">
         <f>(S40-$AC$1)/365*12</f>
-        <v>21.895890410958906</v>
+        <v>21.830136986301369</v>
       </c>
       <c r="U40" s="34"/>
       <c r="AB40" s="7"/>
     </row>
     <row r="41" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="B41" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="7">
-        <v>1</v>
-      </c>
-      <c r="D41" s="7">
-        <v>13</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="C41" s="40">
+        <v>85</v>
+      </c>
+      <c r="D41" s="7"/>
       <c r="E41" s="14">
-        <v>46260</v>
+        <v>46352</v>
       </c>
       <c r="F41" s="9">
         <f>(E41-$AC$1)/365*12</f>
-        <v>18.871232876712327</v>
+        <v>21.830136986301369</v>
       </c>
       <c r="G41" s="33"/>
       <c r="H41" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I41" s="7">
         <v>156642</v>
@@ -3169,8 +3191,8 @@
         <v>46197</v>
       </c>
       <c r="M41" s="9">
-        <f t="shared" ref="M41:M42" si="33">(L41-$AC$1)/365*12</f>
-        <v>16.799999999999997</v>
+        <f t="shared" ref="M41:M42" si="35">(L41-$AC$1)/365*12</f>
+        <v>16.734246575342464</v>
       </c>
       <c r="N41" s="33"/>
       <c r="P41" s="46" t="s">
@@ -3185,21 +3207,15 @@
       <c r="AB41" s="7"/>
     </row>
     <row r="42" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="6"/>
-      <c r="B42" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="C42" s="7">
-        <v>62</v>
-      </c>
-      <c r="D42" s="7"/>
-      <c r="E42" s="14">
-        <v>46291</v>
-      </c>
-      <c r="F42" s="9">
-        <f>(E42-$AC$1)/365*12</f>
-        <v>19.890410958904109</v>
-      </c>
+      <c r="B42" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="49">
+        <f>SUM(C39:C41)*30+D39</f>
+        <v>3276</v>
+      </c>
+      <c r="D42" s="50"/>
+      <c r="F42" s="7"/>
       <c r="G42" s="33"/>
       <c r="H42" s="27"/>
       <c r="I42" s="7">
@@ -3213,22 +3229,16 @@
         <v>46197</v>
       </c>
       <c r="M42" s="9">
-        <f t="shared" si="33"/>
-        <v>16.799999999999997</v>
+        <f t="shared" si="35"/>
+        <v>16.734246575342464</v>
       </c>
       <c r="N42" s="33"/>
       <c r="U42" s="24"/>
       <c r="AB42" s="7"/>
     </row>
     <row r="43" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C43" s="49">
-        <f>SUM(C41:C42)*30+D41</f>
-        <v>1903</v>
-      </c>
-      <c r="D43" s="50"/>
+      <c r="B43" s="43"/>
+      <c r="D43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="33"/>
       <c r="I43" s="46" t="s">
@@ -3250,9 +3260,25 @@
       <c r="AB43" s="7"/>
     </row>
     <row r="44" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="43"/>
-      <c r="D44" s="7"/>
-      <c r="F44" s="7"/>
+      <c r="A44" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="7">
+        <v>1</v>
+      </c>
+      <c r="D44" s="7">
+        <v>13</v>
+      </c>
+      <c r="E44" s="14">
+        <v>46260</v>
+      </c>
+      <c r="F44" s="9">
+        <f>(E44-$AC$1)/365*12</f>
+        <v>18.805479452054794</v>
+      </c>
       <c r="G44" s="33"/>
       <c r="K44" s="7"/>
       <c r="N44" s="33"/>
@@ -3260,29 +3286,25 @@
       <c r="U44" s="24"/>
       <c r="AB44" s="7"/>
     </row>
-    <row r="45" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="6" t="s">
-        <v>77</v>
-      </c>
+    <row r="45" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="6"/>
       <c r="B45" s="44" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="C45" s="7">
-        <v>0</v>
-      </c>
-      <c r="D45" s="15">
-        <v>2</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="D45" s="7"/>
       <c r="E45" s="14">
         <v>46291</v>
       </c>
       <c r="F45" s="9">
-        <f t="shared" ref="F45:F46" si="34">(E45-$AC$1)/365*12</f>
-        <v>19.890410958904109</v>
+        <f>(E45-$AC$1)/365*12</f>
+        <v>19.824657534246576</v>
       </c>
       <c r="G45" s="33"/>
       <c r="H45" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I45" s="7">
         <v>156641</v>
@@ -3297,8 +3319,8 @@
         <v>46197</v>
       </c>
       <c r="M45" s="9">
-        <f t="shared" ref="M45:M46" si="35">(L45-$AC$1)/365*12</f>
-        <v>16.799999999999997</v>
+        <f t="shared" ref="M45:M46" si="36">(L45-$AC$1)/365*12</f>
+        <v>16.734246575342464</v>
       </c>
       <c r="N45" s="33"/>
       <c r="O45" s="6" t="s">
@@ -3311,23 +3333,15 @@
       <c r="AB45" s="7"/>
     </row>
     <row r="46" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="6"/>
-      <c r="B46" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="C46" s="11">
-        <v>55</v>
-      </c>
-      <c r="D46" s="15">
-        <v>5</v>
-      </c>
-      <c r="E46" s="14">
-        <v>46352</v>
-      </c>
-      <c r="F46" s="9">
-        <f t="shared" si="34"/>
-        <v>21.895890410958906</v>
-      </c>
+      <c r="B46" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="49">
+        <f>SUM(C44:C45)*30+D44</f>
+        <v>1903</v>
+      </c>
+      <c r="D46" s="50"/>
+      <c r="F46" s="7"/>
       <c r="G46" s="33"/>
       <c r="I46" s="7">
         <v>162040</v>
@@ -3340,22 +3354,16 @@
         <v>46303</v>
       </c>
       <c r="M46" s="9">
-        <f t="shared" si="35"/>
-        <v>20.284931506849315</v>
+        <f t="shared" si="36"/>
+        <v>20.219178082191782</v>
       </c>
       <c r="N46" s="33"/>
       <c r="U46" s="24"/>
       <c r="AB46" s="7"/>
     </row>
     <row r="47" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C47" s="49">
-        <f>SUM(C45:C46)*30+D45</f>
-        <v>1652</v>
-      </c>
-      <c r="D47" s="50"/>
+      <c r="B47" s="43"/>
+      <c r="D47" s="7"/>
       <c r="F47" s="7"/>
       <c r="G47" s="33"/>
       <c r="H47" s="36"/>
@@ -3373,9 +3381,25 @@
       <c r="AB47" s="7"/>
     </row>
     <row r="48" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="43"/>
-      <c r="D48" s="7"/>
-      <c r="F48" s="7"/>
+      <c r="A48" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48" s="7">
+        <v>0</v>
+      </c>
+      <c r="D48" s="15">
+        <v>2</v>
+      </c>
+      <c r="E48" s="14">
+        <v>46291</v>
+      </c>
+      <c r="F48" s="9">
+        <f t="shared" ref="F48:F49" si="37">(E48-$AC$1)/365*12</f>
+        <v>19.824657534246576</v>
+      </c>
       <c r="G48" s="33"/>
       <c r="H48" s="24"/>
       <c r="K48" s="7"/>
@@ -3383,25 +3407,23 @@
       <c r="U48" s="24"/>
       <c r="AB48" s="7"/>
     </row>
-    <row r="49" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B49" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="C49" s="7">
-        <v>7</v>
-      </c>
-      <c r="D49" s="11">
-        <v>18</v>
+    <row r="49" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="6"/>
+      <c r="B49" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" s="11">
+        <v>55</v>
+      </c>
+      <c r="D49" s="15">
+        <v>5</v>
       </c>
       <c r="E49" s="14">
-        <v>46260</v>
+        <v>46352</v>
       </c>
       <c r="F49" s="9">
-        <f t="shared" ref="F49:F50" si="36">(E49-$AC$1)/365*12</f>
-        <v>18.871232876712327</v>
+        <f t="shared" si="37"/>
+        <v>21.830136986301369</v>
       </c>
       <c r="G49" s="33"/>
       <c r="I49" s="11"/>
@@ -3414,42 +3436,28 @@
       <c r="AB49" s="7"/>
     </row>
     <row r="50" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="6"/>
-      <c r="B50" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="C50" s="7">
-        <v>53</v>
-      </c>
-      <c r="D50" s="11">
-        <v>9</v>
-      </c>
-      <c r="E50" s="14">
-        <v>46291</v>
-      </c>
-      <c r="F50" s="9">
-        <f t="shared" si="36"/>
-        <v>19.890410958904109</v>
-      </c>
+      <c r="B50" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="49">
+        <f>SUM(C48:C49)*30+D48</f>
+        <v>1652</v>
+      </c>
+      <c r="D50" s="50"/>
+      <c r="F50" s="7"/>
       <c r="G50" s="33"/>
       <c r="I50" s="39"/>
-      <c r="J50" s="52"/>
-      <c r="K50" s="52"/>
+      <c r="J50" s="51"/>
+      <c r="K50" s="51"/>
       <c r="L50" s="24"/>
       <c r="M50" s="24"/>
       <c r="N50" s="24"/>
       <c r="U50" s="24"/>
       <c r="AB50" s="7"/>
     </row>
-    <row r="51" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" s="49" cm="1">
-        <f t="array" ref="C51">SUM(C49:C50*40)+D49+D50</f>
-        <v>2427</v>
-      </c>
-      <c r="D51" s="50"/>
+    <row r="51" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="43"/>
+      <c r="D51" s="7"/>
       <c r="F51" s="7"/>
       <c r="G51" s="33"/>
       <c r="K51" s="7"/>
@@ -3458,9 +3466,25 @@
       <c r="AB51" s="7"/>
     </row>
     <row r="52" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="43"/>
-      <c r="D52" s="7"/>
-      <c r="F52" s="7"/>
+      <c r="A52" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B52" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="C52" s="7">
+        <v>7</v>
+      </c>
+      <c r="D52" s="11">
+        <v>18</v>
+      </c>
+      <c r="E52" s="14">
+        <v>46260</v>
+      </c>
+      <c r="F52" s="9">
+        <f t="shared" ref="F52:F53" si="38">(E52-$AC$1)/365*12</f>
+        <v>18.805479452054794</v>
+      </c>
       <c r="G52" s="33"/>
       <c r="K52" s="7"/>
       <c r="N52" s="24"/>
@@ -3468,24 +3492,22 @@
       <c r="AB52" s="7"/>
     </row>
     <row r="53" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B53" s="44" t="s">
-        <v>45</v>
+      <c r="A53" s="6"/>
+      <c r="B53" s="43" t="s">
+        <v>48</v>
       </c>
       <c r="C53" s="7">
-        <v>10</v>
-      </c>
-      <c r="D53" s="7">
-        <v>19</v>
+        <v>53</v>
+      </c>
+      <c r="D53" s="11">
+        <v>9</v>
       </c>
       <c r="E53" s="14">
-        <v>45528</v>
-      </c>
-      <c r="F53" s="16">
-        <f>(E53-$AC$1)/365*12</f>
-        <v>-5.1945205479452055</v>
+        <v>46291</v>
+      </c>
+      <c r="F53" s="9">
+        <f t="shared" si="38"/>
+        <v>19.824657534246576</v>
       </c>
       <c r="G53" s="33"/>
       <c r="K53" s="7"/>
@@ -3497,9 +3519,9 @@
       <c r="B54" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C54" s="49">
-        <f>SUM(C53)*30+D53</f>
-        <v>319</v>
+      <c r="C54" s="49" cm="1">
+        <f t="array" ref="C54">SUM(C52:C53*40)+D52+D53</f>
+        <v>2427</v>
       </c>
       <c r="D54" s="50"/>
       <c r="F54" s="7"/>
@@ -3511,6 +3533,7 @@
       <c r="AB54" s="7"/>
     </row>
     <row r="55" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="43"/>
       <c r="D55" s="7"/>
       <c r="F55" s="7"/>
       <c r="G55" s="33"/>
@@ -3518,16 +3541,40 @@
       <c r="U55" s="24"/>
       <c r="AB55" s="7"/>
     </row>
-    <row r="56" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D56" s="7"/>
-      <c r="F56" s="7"/>
+    <row r="56" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" s="7">
+        <v>10</v>
+      </c>
+      <c r="D56" s="7">
+        <v>19</v>
+      </c>
+      <c r="E56" s="14">
+        <v>45528</v>
+      </c>
+      <c r="F56" s="16">
+        <f>(E56-$AC$1)/365*12</f>
+        <v>-5.2602739726027394</v>
+      </c>
       <c r="G56" s="33"/>
       <c r="K56" s="7"/>
       <c r="U56" s="24"/>
       <c r="AB56" s="7"/>
     </row>
-    <row r="57" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D57" s="7"/>
+    <row r="57" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="49">
+        <f>SUM(C56)*30+D56</f>
+        <v>319</v>
+      </c>
+      <c r="D57" s="50"/>
       <c r="F57" s="7"/>
       <c r="G57" s="33"/>
       <c r="K57" s="7"/>
@@ -4443,9 +4490,30 @@
       <c r="E193" s="10"/>
       <c r="F193" s="7"/>
     </row>
-    <row r="194" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A194" s="10"/>
+      <c r="B194" s="10"/>
+      <c r="C194" s="10"/>
+      <c r="D194" s="7"/>
+      <c r="E194" s="10"/>
+      <c r="F194" s="7"/>
+    </row>
+    <row r="195" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A195" s="10"/>
+      <c r="B195" s="10"/>
+      <c r="C195" s="10"/>
+      <c r="D195" s="7"/>
+      <c r="E195" s="10"/>
+      <c r="F195" s="7"/>
+    </row>
+    <row r="196" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="10"/>
+      <c r="B196" s="10"/>
+      <c r="C196" s="10"/>
+      <c r="D196" s="7"/>
+      <c r="E196" s="10"/>
+      <c r="F196" s="7"/>
+    </row>
     <row r="197" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="198" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="199" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4536,30 +4604,17 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="44">
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="V25:V26"/>
+    <mergeCell ref="X31:Y31"/>
+    <mergeCell ref="X27:Y27"/>
+    <mergeCell ref="X38:Y38"/>
+    <mergeCell ref="X35:Y35"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="X9:Y9"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="X17:Y17"/>
+    <mergeCell ref="X20:Y20"/>
     <mergeCell ref="Q41:R41"/>
     <mergeCell ref="Q6:R6"/>
     <mergeCell ref="Q11:R11"/>
@@ -4569,17 +4624,30 @@
     <mergeCell ref="Q19:R19"/>
     <mergeCell ref="Q32:R32"/>
     <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="X9:Y9"/>
-    <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="X17:Y17"/>
-    <mergeCell ref="X20:Y20"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="V25:V26"/>
-    <mergeCell ref="X31:Y31"/>
-    <mergeCell ref="X27:Y27"/>
-    <mergeCell ref="X38:Y38"/>
-    <mergeCell ref="X35:Y35"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="J39:K39"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4597,26 +4665,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e752113-b2fb-4b78-ae69-b10b93a6ace4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a2a82fc2-af7c-43c6-84e4-151c3b8f78f4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100209DA956FF56E441BE05848EA9FE5D9E" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="653cb4525f4b44831e30160e01e31f8e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4e752113-b2fb-4b78-ae69-b10b93a6ace4" xmlns:ns3="a2a82fc2-af7c-43c6-84e4-151c3b8f78f4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b41c74b500ee99c4b638ee97fa7cc63" ns2:_="" ns3:_="">
     <xsd:import namespace="4e752113-b2fb-4b78-ae69-b10b93a6ace4"/>
@@ -4857,26 +4905,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E564C7A4-BCA4-4794-8A6C-B04A14263787}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4e752113-b2fb-4b78-ae69-b10b93a6ace4"/>
-    <ds:schemaRef ds:uri="a2a82fc2-af7c-43c6-84e4-151c3b8f78f4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64C959BB-4F03-4A27-81AC-6DE1AA020D13}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e752113-b2fb-4b78-ae69-b10b93a6ace4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a2a82fc2-af7c-43c6-84e4-151c3b8f78f4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE15010B-5DC6-42B6-A17A-972FF152A8D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4893,4 +4942,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64C959BB-4F03-4A27-81AC-6DE1AA020D13}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E564C7A4-BCA4-4794-8A6C-B04A14263787}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4e752113-b2fb-4b78-ae69-b10b93a6ace4"/>
+    <ds:schemaRef ds:uri="a2a82fc2-af7c-43c6-84e4-151c3b8f78f4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update lot codes - 2025-02-04 09:53:32
</commit_message>
<xml_diff>
--- a/LotCode.xlsx
+++ b/LotCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf.sharepoint.com/sites/production-warehouse/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7269" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39A3E9BF-8CDA-4E2F-BE0E-03911E557E92}"/>
+  <xr:revisionPtr revIDLastSave="7270" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D08E1E43-FC3C-4293-8402-B553D3BAEEE4}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="a/VZ8kgdZMyU/a42HcB04O8OBNrnh4WxCIPRCv9GqcObOgYeM9oYcSfQqndR/nnirMykfzLaq88Ahwir6HajhQ==" workbookSaltValue="jsEDzk1n/+JkLoe+dWrmxg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="105">
   <si>
     <t>SKU</t>
   </si>
@@ -374,6 +374,9 @@
   </si>
   <si>
     <t>1.31.25</t>
+  </si>
+  <si>
+    <t>2.4.25</t>
   </si>
 </sst>
 </file>
@@ -738,19 +741,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1097,7 +1100,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC2" sqref="AC2"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,7 +1222,7 @@
     </row>
     <row r="2" spans="1:31" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="42" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G2" s="32"/>
       <c r="H2" s="23" t="s">
@@ -1260,7 +1263,7 @@
       <c r="H3" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="I3" s="53">
+      <c r="I3" s="49">
         <v>158587</v>
       </c>
       <c r="J3" s="7">
@@ -1402,11 +1405,11 @@
       <c r="I5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="49">
+      <c r="J5" s="50">
         <f>SUM(J3:J4)*40+K3</f>
         <v>4329</v>
       </c>
-      <c r="K5" s="50"/>
+      <c r="K5" s="51"/>
       <c r="N5" s="33"/>
       <c r="O5" s="27"/>
       <c r="P5" s="7" t="s">
@@ -1429,22 +1432,22 @@
       <c r="W5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X5" s="49">
+      <c r="X5" s="50">
         <f>SUM(X3:X4)*6+Y3+Y4</f>
         <v>1122</v>
       </c>
-      <c r="Y5" s="50"/>
+      <c r="Y5" s="51"/>
       <c r="AB5" s="7"/>
     </row>
     <row r="6" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="50">
         <f>SUM(C3:C5)*40+D3</f>
         <v>6468</v>
       </c>
-      <c r="D6" s="50"/>
+      <c r="D6" s="51"/>
       <c r="F6" s="7"/>
       <c r="G6" s="33"/>
       <c r="K6" s="7"/>
@@ -1452,11 +1455,11 @@
       <c r="P6" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q6" s="49">
+      <c r="Q6" s="50">
         <f>SUM(Q3:Q5)*30+R3+R5</f>
         <v>7809</v>
       </c>
-      <c r="R6" s="50"/>
+      <c r="R6" s="51"/>
       <c r="U6" s="33"/>
       <c r="V6" s="10" t="s">
         <v>10</v>
@@ -1606,11 +1609,11 @@
       <c r="I9" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="49">
+      <c r="J9" s="50">
         <f>SUM(J7:J8)*24+K7</f>
         <v>3634</v>
       </c>
-      <c r="K9" s="50"/>
+      <c r="K9" s="51"/>
       <c r="N9" s="33"/>
       <c r="P9" s="7" t="s">
         <v>49</v>
@@ -1630,11 +1633,11 @@
       <c r="W9" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X9" s="49">
+      <c r="X9" s="50">
         <f>SUM(X7:X8)*6+Y7+Y8</f>
         <v>412</v>
       </c>
-      <c r="Y9" s="50"/>
+      <c r="Y9" s="51"/>
       <c r="AB9" s="7"/>
     </row>
     <row r="10" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1711,11 +1714,11 @@
       <c r="P11" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q11" s="49">
+      <c r="Q11" s="50">
         <f>SUM(Q8:Q10)*30+R8</f>
         <v>6337</v>
       </c>
-      <c r="R11" s="50"/>
+      <c r="R11" s="51"/>
       <c r="U11" s="33"/>
       <c r="V11" s="6" t="s">
         <v>92</v>
@@ -1792,11 +1795,11 @@
       <c r="B13" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="49">
+      <c r="C13" s="50">
         <f>SUM(C8:C12)*24+D8</f>
         <v>5336</v>
       </c>
-      <c r="D13" s="50"/>
+      <c r="D13" s="51"/>
       <c r="F13" s="7"/>
       <c r="G13" s="33"/>
       <c r="H13" s="27"/>
@@ -1838,11 +1841,11 @@
       <c r="W13" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X13" s="49">
+      <c r="X13" s="50">
         <f>SUM(X11:X12)*6+Y11+Y12</f>
         <v>1240</v>
       </c>
-      <c r="Y13" s="50"/>
+      <c r="Y13" s="51"/>
       <c r="AB13" s="7"/>
     </row>
     <row r="14" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1907,20 +1910,20 @@
       <c r="I15" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J15" s="49">
+      <c r="J15" s="50">
         <f>SUM(J11:J14)*24+K11</f>
         <v>5520</v>
       </c>
-      <c r="K15" s="50"/>
+      <c r="K15" s="51"/>
       <c r="N15" s="33"/>
       <c r="P15" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q15" s="49">
+      <c r="Q15" s="50">
         <f>SUM(Q13:Q14)*30+R13+R14</f>
         <v>3879</v>
       </c>
-      <c r="R15" s="50"/>
+      <c r="R15" s="51"/>
       <c r="U15" s="33"/>
       <c r="V15" s="6" t="s">
         <v>72</v>
@@ -2040,11 +2043,11 @@
       <c r="W17" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X17" s="49">
+      <c r="X17" s="50">
         <f>SUM(X15:X16)*6+Y15+Y16</f>
         <v>517</v>
       </c>
-      <c r="Y17" s="50"/>
+      <c r="Y17" s="51"/>
       <c r="AB17" s="7"/>
     </row>
     <row r="18" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2102,11 +2105,11 @@
       <c r="B19" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="49">
+      <c r="C19" s="50">
         <f>SUM(C15:C18)*24+D16</f>
         <v>5154</v>
       </c>
-      <c r="D19" s="50"/>
+      <c r="D19" s="51"/>
       <c r="F19" s="7"/>
       <c r="G19" s="33"/>
       <c r="H19" s="6"/>
@@ -2128,11 +2131,11 @@
       <c r="P19" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q19" s="49">
+      <c r="Q19" s="50">
         <f>SUM(Q17:Q18)*30+R17+R18</f>
         <v>1385</v>
       </c>
-      <c r="R19" s="50"/>
+      <c r="R19" s="51"/>
       <c r="U19" s="33"/>
       <c r="V19" s="6" t="s">
         <v>20</v>
@@ -2163,11 +2166,11 @@
       <c r="I20" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J20" s="49">
+      <c r="J20" s="50">
         <f>SUM(J17:J19)*12+K17</f>
         <v>2455</v>
       </c>
-      <c r="K20" s="50"/>
+      <c r="K20" s="51"/>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
       <c r="N20" s="33"/>
@@ -2179,11 +2182,11 @@
       <c r="W20" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X20" s="49">
+      <c r="X20" s="50">
         <f>SUM(X19*200)+Y19</f>
         <v>1118</v>
       </c>
-      <c r="Y20" s="50"/>
+      <c r="Y20" s="51"/>
       <c r="AB20" s="7"/>
     </row>
     <row r="21" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
@@ -2339,41 +2342,41 @@
       <c r="P23" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q23" s="49">
+      <c r="Q23" s="50">
         <f>SUM(Q21:Q22)*30+R21</f>
         <v>1841</v>
       </c>
-      <c r="R23" s="50"/>
+      <c r="R23" s="51"/>
       <c r="U23" s="33"/>
       <c r="W23" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X23" s="49">
+      <c r="X23" s="50">
         <f>SUM(X22*200)+Y22</f>
         <v>780</v>
       </c>
-      <c r="Y23" s="50"/>
+      <c r="Y23" s="51"/>
       <c r="AB23" s="7"/>
     </row>
     <row r="24" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="49">
+      <c r="C24" s="50">
         <f>SUM(C21:C23)*12+D21</f>
         <v>2172</v>
       </c>
-      <c r="D24" s="50"/>
+      <c r="D24" s="51"/>
       <c r="F24" s="7"/>
       <c r="G24" s="33"/>
       <c r="I24" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J24" s="49">
+      <c r="J24" s="50">
         <f>SUM(J22:J23)*30+K22+K23</f>
         <v>2722</v>
       </c>
-      <c r="K24" s="50"/>
+      <c r="K24" s="51"/>
       <c r="N24" s="33"/>
       <c r="U24" s="33"/>
       <c r="AB24" s="7"/>
@@ -2548,41 +2551,41 @@
       <c r="W27" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X27" s="49">
+      <c r="X27" s="50">
         <f>SUM(X25:X26)*4+Y25+Y26</f>
         <v>174</v>
       </c>
-      <c r="Y27" s="50"/>
+      <c r="Y27" s="51"/>
       <c r="AB27" s="7"/>
     </row>
     <row r="28" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="49">
+      <c r="C28" s="50">
         <f>SUM(C26:C27)*40+D26+D27</f>
         <v>1458</v>
       </c>
-      <c r="D28" s="50"/>
+      <c r="D28" s="51"/>
       <c r="F28" s="7"/>
       <c r="G28" s="33"/>
       <c r="I28" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J28" s="49">
+      <c r="J28" s="50">
         <f>SUM(J26:J27)*30+K26</f>
         <v>2292</v>
       </c>
-      <c r="K28" s="50"/>
+      <c r="K28" s="51"/>
       <c r="N28" s="33"/>
       <c r="P28" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q28" s="49">
+      <c r="Q28" s="50">
         <f>SUM(Q25:Q27)*30+R25+R26+R27</f>
         <v>2418</v>
       </c>
-      <c r="R28" s="50"/>
+      <c r="R28" s="51"/>
       <c r="U28" s="33"/>
       <c r="AB28" s="7"/>
     </row>
@@ -2710,11 +2713,11 @@
       <c r="I31" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J31" s="49">
+      <c r="J31" s="50">
         <f>SUM(J30)*30+K30</f>
         <v>234</v>
       </c>
-      <c r="K31" s="50"/>
+      <c r="K31" s="51"/>
       <c r="N31" s="33"/>
       <c r="O31" s="6"/>
       <c r="P31" s="7" t="s">
@@ -2735,11 +2738,11 @@
       <c r="W31" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X31" s="49">
+      <c r="X31" s="50">
         <f>SUM(X29:X30)*30+Y29</f>
         <v>1270</v>
       </c>
-      <c r="Y31" s="50"/>
+      <c r="Y31" s="51"/>
       <c r="AB31" s="7"/>
     </row>
     <row r="32" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2763,11 +2766,11 @@
       <c r="P32" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q32" s="49">
+      <c r="Q32" s="50">
         <f>SUM(Q30:Q31)*30+R30</f>
         <v>609</v>
       </c>
-      <c r="R32" s="50"/>
+      <c r="R32" s="51"/>
       <c r="U32" s="33"/>
       <c r="AB32" s="7"/>
     </row>
@@ -2775,11 +2778,11 @@
       <c r="B33" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="49">
+      <c r="C33" s="50">
         <f>SUM(C30:C32)*24+D30</f>
         <v>3456</v>
       </c>
-      <c r="D33" s="50"/>
+      <c r="D33" s="51"/>
       <c r="F33" s="7"/>
       <c r="G33" s="33"/>
       <c r="H33" s="17" t="s">
@@ -2902,11 +2905,11 @@
       <c r="I35" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J35" s="49">
+      <c r="J35" s="50">
         <f>SUM(J33:J34)*24+K33</f>
         <v>1129</v>
       </c>
-      <c r="K35" s="50"/>
+      <c r="K35" s="51"/>
       <c r="N35" s="33"/>
       <c r="O35" s="6"/>
       <c r="P35" s="7" t="s">
@@ -2927,11 +2930,11 @@
       <c r="W35" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X35" s="49">
+      <c r="X35" s="50">
         <f>SUM(X33:X34)*18+Y33</f>
         <v>1175</v>
       </c>
-      <c r="Y35" s="50"/>
+      <c r="Y35" s="51"/>
       <c r="AB35" s="7"/>
     </row>
     <row r="36" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2956,11 +2959,11 @@
       <c r="P36" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q36" s="49">
+      <c r="Q36" s="50">
         <f>SUM(Q34:Q35)*30+R34</f>
         <v>828</v>
       </c>
-      <c r="R36" s="50"/>
+      <c r="R36" s="51"/>
       <c r="S36" s="7"/>
       <c r="T36" s="7"/>
       <c r="U36" s="33"/>
@@ -2970,11 +2973,11 @@
       <c r="B37" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="49">
+      <c r="C37" s="50">
         <f>SUM(C35:C36)*24+D35</f>
         <v>2238</v>
       </c>
-      <c r="D37" s="50"/>
+      <c r="D37" s="51"/>
       <c r="F37" s="7"/>
       <c r="G37" s="33"/>
       <c r="H37" s="6" t="s">
@@ -3064,11 +3067,11 @@
       <c r="W38" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X38" s="49">
+      <c r="X38" s="50">
         <f>SUM(X37:X37)*18+Y37</f>
         <v>2</v>
       </c>
-      <c r="Y38" s="50"/>
+      <c r="Y38" s="51"/>
       <c r="AB38" s="7"/>
     </row>
     <row r="39" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3095,11 +3098,11 @@
       <c r="I39" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J39" s="49">
+      <c r="J39" s="50">
         <f>SUM(J37:J38)*24+K37</f>
         <v>972</v>
       </c>
-      <c r="K39" s="50"/>
+      <c r="K39" s="51"/>
       <c r="N39" s="33"/>
       <c r="O39" s="24"/>
       <c r="P39" s="7" t="s">
@@ -3198,11 +3201,11 @@
       <c r="P41" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q41" s="49">
+      <c r="Q41" s="50">
         <f>SUM(Q38:Q40)*30+R38+R40</f>
         <v>3245</v>
       </c>
-      <c r="R41" s="50"/>
+      <c r="R41" s="51"/>
       <c r="U41" s="34"/>
       <c r="AB41" s="7"/>
     </row>
@@ -3210,11 +3213,11 @@
       <c r="B42" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="49">
+      <c r="C42" s="50">
         <f>SUM(C39:C41)*30+D39</f>
         <v>3276</v>
       </c>
-      <c r="D42" s="50"/>
+      <c r="D42" s="51"/>
       <c r="F42" s="7"/>
       <c r="G42" s="33"/>
       <c r="H42" s="27"/>
@@ -3244,11 +3247,11 @@
       <c r="I43" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J43" s="49">
+      <c r="J43" s="50">
         <f>SUM(J41:J42)*24+K41</f>
         <v>555</v>
       </c>
-      <c r="K43" s="50"/>
+      <c r="K43" s="51"/>
       <c r="N43" s="33"/>
       <c r="O43" s="6" t="s">
         <v>37</v>
@@ -3336,11 +3339,11 @@
       <c r="B46" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C46" s="49">
+      <c r="C46" s="50">
         <f>SUM(C44:C45)*30+D44</f>
         <v>1903</v>
       </c>
-      <c r="D46" s="50"/>
+      <c r="D46" s="51"/>
       <c r="F46" s="7"/>
       <c r="G46" s="33"/>
       <c r="I46" s="7">
@@ -3370,11 +3373,11 @@
       <c r="I47" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J47" s="49">
+      <c r="J47" s="50">
         <f>SUM(J45:J46)*24+K45</f>
         <v>1414</v>
       </c>
-      <c r="K47" s="50"/>
+      <c r="K47" s="51"/>
       <c r="N47" s="33"/>
       <c r="S47" s="4"/>
       <c r="U47" s="24"/>
@@ -3439,16 +3442,16 @@
       <c r="B50" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C50" s="49">
+      <c r="C50" s="50">
         <f>SUM(C48:C49)*30+D48</f>
         <v>1652</v>
       </c>
-      <c r="D50" s="50"/>
+      <c r="D50" s="51"/>
       <c r="F50" s="7"/>
       <c r="G50" s="33"/>
       <c r="I50" s="39"/>
-      <c r="J50" s="51"/>
-      <c r="K50" s="51"/>
+      <c r="J50" s="53"/>
+      <c r="K50" s="53"/>
       <c r="L50" s="24"/>
       <c r="M50" s="24"/>
       <c r="N50" s="24"/>
@@ -3519,11 +3522,11 @@
       <c r="B54" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C54" s="49" cm="1">
+      <c r="C54" s="50" cm="1">
         <f t="array" ref="C54">SUM(C52:C53*40)+D52+D53</f>
         <v>2427</v>
       </c>
-      <c r="D54" s="50"/>
+      <c r="D54" s="51"/>
       <c r="F54" s="7"/>
       <c r="G54" s="33"/>
       <c r="K54" s="7"/>
@@ -3570,11 +3573,11 @@
       <c r="B57" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="49">
+      <c r="C57" s="50">
         <f>SUM(C56)*30+D56</f>
         <v>319</v>
       </c>
-      <c r="D57" s="50"/>
+      <c r="D57" s="51"/>
       <c r="F57" s="7"/>
       <c r="G57" s="33"/>
       <c r="K57" s="7"/>
@@ -4604,35 +4607,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="44">
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="V25:V26"/>
-    <mergeCell ref="X31:Y31"/>
-    <mergeCell ref="X27:Y27"/>
-    <mergeCell ref="X38:Y38"/>
-    <mergeCell ref="X35:Y35"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="X9:Y9"/>
-    <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="X17:Y17"/>
-    <mergeCell ref="X20:Y20"/>
-    <mergeCell ref="Q41:R41"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="J20:K20"/>
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="C57:D57"/>
@@ -4648,6 +4622,35 @@
     <mergeCell ref="J31:K31"/>
     <mergeCell ref="J35:K35"/>
     <mergeCell ref="J39:K39"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="Q41:R41"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="X9:Y9"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="X17:Y17"/>
+    <mergeCell ref="X20:Y20"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="V25:V26"/>
+    <mergeCell ref="X31:Y31"/>
+    <mergeCell ref="X27:Y27"/>
+    <mergeCell ref="X38:Y38"/>
+    <mergeCell ref="X35:Y35"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4665,6 +4668,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100209DA956FF56E441BE05848EA9FE5D9E" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="653cb4525f4b44831e30160e01e31f8e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4e752113-b2fb-4b78-ae69-b10b93a6ace4" xmlns:ns3="a2a82fc2-af7c-43c6-84e4-151c3b8f78f4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b41c74b500ee99c4b638ee97fa7cc63" ns2:_="" ns3:_="">
     <xsd:import namespace="4e752113-b2fb-4b78-ae69-b10b93a6ace4"/>
@@ -4905,15 +4917,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4926,6 +4929,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64C959BB-4F03-4A27-81AC-6DE1AA020D13}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE15010B-5DC6-42B6-A17A-972FF152A8D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4944,14 +4955,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64C959BB-4F03-4A27-81AC-6DE1AA020D13}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E564C7A4-BCA4-4794-8A6C-B04A14263787}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Update lot codes - 2025-02-04 10:36:42
</commit_message>
<xml_diff>
--- a/LotCode.xlsx
+++ b/LotCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf.sharepoint.com/sites/production-warehouse/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7270" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D08E1E43-FC3C-4293-8402-B553D3BAEEE4}"/>
+  <xr:revisionPtr revIDLastSave="7324" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5209830-0D9B-4503-A669-AA77CDEFA79E}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="a/VZ8kgdZMyU/a42HcB04O8OBNrnh4WxCIPRCv9GqcObOgYeM9oYcSfQqndR/nnirMykfzLaq88Ahwir6HajhQ==" workbookSaltValue="jsEDzk1n/+JkLoe+dWrmxg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="106">
   <si>
     <t>SKU</t>
   </si>
@@ -190,9 +190,6 @@
     <t>600-SR-HO</t>
   </si>
   <si>
-    <t>0824FS608</t>
-  </si>
-  <si>
     <t>0824FS311-1</t>
   </si>
   <si>
@@ -316,9 +313,6 @@
     <t>1024CC07</t>
   </si>
   <si>
-    <t>0624FR1808</t>
-  </si>
-  <si>
     <t>PRC24912</t>
   </si>
   <si>
@@ -377,6 +371,15 @@
   </si>
   <si>
     <t>2.4.25</t>
+  </si>
+  <si>
+    <t>4 on blue rack</t>
+  </si>
+  <si>
+    <t>165893</t>
+  </si>
+  <si>
+    <t>163030</t>
   </si>
 </sst>
 </file>
@@ -619,7 +622,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -755,6 +758,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1099,8 +1105,8 @@
   <dimension ref="A1:AE283"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,32 +1228,32 @@
     </row>
     <row r="2" spans="1:31" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="42" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G2" s="32"/>
       <c r="H2" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="N2" s="32"/>
       <c r="O2" s="23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="U2" s="32"/>
       <c r="V2" s="42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AB2" s="8"/>
       <c r="AE2" s="18"/>
     </row>
     <row r="3" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="40">
         <v>159368</v>
       </c>
       <c r="C3" s="7">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D3" s="7">
         <v>28</v>
@@ -1261,7 +1267,7 @@
       </c>
       <c r="G3" s="33"/>
       <c r="H3" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I3" s="49">
         <v>158587</v>
@@ -1301,10 +1307,10 @@
       </c>
       <c r="U3" s="33"/>
       <c r="V3" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W3" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X3" s="7">
         <v>9</v>
@@ -1322,6 +1328,9 @@
       <c r="AB3" s="12"/>
     </row>
     <row r="4" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="54" t="s">
+        <v>103</v>
+      </c>
       <c r="B4" s="40">
         <v>163236</v>
       </c>
@@ -1369,7 +1378,7 @@
       </c>
       <c r="U4" s="33"/>
       <c r="W4" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X4" s="15">
         <v>177</v>
@@ -1395,11 +1404,11 @@
       </c>
       <c r="D5" s="40"/>
       <c r="E5" s="41">
-        <v>46323</v>
+        <v>46351</v>
       </c>
       <c r="F5" s="9">
         <f t="shared" si="0"/>
-        <v>20.876712328767123</v>
+        <v>21.797260273972604</v>
       </c>
       <c r="G5" s="33"/>
       <c r="I5" s="46" t="s">
@@ -1413,7 +1422,7 @@
       <c r="N5" s="33"/>
       <c r="O5" s="27"/>
       <c r="P5" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Q5" s="7">
         <v>195</v>
@@ -1445,7 +1454,7 @@
       </c>
       <c r="C6" s="50">
         <f>SUM(C3:C5)*40+D3</f>
-        <v>6468</v>
+        <v>6188</v>
       </c>
       <c r="D6" s="51"/>
       <c r="F6" s="7"/>
@@ -1473,7 +1482,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="33"/>
       <c r="H7" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I7" s="7">
         <v>163237</v>
@@ -1494,7 +1503,7 @@
       <c r="N7" s="33"/>
       <c r="U7" s="33"/>
       <c r="V7" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="W7" s="7" t="s">
         <v>12</v>
@@ -1516,23 +1525,23 @@
     </row>
     <row r="8" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="7">
-        <v>158583</v>
+        <v>159367</v>
       </c>
       <c r="C8" s="7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D8" s="7">
         <v>8</v>
       </c>
       <c r="E8" s="8">
-        <v>46250</v>
+        <v>46283</v>
       </c>
       <c r="F8" s="9">
         <f t="shared" ref="F8" si="7">(E8-$AC$1)/365*12</f>
-        <v>18.476712328767121</v>
+        <v>19.56164383561644</v>
       </c>
       <c r="G8" s="33"/>
       <c r="H8" s="27"/>
@@ -1555,7 +1564,7 @@
         <v>11</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q8" s="7">
         <v>9</v>
@@ -1572,7 +1581,7 @@
       </c>
       <c r="U8" s="33"/>
       <c r="W8" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="X8" s="7">
         <v>54</v>
@@ -1592,18 +1601,18 @@
     <row r="9" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="27"/>
       <c r="B9" s="7">
-        <v>159367</v>
+        <v>161798</v>
       </c>
       <c r="C9" s="11">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="8">
-        <v>46283</v>
+        <v>46324</v>
       </c>
       <c r="F9" s="9">
-        <f>(E9-$AC$1)/365*12</f>
-        <v>19.56164383561644</v>
+        <f t="shared" ref="F9:F10" si="10">(E9-$AC$1)/365*12</f>
+        <v>20.909589041095892</v>
       </c>
       <c r="G9" s="33"/>
       <c r="I9" s="46" t="s">
@@ -1616,7 +1625,7 @@
       <c r="K9" s="51"/>
       <c r="N9" s="33"/>
       <c r="P9" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q9" s="7">
         <v>29</v>
@@ -1643,24 +1652,24 @@
     <row r="10" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="27"/>
       <c r="B10" s="7">
-        <v>161794</v>
+        <v>162036</v>
       </c>
       <c r="C10" s="11">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="8">
-        <v>46324</v>
+        <v>46337</v>
       </c>
       <c r="F10" s="9">
-        <f>(E10-$AC$1)/365*12</f>
-        <v>20.909589041095892</v>
+        <f t="shared" si="10"/>
+        <v>21.336986301369862</v>
       </c>
       <c r="G10" s="33"/>
       <c r="K10" s="7"/>
       <c r="N10" s="33"/>
       <c r="P10" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="Q10" s="7">
         <v>173</v>
@@ -1677,24 +1686,18 @@
       <c r="AB10" s="7"/>
     </row>
     <row r="11" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="27"/>
-      <c r="B11" s="7">
-        <v>161798</v>
-      </c>
-      <c r="C11" s="11">
-        <v>60</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8">
-        <v>46324</v>
-      </c>
-      <c r="F11" s="9">
-        <f t="shared" ref="F11:F12" si="10">(E11-$AC$1)/365*12</f>
-        <v>20.909589041095892</v>
-      </c>
+      <c r="B11" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="50">
+        <f>SUM(C8:C10)*24+D8</f>
+        <v>2168</v>
+      </c>
+      <c r="D11" s="51"/>
+      <c r="F11" s="7"/>
       <c r="G11" s="33"/>
       <c r="H11" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I11" s="7">
         <v>159369</v>
@@ -1721,7 +1724,7 @@
       <c r="R11" s="51"/>
       <c r="U11" s="33"/>
       <c r="V11" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="W11" s="7" t="s">
         <v>14</v>
@@ -1742,21 +1745,8 @@
       <c r="AB11" s="7"/>
     </row>
     <row r="12" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="27"/>
-      <c r="B12" s="7">
-        <v>162036</v>
-      </c>
-      <c r="C12" s="11">
-        <v>22</v>
-      </c>
       <c r="D12" s="7"/>
-      <c r="E12" s="8">
-        <v>46337</v>
-      </c>
-      <c r="F12" s="9">
-        <f t="shared" si="10"/>
-        <v>21.336986301369862</v>
-      </c>
+      <c r="F12" s="7"/>
       <c r="G12" s="33"/>
       <c r="H12" s="27"/>
       <c r="I12" s="7">
@@ -1776,7 +1766,7 @@
       <c r="N12" s="33"/>
       <c r="U12" s="33"/>
       <c r="W12" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="X12" s="7">
         <v>202</v>
@@ -1792,15 +1782,23 @@
       <c r="AB12" s="7"/>
     </row>
     <row r="13" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="50">
-        <f>SUM(C8:C12)*24+D8</f>
-        <v>5336</v>
-      </c>
-      <c r="D13" s="51"/>
-      <c r="F13" s="7"/>
+      <c r="A13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="35">
+        <v>159366</v>
+      </c>
+      <c r="C13" s="7">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8">
+        <v>46283</v>
+      </c>
+      <c r="F13" s="9">
+        <f>(E13-$AC$1)/365*12</f>
+        <v>19.56164383561644</v>
+      </c>
       <c r="G13" s="33"/>
       <c r="H13" s="27"/>
       <c r="I13" s="7">
@@ -1849,8 +1847,20 @@
       <c r="AB13" s="7"/>
     </row>
     <row r="14" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="35">
+        <v>161793</v>
+      </c>
+      <c r="C14" s="11">
+        <v>74</v>
+      </c>
       <c r="D14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="E14" s="8">
+        <v>46313</v>
+      </c>
+      <c r="F14" s="9">
+        <f t="shared" ref="F14" si="13">(E14-$AC$1)/365*12</f>
+        <v>20.547945205479451</v>
+      </c>
       <c r="G14" s="33"/>
       <c r="H14" s="27"/>
       <c r="I14" s="7">
@@ -1870,7 +1880,7 @@
       <c r="N14" s="33"/>
       <c r="O14" s="27"/>
       <c r="P14" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q14" s="7">
         <v>120</v>
@@ -1889,22 +1899,19 @@
       <c r="AB14" s="7"/>
     </row>
     <row r="15" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="B15" s="35">
-        <v>159366</v>
-      </c>
-      <c r="C15" s="7">
-        <v>4</v>
+        <v>161794</v>
+      </c>
+      <c r="C15" s="11">
+        <v>174</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="8">
-        <v>46283</v>
+        <v>46324</v>
       </c>
       <c r="F15" s="9">
-        <f>(E15-$AC$1)/365*12</f>
-        <v>19.56164383561644</v>
+        <f t="shared" ref="F15" si="14">(E15-$AC$1)/365*12</f>
+        <v>20.909589041095892</v>
       </c>
       <c r="G15" s="33"/>
       <c r="I15" s="46" t="s">
@@ -1926,10 +1933,10 @@
       <c r="R15" s="51"/>
       <c r="U15" s="33"/>
       <c r="V15" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="W15" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="X15" s="7">
         <v>12</v>
@@ -1941,33 +1948,28 @@
         <v>47024</v>
       </c>
       <c r="AA15" s="9">
-        <f t="shared" ref="AA15:AA16" si="13">(Z15-$AC$1)/365*12</f>
+        <f t="shared" ref="AA15:AA16" si="15">(Z15-$AC$1)/365*12</f>
         <v>43.923287671232877</v>
       </c>
       <c r="AB15" s="7"/>
     </row>
     <row r="16" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="35">
-        <v>158221</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="7">
-        <v>18</v>
-      </c>
-      <c r="E16" s="8">
-        <v>46249</v>
-      </c>
-      <c r="F16" s="9">
-        <f>(E16-$AC$1)/365*12</f>
-        <v>18.443835616438356</v>
-      </c>
+      <c r="B16" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="50">
+        <f>SUM(C13:C15)*24+D13</f>
+        <v>5976</v>
+      </c>
+      <c r="D16" s="51"/>
+      <c r="F16" s="7"/>
       <c r="G16" s="33"/>
       <c r="K16" s="7"/>
       <c r="N16" s="33"/>
       <c r="U16" s="33"/>
       <c r="V16" s="6"/>
       <c r="W16" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="X16" s="7">
         <v>73</v>
@@ -1979,29 +1981,18 @@
         <v>47085</v>
       </c>
       <c r="AA16" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>45.92876712328767</v>
       </c>
       <c r="AB16" s="8"/>
     </row>
     <row r="17" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="35">
-        <v>161793</v>
-      </c>
-      <c r="C17" s="11">
-        <v>141</v>
-      </c>
+      <c r="B17" s="43"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="8">
-        <v>46313</v>
-      </c>
-      <c r="F17" s="9">
-        <f t="shared" ref="F17" si="14">(E17-$AC$1)/365*12</f>
-        <v>20.547945205479451</v>
-      </c>
+      <c r="F17" s="7"/>
       <c r="G17" s="33"/>
       <c r="H17" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I17" s="7">
         <v>163238</v>
@@ -2016,7 +2007,7 @@
         <v>46310</v>
       </c>
       <c r="M17" s="9">
-        <f t="shared" ref="M17:M19" si="15">(L17-$AC$1)/365*12</f>
+        <f t="shared" ref="M17:M19" si="16">(L17-$AC$1)/365*12</f>
         <v>20.449315068493153</v>
       </c>
       <c r="N17" s="33"/>
@@ -2024,7 +2015,7 @@
         <v>16</v>
       </c>
       <c r="P17" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q17" s="7">
         <v>9</v>
@@ -2036,7 +2027,7 @@
         <v>46199</v>
       </c>
       <c r="T17" s="9">
-        <f t="shared" ref="T17" si="16">(S17-$AC$1)/365*12</f>
+        <f t="shared" ref="T17" si="17">(S17-$AC$1)/365*12</f>
         <v>16.799999999999997</v>
       </c>
       <c r="U17" s="33"/>
@@ -2051,19 +2042,24 @@
       <c r="AB17" s="7"/>
     </row>
     <row r="18" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="35">
-        <v>161794</v>
+      <c r="A18" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="44" t="s">
+        <v>91</v>
       </c>
       <c r="C18" s="11">
-        <v>69</v>
-      </c>
-      <c r="D18" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="D18" s="7">
+        <v>0</v>
+      </c>
       <c r="E18" s="8">
-        <v>46324</v>
+        <v>46283</v>
       </c>
       <c r="F18" s="9">
-        <f t="shared" ref="F18" si="17">(E18-$AC$1)/365*12</f>
-        <v>20.909589041095892</v>
+        <f t="shared" ref="F18" si="18">(E18-$AC$1)/365*12</f>
+        <v>19.56164383561644</v>
       </c>
       <c r="G18" s="33"/>
       <c r="H18" s="6"/>
@@ -2078,12 +2074,12 @@
         <v>46325</v>
       </c>
       <c r="M18" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>20.942465753424656</v>
       </c>
       <c r="N18" s="33"/>
       <c r="P18" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q18" s="7">
         <v>36</v>
@@ -2095,22 +2091,27 @@
         <v>46321</v>
       </c>
       <c r="T18" s="9">
-        <f t="shared" ref="T18" si="18">(S18-$AC$1)/365*12</f>
+        <f t="shared" ref="T18" si="19">(S18-$AC$1)/365*12</f>
         <v>20.81095890410959</v>
       </c>
       <c r="U18" s="33"/>
       <c r="AB18" s="7"/>
     </row>
     <row r="19" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="50">
-        <f>SUM(C15:C18)*24+D16</f>
-        <v>5154</v>
-      </c>
-      <c r="D19" s="51"/>
-      <c r="F19" s="7"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="7">
+        <v>54</v>
+      </c>
+      <c r="E19" s="8">
+        <v>46283</v>
+      </c>
+      <c r="F19" s="9">
+        <f t="shared" ref="F19:F20" si="20">(E19-$AC$1)/365*12</f>
+        <v>19.56164383561644</v>
+      </c>
       <c r="G19" s="33"/>
       <c r="H19" s="6"/>
       <c r="I19" s="7">
@@ -2124,7 +2125,7 @@
         <v>46361</v>
       </c>
       <c r="M19" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>22.126027397260273</v>
       </c>
       <c r="N19" s="33"/>
@@ -2159,9 +2160,20 @@
       <c r="AB19" s="7"/>
     </row>
     <row r="20" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="43"/>
-      <c r="D20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="7">
+        <v>101</v>
+      </c>
+      <c r="E20" s="8">
+        <v>46303</v>
+      </c>
+      <c r="F20" s="9">
+        <f t="shared" si="20"/>
+        <v>20.219178082191782</v>
+      </c>
       <c r="G20" s="33"/>
       <c r="I20" s="46" t="s">
         <v>8</v>
@@ -2189,26 +2201,16 @@
       <c r="Y20" s="51"/>
       <c r="AB20" s="7"/>
     </row>
-    <row r="21" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="C21" s="11">
-        <v>6</v>
-      </c>
-      <c r="D21" s="7">
-        <v>0</v>
-      </c>
-      <c r="E21" s="8">
-        <v>46283</v>
-      </c>
-      <c r="F21" s="9">
-        <f t="shared" ref="F21" si="19">(E21-$AC$1)/365*12</f>
-        <v>19.56164383561644</v>
-      </c>
+    <row r="21" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="50">
+        <f>SUM(C18:C20)*12+D18</f>
+        <v>1920</v>
+      </c>
+      <c r="D21" s="51"/>
+      <c r="F21" s="7"/>
       <c r="G21" s="33"/>
       <c r="K21" s="7"/>
       <c r="N21" s="33"/>
@@ -2216,7 +2218,7 @@
         <v>19</v>
       </c>
       <c r="P21" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q21" s="7">
         <v>9</v>
@@ -2228,27 +2230,16 @@
         <v>46291</v>
       </c>
       <c r="T21" s="9">
-        <f t="shared" ref="T21:T22" si="20">(S21-$AC$1)/365*12</f>
+        <f t="shared" ref="T21:T22" si="21">(S21-$AC$1)/365*12</f>
         <v>19.824657534246576</v>
       </c>
       <c r="U21" s="33"/>
       <c r="AB21" s="7"/>
     </row>
     <row r="22" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="27"/>
-      <c r="B22" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="C22" s="7">
-        <v>74</v>
-      </c>
-      <c r="E22" s="8">
-        <v>46283</v>
-      </c>
-      <c r="F22" s="9">
-        <f t="shared" ref="F22:F23" si="21">(E22-$AC$1)/365*12</f>
-        <v>19.56164383561644</v>
-      </c>
+      <c r="B22" s="43"/>
+      <c r="D22" s="7"/>
+      <c r="F22" s="7"/>
       <c r="G22" s="33"/>
       <c r="H22" s="6" t="s">
         <v>18</v>
@@ -2271,7 +2262,7 @@
       </c>
       <c r="N22" s="33"/>
       <c r="P22" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q22" s="7">
         <v>52</v>
@@ -2281,12 +2272,12 @@
         <v>46291</v>
       </c>
       <c r="T22" s="9">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>19.824657534246576</v>
       </c>
       <c r="U22" s="33"/>
       <c r="V22" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W22" s="7" t="s">
         <v>27</v>
@@ -2307,23 +2298,26 @@
       <c r="AB22" s="7"/>
     </row>
     <row r="23" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="27"/>
-      <c r="B23" s="44" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" s="7">
-        <v>101</v>
-      </c>
+      <c r="A23" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="11">
+        <v>6</v>
+      </c>
+      <c r="D23" s="7"/>
       <c r="E23" s="8">
-        <v>46303</v>
+        <v>46211</v>
       </c>
       <c r="F23" s="9">
-        <f t="shared" si="21"/>
-        <v>20.219178082191782</v>
+        <f>(E23-$AC$1)/365*12</f>
+        <v>17.194520547945206</v>
       </c>
       <c r="G23" s="33"/>
       <c r="I23" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J23" s="7">
         <v>86</v>
@@ -2359,15 +2353,18 @@
       <c r="AB23" s="7"/>
     </row>
     <row r="24" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="50">
-        <f>SUM(C21:C23)*12+D21</f>
-        <v>2172</v>
-      </c>
-      <c r="D24" s="51"/>
-      <c r="F24" s="7"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="11">
+        <v>119</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8">
+        <v>46211</v>
+      </c>
+      <c r="F24" s="9"/>
       <c r="G24" s="33"/>
       <c r="I24" s="46" t="s">
         <v>8</v>
@@ -2381,10 +2378,22 @@
       <c r="U24" s="33"/>
       <c r="AB24" s="7"/>
     </row>
-    <row r="25" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="43"/>
+    <row r="25" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="29"/>
+      <c r="B25" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="11">
+        <v>36</v>
+      </c>
       <c r="D25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="E25" s="8">
+        <v>46302</v>
+      </c>
+      <c r="F25" s="9">
+        <f>(E25-$AC$1)/365*12</f>
+        <v>20.186301369863013</v>
+      </c>
       <c r="G25" s="33"/>
       <c r="K25" s="7"/>
       <c r="M25" s="10" t="s">
@@ -2412,10 +2421,10 @@
       </c>
       <c r="U25" s="33"/>
       <c r="V25" s="52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="W25" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="X25" s="7">
         <v>43</v>
@@ -2433,25 +2442,15 @@
       <c r="AB25" s="7"/>
     </row>
     <row r="26" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="45">
-        <v>158238</v>
-      </c>
-      <c r="C26" s="7">
-        <v>0</v>
-      </c>
-      <c r="D26" s="7">
-        <v>18</v>
-      </c>
-      <c r="E26" s="8">
-        <v>46190</v>
-      </c>
-      <c r="F26" s="9">
-        <f>(E26-$AC$1)/365*12</f>
-        <v>16.504109589041093</v>
-      </c>
+      <c r="B26" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="50">
+        <f>SUM(C23:C25)*40+D23+D25</f>
+        <v>6440</v>
+      </c>
+      <c r="D26" s="51"/>
+      <c r="F26" s="7"/>
       <c r="G26" s="33"/>
       <c r="H26" s="6" t="s">
         <v>23</v>
@@ -2499,24 +2498,12 @@
       <c r="AB26" s="7"/>
     </row>
     <row r="27" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="29"/>
-      <c r="B27" s="45">
-        <v>163030</v>
-      </c>
-      <c r="C27" s="11">
-        <v>36</v>
-      </c>
+      <c r="B27" s="43"/>
       <c r="D27" s="7"/>
-      <c r="E27" s="8">
-        <v>46302</v>
-      </c>
-      <c r="F27" s="9">
-        <f>(E27-$AC$1)/365*12</f>
-        <v>20.186301369863013</v>
-      </c>
+      <c r="F27" s="7"/>
       <c r="G27" s="33"/>
       <c r="I27" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J27" s="7">
         <v>74</v>
@@ -2531,7 +2518,7 @@
       </c>
       <c r="N27" s="33"/>
       <c r="P27" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q27" s="7">
         <v>50</v>
@@ -2559,15 +2546,25 @@
       <c r="AB27" s="7"/>
     </row>
     <row r="28" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="47" t="s">
+      <c r="A28" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="7">
         <v>8</v>
       </c>
-      <c r="C28" s="50">
-        <f>SUM(C26:C27)*40+D26+D27</f>
-        <v>1458</v>
-      </c>
-      <c r="D28" s="51"/>
-      <c r="F28" s="7"/>
+      <c r="D28" s="7">
+        <v>0</v>
+      </c>
+      <c r="E28" s="8">
+        <v>46211</v>
+      </c>
+      <c r="F28" s="9">
+        <f>(E28-$AC$1)/365*12</f>
+        <v>17.194520547945206</v>
+      </c>
       <c r="G28" s="33"/>
       <c r="I28" s="46" t="s">
         <v>8</v>
@@ -2590,9 +2587,20 @@
       <c r="AB28" s="7"/>
     </row>
     <row r="29" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="43"/>
+      <c r="B29" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="7">
+        <v>55</v>
+      </c>
       <c r="D29" s="7"/>
-      <c r="F29" s="7"/>
+      <c r="E29" s="8">
+        <v>46211</v>
+      </c>
+      <c r="F29" s="9">
+        <f>(E29-$AC$1)/365*12</f>
+        <v>17.194520547945206</v>
+      </c>
       <c r="G29" s="33"/>
       <c r="K29" s="7"/>
       <c r="N29" s="33"/>
@@ -2601,7 +2609,7 @@
         <v>33</v>
       </c>
       <c r="W29" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="X29" s="7">
         <v>10</v>
@@ -2619,24 +2627,19 @@
       <c r="AB29" s="8"/>
     </row>
     <row r="30" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="44">
-        <v>158234</v>
+      <c r="B30" s="44" t="s">
+        <v>100</v>
       </c>
       <c r="C30" s="7">
-        <v>3</v>
-      </c>
-      <c r="D30" s="7">
-        <v>0</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D30" s="7"/>
       <c r="E30" s="8">
-        <v>46191</v>
+        <v>46248</v>
       </c>
       <c r="F30" s="9">
         <f>(E30-$AC$1)/365*12</f>
-        <v>16.536986301369865</v>
+        <v>18.410958904109588</v>
       </c>
       <c r="G30" s="33"/>
       <c r="H30" s="6" t="s">
@@ -2663,7 +2666,7 @@
         <v>28</v>
       </c>
       <c r="P30" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q30" s="7">
         <v>9</v>
@@ -2680,7 +2683,7 @@
       </c>
       <c r="U30" s="33"/>
       <c r="W30" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="X30" s="7">
         <v>32</v>
@@ -2695,20 +2698,15 @@
       </c>
     </row>
     <row r="31" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="7">
-        <v>61</v>
-      </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="8">
-        <v>46211</v>
-      </c>
-      <c r="F31" s="9">
-        <f>(E31-$AC$1)/365*12</f>
-        <v>17.194520547945206</v>
-      </c>
+      <c r="B31" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="50">
+        <f>SUM(C28:C30)*24+D28</f>
+        <v>3432</v>
+      </c>
+      <c r="D31" s="51"/>
+      <c r="F31" s="7"/>
       <c r="G31" s="33"/>
       <c r="I31" s="46" t="s">
         <v>8</v>
@@ -2721,7 +2719,7 @@
       <c r="N31" s="33"/>
       <c r="O31" s="6"/>
       <c r="P31" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q31" s="7">
         <v>11</v>
@@ -2746,20 +2744,9 @@
       <c r="AB31" s="7"/>
     </row>
     <row r="32" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="44" t="s">
-        <v>102</v>
-      </c>
-      <c r="C32" s="7">
-        <v>80</v>
-      </c>
+      <c r="B32" s="43"/>
       <c r="D32" s="7"/>
-      <c r="E32" s="8">
-        <v>46248</v>
-      </c>
-      <c r="F32" s="9">
-        <f>(E32-$AC$1)/365*12</f>
-        <v>18.410958904109588</v>
-      </c>
+      <c r="F32" s="7"/>
       <c r="G32" s="33"/>
       <c r="K32" s="7"/>
       <c r="N32" s="33"/>
@@ -2774,19 +2761,29 @@
       <c r="U32" s="33"/>
       <c r="AB32" s="7"/>
     </row>
-    <row r="33" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="47" t="s">
+    <row r="33" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="7">
         <v>8</v>
       </c>
-      <c r="C33" s="50">
-        <f>SUM(C30:C32)*24+D30</f>
-        <v>3456</v>
-      </c>
-      <c r="D33" s="51"/>
-      <c r="F33" s="7"/>
+      <c r="D33" s="7">
+        <v>6</v>
+      </c>
+      <c r="E33" s="8">
+        <v>46312</v>
+      </c>
+      <c r="F33" s="9">
+        <f>(E33-$AC$1)/365*12</f>
+        <v>20.515068493150686</v>
+      </c>
       <c r="G33" s="33"/>
       <c r="H33" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I33" s="7">
         <v>162839</v>
@@ -2810,7 +2807,7 @@
         <v>36</v>
       </c>
       <c r="W33" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="X33" s="11">
         <v>0</v>
@@ -2828,9 +2825,21 @@
       <c r="AB33" s="7"/>
     </row>
     <row r="34" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="43"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="7">
+        <v>79</v>
+      </c>
       <c r="D34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="E34" s="8">
+        <v>46312</v>
+      </c>
+      <c r="F34" s="9">
+        <f>(E34-$AC$1)/365*12</f>
+        <v>20.515068493150686</v>
+      </c>
       <c r="G34" s="33"/>
       <c r="I34" s="7">
         <v>162839</v>
@@ -2869,7 +2878,7 @@
       <c r="U34" s="33"/>
       <c r="V34" s="6"/>
       <c r="W34" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="X34" s="11">
         <v>65</v>
@@ -2882,25 +2891,15 @@
       <c r="AB34" s="7"/>
     </row>
     <row r="35" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B35" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="C35" s="7">
-        <v>4</v>
-      </c>
-      <c r="D35" s="7">
-        <v>6</v>
-      </c>
-      <c r="E35" s="8">
-        <v>46211</v>
-      </c>
-      <c r="F35" s="9">
-        <f>(E35-$AC$1)/365*12</f>
-        <v>17.194520547945206</v>
-      </c>
+      <c r="B35" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="50">
+        <f>SUM(C33:C34)*24+D33</f>
+        <v>2094</v>
+      </c>
+      <c r="D35" s="51"/>
+      <c r="F35" s="7"/>
       <c r="G35" s="33"/>
       <c r="I35" s="46" t="s">
         <v>8</v>
@@ -2938,21 +2937,9 @@
       <c r="AB35" s="7"/>
     </row>
     <row r="36" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="27"/>
-      <c r="B36" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="C36" s="7">
-        <v>89</v>
-      </c>
+      <c r="B36" s="43"/>
       <c r="D36" s="7"/>
-      <c r="E36" s="8">
-        <v>46312</v>
-      </c>
-      <c r="F36" s="9">
-        <f>(E36-$AC$1)/365*12</f>
-        <v>20.515068493150686</v>
-      </c>
+      <c r="F36" s="7"/>
       <c r="G36" s="33"/>
       <c r="K36" s="7"/>
       <c r="N36" s="33"/>
@@ -2970,18 +2957,28 @@
       <c r="AB36" s="7"/>
     </row>
     <row r="37" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="50">
-        <f>SUM(C35:C36)*24+D35</f>
-        <v>2238</v>
-      </c>
-      <c r="D37" s="51"/>
-      <c r="F37" s="7"/>
+      <c r="A37" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="11">
+        <v>7</v>
+      </c>
+      <c r="D37" s="7">
+        <v>6</v>
+      </c>
+      <c r="E37" s="14">
+        <v>46260</v>
+      </c>
+      <c r="F37" s="9">
+        <f>(E37-$AC$1)/365*12</f>
+        <v>18.805479452054794</v>
+      </c>
       <c r="G37" s="33"/>
       <c r="H37" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I37" s="7">
         <v>161789</v>
@@ -3006,7 +3003,7 @@
       <c r="T37" s="7"/>
       <c r="U37" s="33"/>
       <c r="V37" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="W37" s="7" t="s">
         <v>38</v>
@@ -3025,9 +3022,20 @@
       <c r="AB37" s="7"/>
     </row>
     <row r="38" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="43"/>
+      <c r="B38" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="40">
+        <v>81</v>
+      </c>
       <c r="D38" s="7"/>
-      <c r="F38" s="7"/>
+      <c r="E38" s="14">
+        <v>46352</v>
+      </c>
+      <c r="F38" s="9">
+        <f>(E38-$AC$1)/365*12</f>
+        <v>21.830136986301369</v>
+      </c>
       <c r="G38" s="33"/>
       <c r="I38" s="7">
         <v>161789</v>
@@ -3075,25 +3083,15 @@
       <c r="AB38" s="7"/>
     </row>
     <row r="39" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="11">
-        <v>1</v>
-      </c>
-      <c r="D39" s="7">
-        <v>6</v>
-      </c>
-      <c r="E39" s="14">
-        <v>46260</v>
-      </c>
-      <c r="F39" s="9">
-        <f>(E39-$AC$1)/365*12</f>
-        <v>18.805479452054794</v>
-      </c>
+      <c r="B39" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="50">
+        <f>SUM(C37:C38)*30+D37</f>
+        <v>2646</v>
+      </c>
+      <c r="D39" s="51"/>
+      <c r="F39" s="7"/>
       <c r="G39" s="33"/>
       <c r="I39" s="46" t="s">
         <v>8</v>
@@ -3123,20 +3121,9 @@
       <c r="AB39" s="7"/>
     </row>
     <row r="40" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" s="40">
-        <v>23</v>
-      </c>
+      <c r="B40" s="43"/>
       <c r="D40" s="7"/>
-      <c r="E40" s="14">
-        <v>46291</v>
-      </c>
-      <c r="F40" s="9">
-        <f>(E40-$AC$1)/365*12</f>
-        <v>19.824657534246576</v>
-      </c>
+      <c r="F40" s="7"/>
       <c r="G40" s="33"/>
       <c r="I40" s="13"/>
       <c r="J40" s="30"/>
@@ -3144,7 +3131,7 @@
       <c r="N40" s="33"/>
       <c r="O40" s="24"/>
       <c r="P40" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q40" s="7">
         <v>69</v>
@@ -3163,23 +3150,28 @@
       <c r="AB40" s="7"/>
     </row>
     <row r="41" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="B41" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="C41" s="40">
-        <v>85</v>
-      </c>
-      <c r="D41" s="7"/>
+        <v>46</v>
+      </c>
+      <c r="C41" s="7">
+        <v>5</v>
+      </c>
+      <c r="D41" s="7">
+        <v>9</v>
+      </c>
       <c r="E41" s="14">
-        <v>46352</v>
+        <v>46291</v>
       </c>
       <c r="F41" s="9">
         <f>(E41-$AC$1)/365*12</f>
-        <v>21.830136986301369</v>
+        <v>19.824657534246576</v>
       </c>
       <c r="G41" s="33"/>
       <c r="H41" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I41" s="7">
         <v>156642</v>
@@ -3210,15 +3202,21 @@
       <c r="AB41" s="7"/>
     </row>
     <row r="42" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="50">
-        <f>SUM(C39:C41)*30+D39</f>
-        <v>3276</v>
-      </c>
-      <c r="D42" s="51"/>
-      <c r="F42" s="7"/>
+      <c r="A42" s="6"/>
+      <c r="B42" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="7">
+        <v>48</v>
+      </c>
+      <c r="D42" s="7"/>
+      <c r="E42" s="14">
+        <v>46291</v>
+      </c>
+      <c r="F42" s="9">
+        <f>(E42-$AC$1)/365*12</f>
+        <v>19.824657534246576</v>
+      </c>
       <c r="G42" s="33"/>
       <c r="H42" s="27"/>
       <c r="I42" s="7">
@@ -3240,8 +3238,14 @@
       <c r="AB42" s="7"/>
     </row>
     <row r="43" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="43"/>
-      <c r="D43" s="7"/>
+      <c r="B43" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="50">
+        <f>SUM(C41:C42)*30+D41</f>
+        <v>1599</v>
+      </c>
+      <c r="D43" s="51"/>
       <c r="F43" s="7"/>
       <c r="G43" s="33"/>
       <c r="I43" s="46" t="s">
@@ -3263,25 +3267,9 @@
       <c r="AB43" s="7"/>
     </row>
     <row r="44" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B44" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="C44" s="7">
-        <v>1</v>
-      </c>
-      <c r="D44" s="7">
-        <v>13</v>
-      </c>
-      <c r="E44" s="14">
-        <v>46260</v>
-      </c>
-      <c r="F44" s="9">
-        <f>(E44-$AC$1)/365*12</f>
-        <v>18.805479452054794</v>
-      </c>
+      <c r="B44" s="43"/>
+      <c r="D44" s="7"/>
+      <c r="F44" s="7"/>
       <c r="G44" s="33"/>
       <c r="K44" s="7"/>
       <c r="N44" s="33"/>
@@ -3289,25 +3277,29 @@
       <c r="U44" s="24"/>
       <c r="AB44" s="7"/>
     </row>
-    <row r="45" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="6"/>
+    <row r="45" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="B45" s="44" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="C45" s="7">
-        <v>62</v>
-      </c>
-      <c r="D45" s="7"/>
+        <v>10</v>
+      </c>
+      <c r="D45" s="15">
+        <v>2</v>
+      </c>
       <c r="E45" s="14">
-        <v>46291</v>
+        <v>46352</v>
       </c>
       <c r="F45" s="9">
-        <f>(E45-$AC$1)/365*12</f>
-        <v>19.824657534246576</v>
+        <f t="shared" ref="F45:F46" si="36">(E45-$AC$1)/365*12</f>
+        <v>21.830136986301369</v>
       </c>
       <c r="G45" s="33"/>
       <c r="H45" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I45" s="7">
         <v>156641</v>
@@ -3322,7 +3314,7 @@
         <v>46197</v>
       </c>
       <c r="M45" s="9">
-        <f t="shared" ref="M45:M46" si="36">(L45-$AC$1)/365*12</f>
+        <f t="shared" ref="M45:M46" si="37">(L45-$AC$1)/365*12</f>
         <v>16.734246575342464</v>
       </c>
       <c r="N45" s="33"/>
@@ -3336,15 +3328,23 @@
       <c r="AB45" s="7"/>
     </row>
     <row r="46" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" s="50">
-        <f>SUM(C44:C45)*30+D44</f>
-        <v>1903</v>
-      </c>
-      <c r="D46" s="51"/>
-      <c r="F46" s="7"/>
+      <c r="A46" s="6"/>
+      <c r="B46" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="11">
+        <v>55</v>
+      </c>
+      <c r="D46" s="15">
+        <v>5</v>
+      </c>
+      <c r="E46" s="14">
+        <v>46352</v>
+      </c>
+      <c r="F46" s="9">
+        <f t="shared" si="36"/>
+        <v>21.830136986301369</v>
+      </c>
       <c r="G46" s="33"/>
       <c r="I46" s="7">
         <v>162040</v>
@@ -3357,7 +3357,7 @@
         <v>46303</v>
       </c>
       <c r="M46" s="9">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>20.219178082191782</v>
       </c>
       <c r="N46" s="33"/>
@@ -3365,8 +3365,14 @@
       <c r="AB46" s="7"/>
     </row>
     <row r="47" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="43"/>
-      <c r="D47" s="7"/>
+      <c r="B47" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="50">
+        <f>SUM(C45:C46)*30+D45</f>
+        <v>1952</v>
+      </c>
+      <c r="D47" s="51"/>
       <c r="F47" s="7"/>
       <c r="G47" s="33"/>
       <c r="H47" s="36"/>
@@ -3384,25 +3390,9 @@
       <c r="AB47" s="7"/>
     </row>
     <row r="48" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B48" s="44" t="s">
-        <v>84</v>
-      </c>
-      <c r="C48" s="7">
-        <v>0</v>
-      </c>
-      <c r="D48" s="15">
-        <v>2</v>
-      </c>
-      <c r="E48" s="14">
-        <v>46291</v>
-      </c>
-      <c r="F48" s="9">
-        <f t="shared" ref="F48:F49" si="37">(E48-$AC$1)/365*12</f>
-        <v>19.824657534246576</v>
-      </c>
+      <c r="B48" s="43"/>
+      <c r="D48" s="7"/>
+      <c r="F48" s="7"/>
       <c r="G48" s="33"/>
       <c r="H48" s="24"/>
       <c r="K48" s="7"/>
@@ -3410,23 +3400,25 @@
       <c r="U48" s="24"/>
       <c r="AB48" s="7"/>
     </row>
-    <row r="49" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="6"/>
-      <c r="B49" s="44" t="s">
-        <v>91</v>
-      </c>
-      <c r="C49" s="11">
-        <v>55</v>
-      </c>
-      <c r="D49" s="15">
-        <v>5</v>
+    <row r="49" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" s="7">
+        <v>7</v>
+      </c>
+      <c r="D49" s="11">
+        <v>18</v>
       </c>
       <c r="E49" s="14">
-        <v>46352</v>
+        <v>46260</v>
       </c>
       <c r="F49" s="9">
-        <f t="shared" si="37"/>
-        <v>21.830136986301369</v>
+        <f t="shared" ref="F49:F50" si="38">(E49-$AC$1)/365*12</f>
+        <v>18.805479452054794</v>
       </c>
       <c r="G49" s="33"/>
       <c r="I49" s="11"/>
@@ -3439,15 +3431,23 @@
       <c r="AB49" s="7"/>
     </row>
     <row r="50" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" s="50">
-        <f>SUM(C48:C49)*30+D48</f>
-        <v>1652</v>
-      </c>
-      <c r="D50" s="51"/>
-      <c r="F50" s="7"/>
+      <c r="A50" s="6"/>
+      <c r="B50" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" s="7">
+        <v>39</v>
+      </c>
+      <c r="D50" s="11">
+        <v>9</v>
+      </c>
+      <c r="E50" s="14">
+        <v>46291</v>
+      </c>
+      <c r="F50" s="9">
+        <f t="shared" si="38"/>
+        <v>19.824657534246576</v>
+      </c>
       <c r="G50" s="33"/>
       <c r="I50" s="39"/>
       <c r="J50" s="53"/>
@@ -3458,9 +3458,15 @@
       <c r="U50" s="24"/>
       <c r="AB50" s="7"/>
     </row>
-    <row r="51" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="43"/>
-      <c r="D51" s="7"/>
+    <row r="51" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="50" cm="1">
+        <f t="array" ref="C51">SUM(C49:C50*40)+D49+D50</f>
+        <v>1867</v>
+      </c>
+      <c r="D51" s="51"/>
       <c r="F51" s="7"/>
       <c r="G51" s="33"/>
       <c r="K51" s="7"/>
@@ -3469,25 +3475,9 @@
       <c r="AB51" s="7"/>
     </row>
     <row r="52" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B52" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="C52" s="7">
-        <v>7</v>
-      </c>
-      <c r="D52" s="11">
-        <v>18</v>
-      </c>
-      <c r="E52" s="14">
-        <v>46260</v>
-      </c>
-      <c r="F52" s="9">
-        <f t="shared" ref="F52:F53" si="38">(E52-$AC$1)/365*12</f>
-        <v>18.805479452054794</v>
-      </c>
+      <c r="B52" s="43"/>
+      <c r="D52" s="7"/>
+      <c r="F52" s="7"/>
       <c r="G52" s="33"/>
       <c r="K52" s="7"/>
       <c r="N52" s="24"/>
@@ -3495,22 +3485,24 @@
       <c r="AB52" s="7"/>
     </row>
     <row r="53" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="6"/>
-      <c r="B53" s="43" t="s">
-        <v>48</v>
+      <c r="A53" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="44" t="s">
+        <v>44</v>
       </c>
       <c r="C53" s="7">
-        <v>53</v>
-      </c>
-      <c r="D53" s="11">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="D53" s="7">
+        <v>19</v>
       </c>
       <c r="E53" s="14">
-        <v>46291</v>
-      </c>
-      <c r="F53" s="9">
-        <f t="shared" si="38"/>
-        <v>19.824657534246576</v>
+        <v>45528</v>
+      </c>
+      <c r="F53" s="16">
+        <f>(E53-$AC$1)/365*12</f>
+        <v>-5.2602739726027394</v>
       </c>
       <c r="G53" s="33"/>
       <c r="K53" s="7"/>
@@ -3522,9 +3514,9 @@
       <c r="B54" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C54" s="50" cm="1">
-        <f t="array" ref="C54">SUM(C52:C53*40)+D52+D53</f>
-        <v>2427</v>
+      <c r="C54" s="50">
+        <f>SUM(C53)*30+D53</f>
+        <v>319</v>
       </c>
       <c r="D54" s="51"/>
       <c r="F54" s="7"/>
@@ -3536,7 +3528,6 @@
       <c r="AB54" s="7"/>
     </row>
     <row r="55" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="43"/>
       <c r="D55" s="7"/>
       <c r="F55" s="7"/>
       <c r="G55" s="33"/>
@@ -3544,40 +3535,16 @@
       <c r="U55" s="24"/>
       <c r="AB55" s="7"/>
     </row>
-    <row r="56" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B56" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="C56" s="7">
-        <v>10</v>
-      </c>
-      <c r="D56" s="7">
-        <v>19</v>
-      </c>
-      <c r="E56" s="14">
-        <v>45528</v>
-      </c>
-      <c r="F56" s="16">
-        <f>(E56-$AC$1)/365*12</f>
-        <v>-5.2602739726027394</v>
-      </c>
+    <row r="56" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D56" s="7"/>
+      <c r="F56" s="7"/>
       <c r="G56" s="33"/>
       <c r="K56" s="7"/>
       <c r="U56" s="24"/>
       <c r="AB56" s="7"/>
     </row>
-    <row r="57" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C57" s="50">
-        <f>SUM(C56)*30+D56</f>
-        <v>319</v>
-      </c>
-      <c r="D57" s="51"/>
+    <row r="57" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D57" s="7"/>
       <c r="F57" s="7"/>
       <c r="G57" s="33"/>
       <c r="K57" s="7"/>
@@ -4493,30 +4460,9 @@
       <c r="E193" s="10"/>
       <c r="F193" s="7"/>
     </row>
-    <row r="194" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A194" s="10"/>
-      <c r="B194" s="10"/>
-      <c r="C194" s="10"/>
-      <c r="D194" s="7"/>
-      <c r="E194" s="10"/>
-      <c r="F194" s="7"/>
-    </row>
-    <row r="195" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="10"/>
-      <c r="B195" s="10"/>
-      <c r="C195" s="10"/>
-      <c r="D195" s="7"/>
-      <c r="E195" s="10"/>
-      <c r="F195" s="7"/>
-    </row>
-    <row r="196" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="10"/>
-      <c r="B196" s="10"/>
-      <c r="C196" s="10"/>
-      <c r="D196" s="7"/>
-      <c r="E196" s="10"/>
-      <c r="F196" s="7"/>
-    </row>
+    <row r="194" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="197" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="198" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="199" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4607,14 +4553,14 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="44">
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C47:D47"/>
     <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C51:D51"/>
     <mergeCell ref="J24:K24"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C39:D39"/>
     <mergeCell ref="J47:K47"/>
     <mergeCell ref="J50:K50"/>
     <mergeCell ref="J43:K43"/>
@@ -4622,14 +4568,14 @@
     <mergeCell ref="J31:K31"/>
     <mergeCell ref="J35:K35"/>
     <mergeCell ref="J39:K39"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C26:D26"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="Q41:R41"/>
     <mergeCell ref="Q6:R6"/>

</xml_diff>

<commit_message>
Update lot codes - 2025-02-04 10:54:59
</commit_message>
<xml_diff>
--- a/LotCode.xlsx
+++ b/LotCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf.sharepoint.com/sites/production-warehouse/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7324" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5209830-0D9B-4503-A669-AA77CDEFA79E}"/>
+  <xr:revisionPtr revIDLastSave="7325" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F3F97A2-EE46-47CA-84D5-7A920009370C}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="a/VZ8kgdZMyU/a42HcB04O8OBNrnh4WxCIPRCv9GqcObOgYeM9oYcSfQqndR/nnirMykfzLaq88Ahwir6HajhQ==" workbookSaltValue="jsEDzk1n/+JkLoe+dWrmxg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
@@ -3436,7 +3436,7 @@
         <v>47</v>
       </c>
       <c r="C50" s="7">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D50" s="11">
         <v>9</v>
@@ -3464,7 +3464,7 @@
       </c>
       <c r="C51" s="50" cm="1">
         <f t="array" ref="C51">SUM(C49:C50*40)+D49+D50</f>
-        <v>1867</v>
+        <v>2347</v>
       </c>
       <c r="D51" s="51"/>
       <c r="F51" s="7"/>

</xml_diff>

<commit_message>
Update lot codes - 2025-02-04 11:14:25
</commit_message>
<xml_diff>
--- a/LotCode.xlsx
+++ b/LotCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf.sharepoint.com/sites/production-warehouse/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7325" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F3F97A2-EE46-47CA-84D5-7A920009370C}"/>
+  <xr:revisionPtr revIDLastSave="7330" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F26A635-684E-4817-9A06-907C29D0577E}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="a/VZ8kgdZMyU/a42HcB04O8OBNrnh4WxCIPRCv9GqcObOgYeM9oYcSfQqndR/nnirMykfzLaq88Ahwir6HajhQ==" workbookSaltValue="jsEDzk1n/+JkLoe+dWrmxg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
@@ -622,7 +622,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -743,9 +743,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1105,8 +1102,8 @@
   <dimension ref="A1:AE283"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,6 +1231,9 @@
       <c r="H2" s="23" t="s">
         <v>101</v>
       </c>
+      <c r="K2" s="4">
+        <v>511</v>
+      </c>
       <c r="N2" s="32"/>
       <c r="O2" s="23" t="s">
         <v>95</v>
@@ -1269,14 +1269,14 @@
       <c r="H3" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="49">
+      <c r="I3" s="11">
         <v>158587</v>
       </c>
       <c r="J3" s="7">
         <v>8</v>
       </c>
       <c r="K3" s="7">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="L3" s="8">
         <v>46094</v>
@@ -1328,7 +1328,7 @@
       <c r="AB3" s="12"/>
     </row>
     <row r="4" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="53" t="s">
         <v>103</v>
       </c>
       <c r="B4" s="40">
@@ -1414,11 +1414,11 @@
       <c r="I5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="50">
+      <c r="J5" s="49">
         <f>SUM(J3:J4)*40+K3</f>
-        <v>4329</v>
-      </c>
-      <c r="K5" s="51"/>
+        <v>4336</v>
+      </c>
+      <c r="K5" s="50"/>
       <c r="N5" s="33"/>
       <c r="O5" s="27"/>
       <c r="P5" s="7" t="s">
@@ -1441,22 +1441,22 @@
       <c r="W5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X5" s="50">
+      <c r="X5" s="49">
         <f>SUM(X3:X4)*6+Y3+Y4</f>
         <v>1122</v>
       </c>
-      <c r="Y5" s="51"/>
+      <c r="Y5" s="50"/>
       <c r="AB5" s="7"/>
     </row>
     <row r="6" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="50">
+      <c r="C6" s="49">
         <f>SUM(C3:C5)*40+D3</f>
         <v>6188</v>
       </c>
-      <c r="D6" s="51"/>
+      <c r="D6" s="50"/>
       <c r="F6" s="7"/>
       <c r="G6" s="33"/>
       <c r="K6" s="7"/>
@@ -1464,11 +1464,11 @@
       <c r="P6" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q6" s="50">
+      <c r="Q6" s="49">
         <f>SUM(Q3:Q5)*30+R3+R5</f>
         <v>7809</v>
       </c>
-      <c r="R6" s="51"/>
+      <c r="R6" s="50"/>
       <c r="U6" s="33"/>
       <c r="V6" s="10" t="s">
         <v>10</v>
@@ -1618,11 +1618,11 @@
       <c r="I9" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="50">
+      <c r="J9" s="49">
         <f>SUM(J7:J8)*24+K7</f>
         <v>3634</v>
       </c>
-      <c r="K9" s="51"/>
+      <c r="K9" s="50"/>
       <c r="N9" s="33"/>
       <c r="P9" s="7" t="s">
         <v>48</v>
@@ -1642,11 +1642,11 @@
       <c r="W9" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X9" s="50">
+      <c r="X9" s="49">
         <f>SUM(X7:X8)*6+Y7+Y8</f>
         <v>412</v>
       </c>
-      <c r="Y9" s="51"/>
+      <c r="Y9" s="50"/>
       <c r="AB9" s="7"/>
     </row>
     <row r="10" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1689,11 +1689,11 @@
       <c r="B11" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="50">
+      <c r="C11" s="49">
         <f>SUM(C8:C10)*24+D8</f>
         <v>2168</v>
       </c>
-      <c r="D11" s="51"/>
+      <c r="D11" s="50"/>
       <c r="F11" s="7"/>
       <c r="G11" s="33"/>
       <c r="H11" s="6" t="s">
@@ -1717,11 +1717,11 @@
       <c r="P11" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q11" s="50">
+      <c r="Q11" s="49">
         <f>SUM(Q8:Q10)*30+R8</f>
         <v>6337</v>
       </c>
-      <c r="R11" s="51"/>
+      <c r="R11" s="50"/>
       <c r="U11" s="33"/>
       <c r="V11" s="6" t="s">
         <v>90</v>
@@ -1839,11 +1839,11 @@
       <c r="W13" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X13" s="50">
+      <c r="X13" s="49">
         <f>SUM(X11:X12)*6+Y11+Y12</f>
         <v>1240</v>
       </c>
-      <c r="Y13" s="51"/>
+      <c r="Y13" s="50"/>
       <c r="AB13" s="7"/>
     </row>
     <row r="14" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1917,20 +1917,20 @@
       <c r="I15" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J15" s="50">
+      <c r="J15" s="49">
         <f>SUM(J11:J14)*24+K11</f>
         <v>5520</v>
       </c>
-      <c r="K15" s="51"/>
+      <c r="K15" s="50"/>
       <c r="N15" s="33"/>
       <c r="P15" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q15" s="50">
+      <c r="Q15" s="49">
         <f>SUM(Q13:Q14)*30+R13+R14</f>
         <v>3879</v>
       </c>
-      <c r="R15" s="51"/>
+      <c r="R15" s="50"/>
       <c r="U15" s="33"/>
       <c r="V15" s="6" t="s">
         <v>71</v>
@@ -1957,11 +1957,11 @@
       <c r="B16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="50">
+      <c r="C16" s="49">
         <f>SUM(C13:C15)*24+D13</f>
         <v>5976</v>
       </c>
-      <c r="D16" s="51"/>
+      <c r="D16" s="50"/>
       <c r="F16" s="7"/>
       <c r="G16" s="33"/>
       <c r="K16" s="7"/>
@@ -2034,11 +2034,11 @@
       <c r="W17" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X17" s="50">
+      <c r="X17" s="49">
         <f>SUM(X15:X16)*6+Y15+Y16</f>
         <v>517</v>
       </c>
-      <c r="Y17" s="51"/>
+      <c r="Y17" s="50"/>
       <c r="AB17" s="7"/>
     </row>
     <row r="18" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2132,11 +2132,11 @@
       <c r="P19" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q19" s="50">
+      <c r="Q19" s="49">
         <f>SUM(Q17:Q18)*30+R17+R18</f>
         <v>1385</v>
       </c>
-      <c r="R19" s="51"/>
+      <c r="R19" s="50"/>
       <c r="U19" s="33"/>
       <c r="V19" s="6" t="s">
         <v>20</v>
@@ -2178,11 +2178,11 @@
       <c r="I20" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J20" s="50">
+      <c r="J20" s="49">
         <f>SUM(J17:J19)*12+K17</f>
         <v>2455</v>
       </c>
-      <c r="K20" s="51"/>
+      <c r="K20" s="50"/>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
       <c r="N20" s="33"/>
@@ -2194,22 +2194,22 @@
       <c r="W20" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X20" s="50">
+      <c r="X20" s="49">
         <f>SUM(X19*200)+Y19</f>
         <v>1118</v>
       </c>
-      <c r="Y20" s="51"/>
+      <c r="Y20" s="50"/>
       <c r="AB20" s="7"/>
     </row>
     <row r="21" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="50">
+      <c r="C21" s="49">
         <f>SUM(C18:C20)*12+D18</f>
         <v>1920</v>
       </c>
-      <c r="D21" s="51"/>
+      <c r="D21" s="50"/>
       <c r="F21" s="7"/>
       <c r="G21" s="33"/>
       <c r="K21" s="7"/>
@@ -2336,20 +2336,20 @@
       <c r="P23" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q23" s="50">
+      <c r="Q23" s="49">
         <f>SUM(Q21:Q22)*30+R21</f>
         <v>1841</v>
       </c>
-      <c r="R23" s="51"/>
+      <c r="R23" s="50"/>
       <c r="U23" s="33"/>
       <c r="W23" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X23" s="50">
+      <c r="X23" s="49">
         <f>SUM(X22*200)+Y22</f>
         <v>780</v>
       </c>
-      <c r="Y23" s="51"/>
+      <c r="Y23" s="50"/>
       <c r="AB23" s="7"/>
     </row>
     <row r="24" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2369,11 +2369,11 @@
       <c r="I24" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J24" s="50">
+      <c r="J24" s="49">
         <f>SUM(J22:J23)*30+K22+K23</f>
         <v>2722</v>
       </c>
-      <c r="K24" s="51"/>
+      <c r="K24" s="50"/>
       <c r="N24" s="33"/>
       <c r="U24" s="33"/>
       <c r="AB24" s="7"/>
@@ -2420,7 +2420,7 @@
         <v>16.799999999999997</v>
       </c>
       <c r="U25" s="33"/>
-      <c r="V25" s="52" t="s">
+      <c r="V25" s="51" t="s">
         <v>73</v>
       </c>
       <c r="W25" s="7" t="s">
@@ -2445,11 +2445,11 @@
       <c r="B26" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="50">
+      <c r="C26" s="49">
         <f>SUM(C23:C25)*40+D23+D25</f>
         <v>6440</v>
       </c>
-      <c r="D26" s="51"/>
+      <c r="D26" s="50"/>
       <c r="F26" s="7"/>
       <c r="G26" s="33"/>
       <c r="H26" s="6" t="s">
@@ -2489,7 +2489,7 @@
         <v>16.799999999999997</v>
       </c>
       <c r="U26" s="33"/>
-      <c r="V26" s="52"/>
+      <c r="V26" s="51"/>
       <c r="W26" s="7"/>
       <c r="X26" s="7"/>
       <c r="Y26" s="7"/>
@@ -2538,11 +2538,11 @@
       <c r="W27" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X27" s="50">
+      <c r="X27" s="49">
         <f>SUM(X25:X26)*4+Y25+Y26</f>
         <v>174</v>
       </c>
-      <c r="Y27" s="51"/>
+      <c r="Y27" s="50"/>
       <c r="AB27" s="7"/>
     </row>
     <row r="28" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2569,20 +2569,20 @@
       <c r="I28" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J28" s="50">
+      <c r="J28" s="49">
         <f>SUM(J26:J27)*30+K26</f>
         <v>2292</v>
       </c>
-      <c r="K28" s="51"/>
+      <c r="K28" s="50"/>
       <c r="N28" s="33"/>
       <c r="P28" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q28" s="50">
+      <c r="Q28" s="49">
         <f>SUM(Q25:Q27)*30+R25+R26+R27</f>
         <v>2418</v>
       </c>
-      <c r="R28" s="51"/>
+      <c r="R28" s="50"/>
       <c r="U28" s="33"/>
       <c r="AB28" s="7"/>
     </row>
@@ -2701,21 +2701,21 @@
       <c r="B31" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="50">
+      <c r="C31" s="49">
         <f>SUM(C28:C30)*24+D28</f>
         <v>3432</v>
       </c>
-      <c r="D31" s="51"/>
+      <c r="D31" s="50"/>
       <c r="F31" s="7"/>
       <c r="G31" s="33"/>
       <c r="I31" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J31" s="50">
+      <c r="J31" s="49">
         <f>SUM(J30)*30+K30</f>
         <v>234</v>
       </c>
-      <c r="K31" s="51"/>
+      <c r="K31" s="50"/>
       <c r="N31" s="33"/>
       <c r="O31" s="6"/>
       <c r="P31" s="7" t="s">
@@ -2736,11 +2736,11 @@
       <c r="W31" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X31" s="50">
+      <c r="X31" s="49">
         <f>SUM(X29:X30)*30+Y29</f>
         <v>1270</v>
       </c>
-      <c r="Y31" s="51"/>
+      <c r="Y31" s="50"/>
       <c r="AB31" s="7"/>
     </row>
     <row r="32" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2753,11 +2753,11 @@
       <c r="P32" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q32" s="50">
+      <c r="Q32" s="49">
         <f>SUM(Q30:Q31)*30+R30</f>
         <v>609</v>
       </c>
-      <c r="R32" s="51"/>
+      <c r="R32" s="50"/>
       <c r="U32" s="33"/>
       <c r="AB32" s="7"/>
     </row>
@@ -2894,21 +2894,21 @@
       <c r="B35" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="50">
+      <c r="C35" s="49">
         <f>SUM(C33:C34)*24+D33</f>
         <v>2094</v>
       </c>
-      <c r="D35" s="51"/>
+      <c r="D35" s="50"/>
       <c r="F35" s="7"/>
       <c r="G35" s="33"/>
       <c r="I35" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J35" s="50">
+      <c r="J35" s="49">
         <f>SUM(J33:J34)*24+K33</f>
         <v>1129</v>
       </c>
-      <c r="K35" s="51"/>
+      <c r="K35" s="50"/>
       <c r="N35" s="33"/>
       <c r="O35" s="6"/>
       <c r="P35" s="7" t="s">
@@ -2929,11 +2929,11 @@
       <c r="W35" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X35" s="50">
+      <c r="X35" s="49">
         <f>SUM(X33:X34)*18+Y33</f>
         <v>1175</v>
       </c>
-      <c r="Y35" s="51"/>
+      <c r="Y35" s="50"/>
       <c r="AB35" s="7"/>
     </row>
     <row r="36" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2946,11 +2946,11 @@
       <c r="P36" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q36" s="50">
+      <c r="Q36" s="49">
         <f>SUM(Q34:Q35)*30+R34</f>
         <v>828</v>
       </c>
-      <c r="R36" s="51"/>
+      <c r="R36" s="50"/>
       <c r="S36" s="7"/>
       <c r="T36" s="7"/>
       <c r="U36" s="33"/>
@@ -3075,32 +3075,32 @@
       <c r="W38" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X38" s="50">
+      <c r="X38" s="49">
         <f>SUM(X37:X37)*18+Y37</f>
         <v>2</v>
       </c>
-      <c r="Y38" s="51"/>
+      <c r="Y38" s="50"/>
       <c r="AB38" s="7"/>
     </row>
     <row r="39" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="50">
+      <c r="C39" s="49">
         <f>SUM(C37:C38)*30+D37</f>
         <v>2646</v>
       </c>
-      <c r="D39" s="51"/>
+      <c r="D39" s="50"/>
       <c r="F39" s="7"/>
       <c r="G39" s="33"/>
       <c r="I39" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J39" s="50">
+      <c r="J39" s="49">
         <f>SUM(J37:J38)*24+K37</f>
         <v>972</v>
       </c>
-      <c r="K39" s="51"/>
+      <c r="K39" s="50"/>
       <c r="N39" s="33"/>
       <c r="O39" s="24"/>
       <c r="P39" s="7" t="s">
@@ -3193,11 +3193,11 @@
       <c r="P41" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q41" s="50">
+      <c r="Q41" s="49">
         <f>SUM(Q38:Q40)*30+R38+R40</f>
         <v>3245</v>
       </c>
-      <c r="R41" s="51"/>
+      <c r="R41" s="50"/>
       <c r="U41" s="34"/>
       <c r="AB41" s="7"/>
     </row>
@@ -3241,21 +3241,21 @@
       <c r="B43" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C43" s="50">
+      <c r="C43" s="49">
         <f>SUM(C41:C42)*30+D41</f>
         <v>1599</v>
       </c>
-      <c r="D43" s="51"/>
+      <c r="D43" s="50"/>
       <c r="F43" s="7"/>
       <c r="G43" s="33"/>
       <c r="I43" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J43" s="50">
+      <c r="J43" s="49">
         <f>SUM(J41:J42)*24+K41</f>
         <v>555</v>
       </c>
-      <c r="K43" s="51"/>
+      <c r="K43" s="50"/>
       <c r="N43" s="33"/>
       <c r="O43" s="6" t="s">
         <v>37</v>
@@ -3368,22 +3368,22 @@
       <c r="B47" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C47" s="50">
+      <c r="C47" s="49">
         <f>SUM(C45:C46)*30+D45</f>
         <v>1952</v>
       </c>
-      <c r="D47" s="51"/>
+      <c r="D47" s="50"/>
       <c r="F47" s="7"/>
       <c r="G47" s="33"/>
       <c r="H47" s="36"/>
       <c r="I47" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J47" s="50">
+      <c r="J47" s="49">
         <f>SUM(J45:J46)*24+K45</f>
         <v>1414</v>
       </c>
-      <c r="K47" s="51"/>
+      <c r="K47" s="50"/>
       <c r="N47" s="33"/>
       <c r="S47" s="4"/>
       <c r="U47" s="24"/>
@@ -3450,8 +3450,8 @@
       </c>
       <c r="G50" s="33"/>
       <c r="I50" s="39"/>
-      <c r="J50" s="53"/>
-      <c r="K50" s="53"/>
+      <c r="J50" s="52"/>
+      <c r="K50" s="52"/>
       <c r="L50" s="24"/>
       <c r="M50" s="24"/>
       <c r="N50" s="24"/>
@@ -3462,11 +3462,11 @@
       <c r="B51" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C51" s="50" cm="1">
+      <c r="C51" s="49" cm="1">
         <f t="array" ref="C51">SUM(C49:C50*40)+D49+D50</f>
         <v>2347</v>
       </c>
-      <c r="D51" s="51"/>
+      <c r="D51" s="50"/>
       <c r="F51" s="7"/>
       <c r="G51" s="33"/>
       <c r="K51" s="7"/>
@@ -3514,11 +3514,11 @@
       <c r="B54" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C54" s="50">
+      <c r="C54" s="49">
         <f>SUM(C53)*30+D53</f>
         <v>319</v>
       </c>
-      <c r="D54" s="51"/>
+      <c r="D54" s="50"/>
       <c r="F54" s="7"/>
       <c r="G54" s="33"/>
       <c r="K54" s="7"/>

</xml_diff>

<commit_message>
Update lot codes - 2025-02-04 12:50:37
</commit_message>
<xml_diff>
--- a/LotCode.xlsx
+++ b/LotCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf.sharepoint.com/sites/production-warehouse/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7330" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F26A635-684E-4817-9A06-907C29D0577E}"/>
+  <xr:revisionPtr revIDLastSave="7335" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{495186B8-DF8B-4CBF-A8CE-0C9B926A7A5A}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="a/VZ8kgdZMyU/a42HcB04O8OBNrnh4WxCIPRCv9GqcObOgYeM9oYcSfQqndR/nnirMykfzLaq88Ahwir6HajhQ==" workbookSaltValue="jsEDzk1n/+JkLoe+dWrmxg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
@@ -391,7 +391,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,6 +442,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -481,7 +487,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -617,12 +623,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -758,6 +777,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1103,7 +1125,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,7 +1553,7 @@
         <v>159367</v>
       </c>
       <c r="C8" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="7">
         <v>8</v>
@@ -1691,7 +1713,7 @@
       </c>
       <c r="C11" s="49">
         <f>SUM(C8:C10)*24+D8</f>
-        <v>2168</v>
+        <v>2144</v>
       </c>
       <c r="D11" s="50"/>
       <c r="F11" s="7"/>
@@ -2384,7 +2406,7 @@
         <v>105</v>
       </c>
       <c r="C25" s="11">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="8">
@@ -2447,7 +2469,7 @@
       </c>
       <c r="C26" s="49">
         <f>SUM(C23:C25)*40+D23+D25</f>
-        <v>6440</v>
+        <v>5360</v>
       </c>
       <c r="D26" s="50"/>
       <c r="F26" s="7"/>
@@ -3556,6 +3578,7 @@
       <c r="F58" s="7"/>
       <c r="G58" s="33"/>
       <c r="K58" s="7"/>
+      <c r="S58" s="54"/>
       <c r="U58" s="24"/>
       <c r="AB58" s="7"/>
     </row>

</xml_diff>

<commit_message>
Update lot codes - 2025-02-04 13:07:22
</commit_message>
<xml_diff>
--- a/LotCode.xlsx
+++ b/LotCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf.sharepoint.com/sites/production-warehouse/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7335" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{495186B8-DF8B-4CBF-A8CE-0C9B926A7A5A}"/>
+  <xr:revisionPtr revIDLastSave="7358" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{123389CA-3E21-4FE2-8B90-DD3D15C779DF}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="a/VZ8kgdZMyU/a42HcB04O8OBNrnh4WxCIPRCv9GqcObOgYeM9oYcSfQqndR/nnirMykfzLaq88Ahwir6HajhQ==" workbookSaltValue="jsEDzk1n/+JkLoe+dWrmxg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="105">
   <si>
     <t>SKU</t>
   </si>
@@ -371,9 +371,6 @@
   </si>
   <si>
     <t>2.4.25</t>
-  </si>
-  <si>
-    <t>4 on blue rack</t>
   </si>
   <si>
     <t>165893</t>
@@ -1275,10 +1272,10 @@
         <v>159368</v>
       </c>
       <c r="C3" s="7">
+        <v>6</v>
+      </c>
+      <c r="D3" s="7">
         <v>2</v>
-      </c>
-      <c r="D3" s="7">
-        <v>28</v>
       </c>
       <c r="E3" s="41">
         <v>46304</v>
@@ -1350,9 +1347,7 @@
       <c r="AB3" s="12"/>
     </row>
     <row r="4" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="53" t="s">
-        <v>103</v>
-      </c>
+      <c r="A4" s="53"/>
       <c r="B4" s="40">
         <v>163236</v>
       </c>
@@ -1476,7 +1471,7 @@
       </c>
       <c r="C6" s="49">
         <f>SUM(C3:C5)*40+D3</f>
-        <v>6188</v>
+        <v>6322</v>
       </c>
       <c r="D6" s="50"/>
       <c r="F6" s="7"/>
@@ -1556,13 +1551,13 @@
         <v>7</v>
       </c>
       <c r="D8" s="7">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E8" s="8">
         <v>46283</v>
       </c>
       <c r="F8" s="9">
-        <f t="shared" ref="F8" si="7">(E8-$AC$1)/365*12</f>
+        <f t="shared" ref="F8:F9" si="7">(E8-$AC$1)/365*12</f>
         <v>19.56164383561644</v>
       </c>
       <c r="G8" s="33"/>
@@ -1621,20 +1616,20 @@
       <c r="AB8" s="7"/>
     </row>
     <row r="9" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="27"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="7">
-        <v>161798</v>
-      </c>
-      <c r="C9" s="11">
-        <v>60</v>
+        <v>159367</v>
+      </c>
+      <c r="C9" s="7">
+        <v>22</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="8">
-        <v>46324</v>
+        <v>46283</v>
       </c>
       <c r="F9" s="9">
-        <f t="shared" ref="F9:F10" si="10">(E9-$AC$1)/365*12</f>
-        <v>20.909589041095892</v>
+        <f t="shared" si="7"/>
+        <v>19.56164383561644</v>
       </c>
       <c r="G9" s="33"/>
       <c r="I9" s="46" t="s">
@@ -1674,18 +1669,18 @@
     <row r="10" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="27"/>
       <c r="B10" s="7">
-        <v>162036</v>
+        <v>161798</v>
       </c>
       <c r="C10" s="11">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="8">
-        <v>46337</v>
+        <v>46324</v>
       </c>
       <c r="F10" s="9">
-        <f t="shared" si="10"/>
-        <v>21.336986301369862</v>
+        <f t="shared" ref="F10:F12" si="10">(E10-$AC$1)/365*12</f>
+        <v>20.909589041095892</v>
       </c>
       <c r="G10" s="33"/>
       <c r="K10" s="7"/>
@@ -1708,15 +1703,21 @@
       <c r="AB10" s="7"/>
     </row>
     <row r="11" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="49">
-        <f>SUM(C8:C10)*24+D8</f>
-        <v>2144</v>
-      </c>
-      <c r="D11" s="50"/>
-      <c r="F11" s="7"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="7">
+        <v>162036</v>
+      </c>
+      <c r="C11" s="11">
+        <v>22</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8">
+        <v>46337</v>
+      </c>
+      <c r="F11" s="9">
+        <f t="shared" si="10"/>
+        <v>21.336986301369862</v>
+      </c>
       <c r="G11" s="33"/>
       <c r="H11" s="6" t="s">
         <v>63</v>
@@ -1767,8 +1768,21 @@
       <c r="AB11" s="7"/>
     </row>
     <row r="12" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="27"/>
+      <c r="B12" s="7">
+        <v>162037</v>
+      </c>
+      <c r="C12" s="11">
+        <v>1</v>
+      </c>
       <c r="D12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="8">
+        <v>46359</v>
+      </c>
+      <c r="F12" s="9">
+        <f t="shared" si="10"/>
+        <v>22.06027397260274</v>
+      </c>
       <c r="G12" s="33"/>
       <c r="H12" s="27"/>
       <c r="I12" s="7">
@@ -1804,23 +1818,15 @@
       <c r="AB12" s="7"/>
     </row>
     <row r="13" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="35">
-        <v>159366</v>
-      </c>
-      <c r="C13" s="7">
-        <v>1</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8">
-        <v>46283</v>
-      </c>
-      <c r="F13" s="9">
-        <f>(E13-$AC$1)/365*12</f>
-        <v>19.56164383561644</v>
-      </c>
+      <c r="B13" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="49">
+        <f>SUM(C8:C12)*24+D8</f>
+        <v>2706</v>
+      </c>
+      <c r="D13" s="50"/>
+      <c r="F13" s="7"/>
       <c r="G13" s="33"/>
       <c r="H13" s="27"/>
       <c r="I13" s="7">
@@ -1869,20 +1875,8 @@
       <c r="AB13" s="7"/>
     </row>
     <row r="14" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="35">
-        <v>161793</v>
-      </c>
-      <c r="C14" s="11">
-        <v>74</v>
-      </c>
       <c r="D14" s="7"/>
-      <c r="E14" s="8">
-        <v>46313</v>
-      </c>
-      <c r="F14" s="9">
-        <f t="shared" ref="F14" si="13">(E14-$AC$1)/365*12</f>
-        <v>20.547945205479451</v>
-      </c>
+      <c r="F14" s="7"/>
       <c r="G14" s="33"/>
       <c r="H14" s="27"/>
       <c r="I14" s="7">
@@ -1921,19 +1915,22 @@
       <c r="AB14" s="7"/>
     </row>
     <row r="15" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="B15" s="35">
-        <v>161794</v>
-      </c>
-      <c r="C15" s="11">
-        <v>174</v>
+        <v>159366</v>
+      </c>
+      <c r="C15" s="7">
+        <v>7</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="8">
-        <v>46324</v>
+        <v>46283</v>
       </c>
       <c r="F15" s="9">
-        <f t="shared" ref="F15" si="14">(E15-$AC$1)/365*12</f>
-        <v>20.909589041095892</v>
+        <f>(E15-$AC$1)/365*12</f>
+        <v>19.56164383561644</v>
       </c>
       <c r="G15" s="33"/>
       <c r="I15" s="46" t="s">
@@ -1970,21 +1967,26 @@
         <v>47024</v>
       </c>
       <c r="AA15" s="9">
-        <f t="shared" ref="AA15:AA16" si="15">(Z15-$AC$1)/365*12</f>
+        <f t="shared" ref="AA15:AA16" si="13">(Z15-$AC$1)/365*12</f>
         <v>43.923287671232877</v>
       </c>
       <c r="AB15" s="7"/>
     </row>
     <row r="16" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="49">
-        <f>SUM(C13:C15)*24+D13</f>
-        <v>5976</v>
-      </c>
-      <c r="D16" s="50"/>
-      <c r="F16" s="7"/>
+      <c r="B16" s="35">
+        <v>161793</v>
+      </c>
+      <c r="C16" s="11">
+        <v>68</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8">
+        <v>46313</v>
+      </c>
+      <c r="F16" s="9">
+        <f t="shared" ref="F16" si="14">(E16-$AC$1)/365*12</f>
+        <v>20.547945205479451</v>
+      </c>
       <c r="G16" s="33"/>
       <c r="K16" s="7"/>
       <c r="N16" s="33"/>
@@ -2003,15 +2005,26 @@
         <v>47085</v>
       </c>
       <c r="AA16" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>45.92876712328767</v>
       </c>
       <c r="AB16" s="8"/>
     </row>
     <row r="17" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="43"/>
+      <c r="B17" s="35">
+        <v>161794</v>
+      </c>
+      <c r="C17" s="11">
+        <v>174</v>
+      </c>
       <c r="D17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="E17" s="8">
+        <v>46324</v>
+      </c>
+      <c r="F17" s="9">
+        <f t="shared" ref="F17" si="15">(E17-$AC$1)/365*12</f>
+        <v>20.909589041095892</v>
+      </c>
       <c r="G17" s="33"/>
       <c r="H17" s="6" t="s">
         <v>64</v>
@@ -2064,25 +2077,15 @@
       <c r="AB17" s="7"/>
     </row>
     <row r="18" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="44" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" s="11">
-        <v>5</v>
-      </c>
-      <c r="D18" s="7">
-        <v>0</v>
-      </c>
-      <c r="E18" s="8">
-        <v>46283</v>
-      </c>
-      <c r="F18" s="9">
-        <f t="shared" ref="F18" si="18">(E18-$AC$1)/365*12</f>
-        <v>19.56164383561644</v>
-      </c>
+      <c r="B18" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="49">
+        <f>SUM(C15:C17)*24+D15</f>
+        <v>5976</v>
+      </c>
+      <c r="D18" s="50"/>
+      <c r="F18" s="7"/>
       <c r="G18" s="33"/>
       <c r="H18" s="6"/>
       <c r="I18" s="7">
@@ -2113,27 +2116,16 @@
         <v>46321</v>
       </c>
       <c r="T18" s="9">
-        <f t="shared" ref="T18" si="19">(S18-$AC$1)/365*12</f>
+        <f t="shared" ref="T18" si="18">(S18-$AC$1)/365*12</f>
         <v>20.81095890410959</v>
       </c>
       <c r="U18" s="33"/>
       <c r="AB18" s="7"/>
     </row>
     <row r="19" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="27"/>
-      <c r="B19" s="44" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="7">
-        <v>54</v>
-      </c>
-      <c r="E19" s="8">
-        <v>46283</v>
-      </c>
-      <c r="F19" s="9">
-        <f t="shared" ref="F19:F20" si="20">(E19-$AC$1)/365*12</f>
-        <v>19.56164383561644</v>
-      </c>
+      <c r="B19" s="43"/>
+      <c r="D19" s="7"/>
+      <c r="F19" s="7"/>
       <c r="G19" s="33"/>
       <c r="H19" s="6"/>
       <c r="I19" s="7">
@@ -2182,19 +2174,24 @@
       <c r="AB19" s="7"/>
     </row>
     <row r="20" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="27"/>
+      <c r="A20" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="B20" s="44" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" s="7">
-        <v>101</v>
+        <v>91</v>
+      </c>
+      <c r="C20" s="11">
+        <v>5</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0</v>
       </c>
       <c r="E20" s="8">
-        <v>46303</v>
+        <v>46283</v>
       </c>
       <c r="F20" s="9">
-        <f t="shared" si="20"/>
-        <v>20.219178082191782</v>
+        <f t="shared" ref="F20" si="19">(E20-$AC$1)/365*12</f>
+        <v>19.56164383561644</v>
       </c>
       <c r="G20" s="33"/>
       <c r="I20" s="46" t="s">
@@ -2223,16 +2220,21 @@
       <c r="Y20" s="50"/>
       <c r="AB20" s="7"/>
     </row>
-    <row r="21" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="49">
-        <f>SUM(C18:C20)*12+D18</f>
-        <v>1920</v>
-      </c>
-      <c r="D21" s="50"/>
-      <c r="F21" s="7"/>
+    <row r="21" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="27"/>
+      <c r="B21" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="7">
+        <v>54</v>
+      </c>
+      <c r="E21" s="8">
+        <v>46283</v>
+      </c>
+      <c r="F21" s="9">
+        <f t="shared" ref="F21:F22" si="20">(E21-$AC$1)/365*12</f>
+        <v>19.56164383561644</v>
+      </c>
       <c r="G21" s="33"/>
       <c r="K21" s="7"/>
       <c r="N21" s="33"/>
@@ -2259,9 +2261,20 @@
       <c r="AB21" s="7"/>
     </row>
     <row r="22" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="43"/>
-      <c r="D22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="7">
+        <v>101</v>
+      </c>
+      <c r="E22" s="8">
+        <v>46303</v>
+      </c>
+      <c r="F22" s="9">
+        <f t="shared" si="20"/>
+        <v>20.219178082191782</v>
+      </c>
       <c r="G22" s="33"/>
       <c r="H22" s="6" t="s">
         <v>18</v>
@@ -2320,23 +2333,15 @@
       <c r="AB22" s="7"/>
     </row>
     <row r="23" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" s="45" t="s">
-        <v>104</v>
-      </c>
-      <c r="C23" s="11">
-        <v>6</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="8">
-        <v>46211</v>
-      </c>
-      <c r="F23" s="9">
-        <f>(E23-$AC$1)/365*12</f>
-        <v>17.194520547945206</v>
-      </c>
+      <c r="B23" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="49">
+        <f>SUM(C20:C22)*12+D20</f>
+        <v>1920</v>
+      </c>
+      <c r="D23" s="50"/>
+      <c r="F23" s="7"/>
       <c r="G23" s="33"/>
       <c r="I23" s="7" t="s">
         <v>87</v>
@@ -2375,18 +2380,9 @@
       <c r="AB23" s="7"/>
     </row>
     <row r="24" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6"/>
-      <c r="B24" s="45" t="s">
-        <v>104</v>
-      </c>
-      <c r="C24" s="11">
-        <v>119</v>
-      </c>
+      <c r="B24" s="43"/>
       <c r="D24" s="7"/>
-      <c r="E24" s="8">
-        <v>46211</v>
-      </c>
-      <c r="F24" s="9"/>
+      <c r="F24" s="7"/>
       <c r="G24" s="33"/>
       <c r="I24" s="46" t="s">
         <v>8</v>
@@ -2400,21 +2396,23 @@
       <c r="U24" s="33"/>
       <c r="AB24" s="7"/>
     </row>
-    <row r="25" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="29"/>
+    <row r="25" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="B25" s="45" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C25" s="11">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="8">
-        <v>46302</v>
+        <v>46211</v>
       </c>
       <c r="F25" s="9">
         <f>(E25-$AC$1)/365*12</f>
-        <v>20.186301369863013</v>
+        <v>17.194520547945206</v>
       </c>
       <c r="G25" s="33"/>
       <c r="K25" s="7"/>
@@ -2464,15 +2462,18 @@
       <c r="AB25" s="7"/>
     </row>
     <row r="26" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="49">
-        <f>SUM(C23:C25)*40+D23+D25</f>
-        <v>5360</v>
-      </c>
-      <c r="D26" s="50"/>
-      <c r="F26" s="7"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" s="11">
+        <v>119</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="8">
+        <v>46211</v>
+      </c>
+      <c r="F26" s="9"/>
       <c r="G26" s="33"/>
       <c r="H26" s="6" t="s">
         <v>23</v>
@@ -2520,9 +2521,21 @@
       <c r="AB26" s="7"/>
     </row>
     <row r="27" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="43"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="11">
+        <v>9</v>
+      </c>
       <c r="D27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="E27" s="8">
+        <v>46302</v>
+      </c>
+      <c r="F27" s="9">
+        <f>(E27-$AC$1)/365*12</f>
+        <v>20.186301369863013</v>
+      </c>
       <c r="G27" s="33"/>
       <c r="I27" s="7" t="s">
         <v>88</v>
@@ -2568,25 +2581,15 @@
       <c r="AB27" s="7"/>
     </row>
     <row r="28" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="7">
+      <c r="B28" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="7">
-        <v>0</v>
-      </c>
-      <c r="E28" s="8">
-        <v>46211</v>
-      </c>
-      <c r="F28" s="9">
-        <f>(E28-$AC$1)/365*12</f>
-        <v>17.194520547945206</v>
-      </c>
+      <c r="C28" s="49">
+        <f>SUM(C25:C27)*40+D25+D27</f>
+        <v>5320</v>
+      </c>
+      <c r="D28" s="50"/>
+      <c r="F28" s="7"/>
       <c r="G28" s="33"/>
       <c r="I28" s="46" t="s">
         <v>8</v>
@@ -2609,20 +2612,9 @@
       <c r="AB28" s="7"/>
     </row>
     <row r="29" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="7">
-        <v>55</v>
-      </c>
+      <c r="B29" s="43"/>
       <c r="D29" s="7"/>
-      <c r="E29" s="8">
-        <v>46211</v>
-      </c>
-      <c r="F29" s="9">
-        <f>(E29-$AC$1)/365*12</f>
-        <v>17.194520547945206</v>
-      </c>
+      <c r="F29" s="7"/>
       <c r="G29" s="33"/>
       <c r="K29" s="7"/>
       <c r="N29" s="33"/>
@@ -2649,19 +2641,24 @@
       <c r="AB29" s="8"/>
     </row>
     <row r="30" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="B30" s="44" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="C30" s="7">
-        <v>80</v>
-      </c>
-      <c r="D30" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="D30" s="7">
+        <v>0</v>
+      </c>
       <c r="E30" s="8">
-        <v>46248</v>
+        <v>46211</v>
       </c>
       <c r="F30" s="9">
         <f>(E30-$AC$1)/365*12</f>
-        <v>18.410958904109588</v>
+        <v>17.194520547945206</v>
       </c>
       <c r="G30" s="33"/>
       <c r="H30" s="6" t="s">
@@ -2720,15 +2717,20 @@
       </c>
     </row>
     <row r="31" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="49">
-        <f>SUM(C28:C30)*24+D28</f>
-        <v>3432</v>
-      </c>
-      <c r="D31" s="50"/>
-      <c r="F31" s="7"/>
+      <c r="B31" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="7">
+        <v>55</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="8">
+        <v>46211</v>
+      </c>
+      <c r="F31" s="9">
+        <f>(E31-$AC$1)/365*12</f>
+        <v>17.194520547945206</v>
+      </c>
       <c r="G31" s="33"/>
       <c r="I31" s="46" t="s">
         <v>8</v>
@@ -2766,9 +2768,20 @@
       <c r="AB31" s="7"/>
     </row>
     <row r="32" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="43"/>
+      <c r="B32" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="7">
+        <v>80</v>
+      </c>
       <c r="D32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="E32" s="8">
+        <v>46248</v>
+      </c>
+      <c r="F32" s="9">
+        <f>(E32-$AC$1)/365*12</f>
+        <v>18.410958904109588</v>
+      </c>
       <c r="G32" s="33"/>
       <c r="K32" s="7"/>
       <c r="N32" s="33"/>
@@ -2783,26 +2796,16 @@
       <c r="U32" s="33"/>
       <c r="AB32" s="7"/>
     </row>
-    <row r="33" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="C33" s="7">
+    <row r="33" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="7">
-        <v>6</v>
-      </c>
-      <c r="E33" s="8">
-        <v>46312</v>
-      </c>
-      <c r="F33" s="9">
-        <f>(E33-$AC$1)/365*12</f>
-        <v>20.515068493150686</v>
-      </c>
+      <c r="C33" s="49">
+        <f>SUM(C30:C32)*24+D30</f>
+        <v>3432</v>
+      </c>
+      <c r="D33" s="50"/>
+      <c r="F33" s="7"/>
       <c r="G33" s="33"/>
       <c r="H33" s="17" t="s">
         <v>65</v>
@@ -2847,21 +2850,9 @@
       <c r="AB33" s="7"/>
     </row>
     <row r="34" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="27"/>
-      <c r="B34" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="C34" s="7">
-        <v>79</v>
-      </c>
+      <c r="B34" s="43"/>
       <c r="D34" s="7"/>
-      <c r="E34" s="8">
-        <v>46312</v>
-      </c>
-      <c r="F34" s="9">
-        <f>(E34-$AC$1)/365*12</f>
-        <v>20.515068493150686</v>
-      </c>
+      <c r="F34" s="7"/>
       <c r="G34" s="33"/>
       <c r="I34" s="7">
         <v>162839</v>
@@ -2913,15 +2904,25 @@
       <c r="AB34" s="7"/>
     </row>
     <row r="35" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="47" t="s">
+      <c r="A35" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="7">
         <v>8</v>
       </c>
-      <c r="C35" s="49">
-        <f>SUM(C33:C34)*24+D33</f>
-        <v>2094</v>
-      </c>
-      <c r="D35" s="50"/>
-      <c r="F35" s="7"/>
+      <c r="D35" s="7">
+        <v>6</v>
+      </c>
+      <c r="E35" s="8">
+        <v>46312</v>
+      </c>
+      <c r="F35" s="9">
+        <f>(E35-$AC$1)/365*12</f>
+        <v>20.515068493150686</v>
+      </c>
       <c r="G35" s="33"/>
       <c r="I35" s="46" t="s">
         <v>8</v>
@@ -2959,9 +2960,21 @@
       <c r="AB35" s="7"/>
     </row>
     <row r="36" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="43"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="7">
+        <v>79</v>
+      </c>
       <c r="D36" s="7"/>
-      <c r="F36" s="7"/>
+      <c r="E36" s="8">
+        <v>46312</v>
+      </c>
+      <c r="F36" s="9">
+        <f>(E36-$AC$1)/365*12</f>
+        <v>20.515068493150686</v>
+      </c>
       <c r="G36" s="33"/>
       <c r="K36" s="7"/>
       <c r="N36" s="33"/>
@@ -2979,25 +2992,15 @@
       <c r="AB36" s="7"/>
     </row>
     <row r="37" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" s="11">
-        <v>7</v>
-      </c>
-      <c r="D37" s="7">
-        <v>6</v>
-      </c>
-      <c r="E37" s="14">
-        <v>46260</v>
-      </c>
-      <c r="F37" s="9">
-        <f>(E37-$AC$1)/365*12</f>
-        <v>18.805479452054794</v>
-      </c>
+      <c r="B37" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="49">
+        <f>SUM(C35:C36)*24+D35</f>
+        <v>2094</v>
+      </c>
+      <c r="D37" s="50"/>
+      <c r="F37" s="7"/>
       <c r="G37" s="33"/>
       <c r="H37" s="6" t="s">
         <v>66</v>
@@ -3044,20 +3047,9 @@
       <c r="AB37" s="7"/>
     </row>
     <row r="38" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="C38" s="40">
-        <v>81</v>
-      </c>
+      <c r="B38" s="43"/>
       <c r="D38" s="7"/>
-      <c r="E38" s="14">
-        <v>46352</v>
-      </c>
-      <c r="F38" s="9">
-        <f>(E38-$AC$1)/365*12</f>
-        <v>21.830136986301369</v>
-      </c>
+      <c r="F38" s="7"/>
       <c r="G38" s="33"/>
       <c r="I38" s="7">
         <v>161789</v>
@@ -3105,15 +3097,25 @@
       <c r="AB38" s="7"/>
     </row>
     <row r="39" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="49">
-        <f>SUM(C37:C38)*30+D37</f>
-        <v>2646</v>
-      </c>
-      <c r="D39" s="50"/>
-      <c r="F39" s="7"/>
+      <c r="A39" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="11">
+        <v>7</v>
+      </c>
+      <c r="D39" s="7">
+        <v>6</v>
+      </c>
+      <c r="E39" s="14">
+        <v>46260</v>
+      </c>
+      <c r="F39" s="9">
+        <f>(E39-$AC$1)/365*12</f>
+        <v>18.805479452054794</v>
+      </c>
       <c r="G39" s="33"/>
       <c r="I39" s="46" t="s">
         <v>8</v>
@@ -3143,9 +3145,20 @@
       <c r="AB39" s="7"/>
     </row>
     <row r="40" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="43"/>
+      <c r="B40" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="40">
+        <v>81</v>
+      </c>
       <c r="D40" s="7"/>
-      <c r="F40" s="7"/>
+      <c r="E40" s="14">
+        <v>46352</v>
+      </c>
+      <c r="F40" s="9">
+        <f>(E40-$AC$1)/365*12</f>
+        <v>21.830136986301369</v>
+      </c>
       <c r="G40" s="33"/>
       <c r="I40" s="13"/>
       <c r="J40" s="30"/>
@@ -3172,25 +3185,15 @@
       <c r="AB40" s="7"/>
     </row>
     <row r="41" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="7">
-        <v>5</v>
-      </c>
-      <c r="D41" s="7">
-        <v>9</v>
-      </c>
-      <c r="E41" s="14">
-        <v>46291</v>
-      </c>
-      <c r="F41" s="9">
-        <f>(E41-$AC$1)/365*12</f>
-        <v>19.824657534246576</v>
-      </c>
+      <c r="B41" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="49">
+        <f>SUM(C39:C40)*30+D39</f>
+        <v>2646</v>
+      </c>
+      <c r="D41" s="50"/>
+      <c r="F41" s="7"/>
       <c r="G41" s="33"/>
       <c r="H41" s="6" t="s">
         <v>67</v>
@@ -3224,21 +3227,9 @@
       <c r="AB41" s="7"/>
     </row>
     <row r="42" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="6"/>
-      <c r="B42" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="C42" s="7">
-        <v>48</v>
-      </c>
+      <c r="B42" s="43"/>
       <c r="D42" s="7"/>
-      <c r="E42" s="14">
-        <v>46291</v>
-      </c>
-      <c r="F42" s="9">
-        <f>(E42-$AC$1)/365*12</f>
-        <v>19.824657534246576</v>
-      </c>
+      <c r="F42" s="7"/>
       <c r="G42" s="33"/>
       <c r="H42" s="27"/>
       <c r="I42" s="7">
@@ -3260,15 +3251,25 @@
       <c r="AB42" s="7"/>
     </row>
     <row r="43" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C43" s="49">
-        <f>SUM(C41:C42)*30+D41</f>
-        <v>1599</v>
-      </c>
-      <c r="D43" s="50"/>
-      <c r="F43" s="7"/>
+      <c r="A43" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="7">
+        <v>5</v>
+      </c>
+      <c r="D43" s="7">
+        <v>9</v>
+      </c>
+      <c r="E43" s="14">
+        <v>46291</v>
+      </c>
+      <c r="F43" s="9">
+        <f>(E43-$AC$1)/365*12</f>
+        <v>19.824657534246576</v>
+      </c>
       <c r="G43" s="33"/>
       <c r="I43" s="46" t="s">
         <v>8</v>
@@ -3288,10 +3289,22 @@
       <c r="U43" s="24"/>
       <c r="AB43" s="7"/>
     </row>
-    <row r="44" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="43"/>
+    <row r="44" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="6"/>
+      <c r="B44" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="7">
+        <v>48</v>
+      </c>
       <c r="D44" s="7"/>
-      <c r="F44" s="7"/>
+      <c r="E44" s="14">
+        <v>46291</v>
+      </c>
+      <c r="F44" s="9">
+        <f>(E44-$AC$1)/365*12</f>
+        <v>19.824657534246576</v>
+      </c>
       <c r="G44" s="33"/>
       <c r="K44" s="7"/>
       <c r="N44" s="33"/>
@@ -3299,26 +3312,16 @@
       <c r="U44" s="24"/>
       <c r="AB44" s="7"/>
     </row>
-    <row r="45" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B45" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45" s="7">
-        <v>10</v>
-      </c>
-      <c r="D45" s="15">
-        <v>2</v>
-      </c>
-      <c r="E45" s="14">
-        <v>46352</v>
-      </c>
-      <c r="F45" s="9">
-        <f t="shared" ref="F45:F46" si="36">(E45-$AC$1)/365*12</f>
-        <v>21.830136986301369</v>
-      </c>
+    <row r="45" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="49">
+        <f>SUM(C43:C44)*30+D43</f>
+        <v>1599</v>
+      </c>
+      <c r="D45" s="50"/>
+      <c r="F45" s="7"/>
       <c r="G45" s="33"/>
       <c r="H45" s="6" t="s">
         <v>68</v>
@@ -3336,7 +3339,7 @@
         <v>46197</v>
       </c>
       <c r="M45" s="9">
-        <f t="shared" ref="M45:M46" si="37">(L45-$AC$1)/365*12</f>
+        <f t="shared" ref="M45:M46" si="36">(L45-$AC$1)/365*12</f>
         <v>16.734246575342464</v>
       </c>
       <c r="N45" s="33"/>
@@ -3350,23 +3353,9 @@
       <c r="AB45" s="7"/>
     </row>
     <row r="46" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="6"/>
-      <c r="B46" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="C46" s="11">
-        <v>55</v>
-      </c>
-      <c r="D46" s="15">
-        <v>5</v>
-      </c>
-      <c r="E46" s="14">
-        <v>46352</v>
-      </c>
-      <c r="F46" s="9">
-        <f t="shared" si="36"/>
-        <v>21.830136986301369</v>
-      </c>
+      <c r="B46" s="43"/>
+      <c r="D46" s="7"/>
+      <c r="F46" s="7"/>
       <c r="G46" s="33"/>
       <c r="I46" s="7">
         <v>162040</v>
@@ -3379,7 +3368,7 @@
         <v>46303</v>
       </c>
       <c r="M46" s="9">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>20.219178082191782</v>
       </c>
       <c r="N46" s="33"/>
@@ -3387,15 +3376,25 @@
       <c r="AB46" s="7"/>
     </row>
     <row r="47" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C47" s="49">
-        <f>SUM(C45:C46)*30+D45</f>
-        <v>1952</v>
-      </c>
-      <c r="D47" s="50"/>
-      <c r="F47" s="7"/>
+      <c r="A47" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="7">
+        <v>11</v>
+      </c>
+      <c r="D47" s="15">
+        <v>2</v>
+      </c>
+      <c r="E47" s="14">
+        <v>46352</v>
+      </c>
+      <c r="F47" s="9">
+        <f t="shared" ref="F47:F48" si="37">(E47-$AC$1)/365*12</f>
+        <v>21.830136986301369</v>
+      </c>
       <c r="G47" s="33"/>
       <c r="H47" s="36"/>
       <c r="I47" s="46" t="s">
@@ -3411,10 +3410,24 @@
       <c r="U47" s="24"/>
       <c r="AB47" s="7"/>
     </row>
-    <row r="48" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="43"/>
-      <c r="D48" s="7"/>
-      <c r="F48" s="7"/>
+    <row r="48" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="6"/>
+      <c r="B48" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="11">
+        <v>55</v>
+      </c>
+      <c r="D48" s="15">
+        <v>5</v>
+      </c>
+      <c r="E48" s="14">
+        <v>46352</v>
+      </c>
+      <c r="F48" s="9">
+        <f t="shared" si="37"/>
+        <v>21.830136986301369</v>
+      </c>
       <c r="G48" s="33"/>
       <c r="H48" s="24"/>
       <c r="K48" s="7"/>
@@ -3422,26 +3435,16 @@
       <c r="U48" s="24"/>
       <c r="AB48" s="7"/>
     </row>
-    <row r="49" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B49" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="C49" s="7">
-        <v>7</v>
-      </c>
-      <c r="D49" s="11">
-        <v>18</v>
-      </c>
-      <c r="E49" s="14">
-        <v>46260</v>
-      </c>
-      <c r="F49" s="9">
-        <f t="shared" ref="F49:F50" si="38">(E49-$AC$1)/365*12</f>
-        <v>18.805479452054794</v>
-      </c>
+    <row r="49" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="49">
+        <f>SUM(C47:C48)*30+D47</f>
+        <v>1982</v>
+      </c>
+      <c r="D49" s="50"/>
+      <c r="F49" s="7"/>
       <c r="G49" s="33"/>
       <c r="I49" s="11"/>
       <c r="J49" s="11"/>
@@ -3452,24 +3455,10 @@
       <c r="U49" s="24"/>
       <c r="AB49" s="7"/>
     </row>
-    <row r="50" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="6"/>
-      <c r="B50" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="C50" s="7">
-        <v>51</v>
-      </c>
-      <c r="D50" s="11">
-        <v>9</v>
-      </c>
-      <c r="E50" s="14">
-        <v>46291</v>
-      </c>
-      <c r="F50" s="9">
-        <f t="shared" si="38"/>
-        <v>19.824657534246576</v>
-      </c>
+    <row r="50" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="43"/>
+      <c r="D50" s="7"/>
+      <c r="F50" s="7"/>
       <c r="G50" s="33"/>
       <c r="I50" s="39"/>
       <c r="J50" s="52"/>
@@ -3480,26 +3469,50 @@
       <c r="U50" s="24"/>
       <c r="AB50" s="7"/>
     </row>
-    <row r="51" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" s="49" cm="1">
-        <f t="array" ref="C51">SUM(C49:C50*40)+D49+D50</f>
-        <v>2347</v>
-      </c>
-      <c r="D51" s="50"/>
-      <c r="F51" s="7"/>
+    <row r="51" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" s="7">
+        <v>16</v>
+      </c>
+      <c r="D51" s="11">
+        <v>18</v>
+      </c>
+      <c r="E51" s="14">
+        <v>46260</v>
+      </c>
+      <c r="F51" s="9">
+        <f t="shared" ref="F51:F52" si="38">(E51-$AC$1)/365*12</f>
+        <v>18.805479452054794</v>
+      </c>
       <c r="G51" s="33"/>
       <c r="K51" s="7"/>
       <c r="N51" s="24"/>
       <c r="U51" s="24"/>
       <c r="AB51" s="7"/>
     </row>
-    <row r="52" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="43"/>
-      <c r="D52" s="7"/>
-      <c r="F52" s="7"/>
+    <row r="52" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="6"/>
+      <c r="B52" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52" s="7">
+        <v>51</v>
+      </c>
+      <c r="D52" s="11">
+        <v>9</v>
+      </c>
+      <c r="E52" s="14">
+        <v>46291</v>
+      </c>
+      <c r="F52" s="9">
+        <f t="shared" si="38"/>
+        <v>19.824657534246576</v>
+      </c>
       <c r="G52" s="33"/>
       <c r="K52" s="7"/>
       <c r="N52" s="24"/>
@@ -3507,40 +3520,24 @@
       <c r="AB52" s="7"/>
     </row>
     <row r="53" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B53" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="C53" s="7">
-        <v>10</v>
-      </c>
-      <c r="D53" s="7">
-        <v>19</v>
-      </c>
-      <c r="E53" s="14">
-        <v>45528</v>
-      </c>
-      <c r="F53" s="16">
-        <f>(E53-$AC$1)/365*12</f>
-        <v>-5.2602739726027394</v>
-      </c>
+      <c r="B53" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="49" cm="1">
+        <f t="array" ref="C53">SUM(C51:C52*40)+D51+D52</f>
+        <v>2707</v>
+      </c>
+      <c r="D53" s="50"/>
+      <c r="F53" s="7"/>
       <c r="G53" s="33"/>
       <c r="K53" s="7"/>
       <c r="N53" s="24"/>
       <c r="U53" s="24"/>
       <c r="AB53" s="7"/>
     </row>
-    <row r="54" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C54" s="49">
-        <f>SUM(C53)*30+D53</f>
-        <v>319</v>
-      </c>
-      <c r="D54" s="50"/>
+    <row r="54" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="43"/>
+      <c r="D54" s="7"/>
       <c r="F54" s="7"/>
       <c r="G54" s="33"/>
       <c r="K54" s="7"/>
@@ -3549,16 +3546,40 @@
       <c r="U54" s="24"/>
       <c r="AB54" s="7"/>
     </row>
-    <row r="55" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="7"/>
-      <c r="F55" s="7"/>
+    <row r="55" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C55" s="7">
+        <v>10</v>
+      </c>
+      <c r="D55" s="7">
+        <v>19</v>
+      </c>
+      <c r="E55" s="14">
+        <v>45528</v>
+      </c>
+      <c r="F55" s="16">
+        <f>(E55-$AC$1)/365*12</f>
+        <v>-5.2602739726027394</v>
+      </c>
       <c r="G55" s="33"/>
       <c r="K55" s="7"/>
       <c r="U55" s="24"/>
       <c r="AB55" s="7"/>
     </row>
-    <row r="56" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D56" s="7"/>
+    <row r="56" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="49">
+        <f>SUM(C55)*30+D55</f>
+        <v>319</v>
+      </c>
+      <c r="D56" s="50"/>
       <c r="F56" s="7"/>
       <c r="G56" s="33"/>
       <c r="K56" s="7"/>
@@ -4483,8 +4504,22 @@
       <c r="E193" s="10"/>
       <c r="F193" s="7"/>
     </row>
-    <row r="194" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A194" s="10"/>
+      <c r="B194" s="10"/>
+      <c r="C194" s="10"/>
+      <c r="D194" s="7"/>
+      <c r="E194" s="10"/>
+      <c r="F194" s="7"/>
+    </row>
+    <row r="195" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A195" s="10"/>
+      <c r="B195" s="10"/>
+      <c r="C195" s="10"/>
+      <c r="D195" s="7"/>
+      <c r="E195" s="10"/>
+      <c r="F195" s="7"/>
+    </row>
     <row r="196" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="197" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="198" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4576,14 +4611,14 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="44">
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C53:D53"/>
     <mergeCell ref="J24:K24"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C41:D41"/>
     <mergeCell ref="J47:K47"/>
     <mergeCell ref="J50:K50"/>
     <mergeCell ref="J43:K43"/>
@@ -4591,14 +4626,14 @@
     <mergeCell ref="J31:K31"/>
     <mergeCell ref="J35:K35"/>
     <mergeCell ref="J39:K39"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C13:D13"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="Q41:R41"/>
     <mergeCell ref="Q6:R6"/>

</xml_diff>

<commit_message>
Update lot codes - 2025-02-04 15:06:34
</commit_message>
<xml_diff>
--- a/LotCode.xlsx
+++ b/LotCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf.sharepoint.com/sites/production-warehouse/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7358" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{123389CA-3E21-4FE2-8B90-DD3D15C779DF}"/>
+  <xr:revisionPtr revIDLastSave="7386" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FDAA322-A064-4705-9B85-9D94138E5318}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="a/VZ8kgdZMyU/a42HcB04O8OBNrnh4WxCIPRCv9GqcObOgYeM9oYcSfQqndR/nnirMykfzLaq88Ahwir6HajhQ==" workbookSaltValue="jsEDzk1n/+JkLoe+dWrmxg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
@@ -638,7 +638,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -776,6 +776,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1122,7 +1125,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,9 +1253,6 @@
       <c r="H2" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="K2" s="4">
-        <v>511</v>
-      </c>
       <c r="N2" s="32"/>
       <c r="O2" s="23" t="s">
         <v>95</v>
@@ -1275,7 +1275,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="7">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E3" s="41">
         <v>46304</v>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="C6" s="49">
         <f>SUM(C3:C5)*40+D3</f>
-        <v>6322</v>
+        <v>6340</v>
       </c>
       <c r="D6" s="50"/>
       <c r="F6" s="7"/>
@@ -1551,7 +1551,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="7">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" s="8">
         <v>46283</v>
@@ -1823,7 +1823,7 @@
       </c>
       <c r="C13" s="49">
         <f>SUM(C8:C12)*24+D8</f>
-        <v>2706</v>
+        <v>2704</v>
       </c>
       <c r="D13" s="50"/>
       <c r="F13" s="7"/>
@@ -1924,7 +1924,9 @@
       <c r="C15" s="7">
         <v>7</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="7">
+        <v>18</v>
+      </c>
       <c r="E15" s="8">
         <v>46283</v>
       </c>
@@ -2082,7 +2084,7 @@
       </c>
       <c r="C18" s="49">
         <f>SUM(C15:C17)*24+D15</f>
-        <v>5976</v>
+        <v>5994</v>
       </c>
       <c r="D18" s="50"/>
       <c r="F18" s="7"/>
@@ -2184,7 +2186,7 @@
         <v>5</v>
       </c>
       <c r="D20" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E20" s="8">
         <v>46283</v>
@@ -2338,7 +2340,7 @@
       </c>
       <c r="C23" s="49">
         <f>SUM(C20:C22)*12+D20</f>
-        <v>1920</v>
+        <v>1930</v>
       </c>
       <c r="D23" s="50"/>
       <c r="F23" s="7"/>
@@ -2406,7 +2408,9 @@
       <c r="C25" s="11">
         <v>5</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="7">
+        <v>38</v>
+      </c>
       <c r="E25" s="8">
         <v>46211</v>
       </c>
@@ -2469,7 +2473,9 @@
       <c r="C26" s="11">
         <v>119</v>
       </c>
-      <c r="D26" s="7"/>
+      <c r="D26" s="7">
+        <v>33</v>
+      </c>
       <c r="E26" s="8">
         <v>46211</v>
       </c>
@@ -2585,8 +2591,8 @@
         <v>8</v>
       </c>
       <c r="C28" s="49">
-        <f>SUM(C25:C27)*40+D25+D27</f>
-        <v>5320</v>
+        <f>SUM(C25:C27)*40+D25+D26</f>
+        <v>5391</v>
       </c>
       <c r="D28" s="50"/>
       <c r="F28" s="7"/>
@@ -2651,7 +2657,7 @@
         <v>8</v>
       </c>
       <c r="D30" s="7">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E30" s="8">
         <v>46211</v>
@@ -2802,7 +2808,7 @@
       </c>
       <c r="C33" s="49">
         <f>SUM(C30:C32)*24+D30</f>
-        <v>3432</v>
+        <v>3446</v>
       </c>
       <c r="D33" s="50"/>
       <c r="F33" s="7"/>
@@ -2914,7 +2920,7 @@
         <v>8</v>
       </c>
       <c r="D35" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E35" s="8">
         <v>46312</v>
@@ -2997,7 +3003,7 @@
       </c>
       <c r="C37" s="49">
         <f>SUM(C35:C36)*24+D35</f>
-        <v>2094</v>
+        <v>2095</v>
       </c>
       <c r="D37" s="50"/>
       <c r="F37" s="7"/>
@@ -3107,7 +3113,7 @@
         <v>7</v>
       </c>
       <c r="D39" s="7">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="E39" s="14">
         <v>46260</v>
@@ -3151,7 +3157,9 @@
       <c r="C40" s="40">
         <v>81</v>
       </c>
-      <c r="D40" s="7"/>
+      <c r="D40" s="7">
+        <v>22</v>
+      </c>
       <c r="E40" s="14">
         <v>46352</v>
       </c>
@@ -3189,8 +3197,8 @@
         <v>8</v>
       </c>
       <c r="C41" s="49">
-        <f>SUM(C39:C40)*30+D39</f>
-        <v>2646</v>
+        <f>SUM(C39:C40)*30+D39+D40</f>
+        <v>2689</v>
       </c>
       <c r="D41" s="50"/>
       <c r="F41" s="7"/>
@@ -3261,7 +3269,7 @@
         <v>5</v>
       </c>
       <c r="D43" s="7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E43" s="14">
         <v>46291</v>
@@ -3318,7 +3326,7 @@
       </c>
       <c r="C45" s="49">
         <f>SUM(C43:C44)*30+D43</f>
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="D45" s="50"/>
       <c r="F45" s="7"/>
@@ -3353,8 +3361,9 @@
       <c r="AB45" s="7"/>
     </row>
     <row r="46" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="43"/>
-      <c r="D46" s="7"/>
+      <c r="B46" s="47"/>
+      <c r="C46" s="55"/>
+      <c r="D46" s="55"/>
       <c r="F46" s="7"/>
       <c r="G46" s="33"/>
       <c r="I46" s="7">
@@ -3377,23 +3386,23 @@
     </row>
     <row r="47" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B47" s="44" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="B47" s="43" t="s">
+        <v>42</v>
       </c>
       <c r="C47" s="7">
-        <v>11</v>
-      </c>
-      <c r="D47" s="15">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="D47" s="11">
+        <v>3</v>
       </c>
       <c r="E47" s="14">
-        <v>46352</v>
+        <v>46260</v>
       </c>
       <c r="F47" s="9">
         <f t="shared" ref="F47:F48" si="37">(E47-$AC$1)/365*12</f>
-        <v>21.830136986301369</v>
+        <v>18.805479452054794</v>
       </c>
       <c r="G47" s="33"/>
       <c r="H47" s="36"/>
@@ -3412,21 +3421,21 @@
     </row>
     <row r="48" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6"/>
-      <c r="B48" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="C48" s="11">
-        <v>55</v>
-      </c>
-      <c r="D48" s="15">
-        <v>5</v>
+      <c r="B48" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" s="7">
+        <v>39</v>
+      </c>
+      <c r="D48" s="11">
+        <v>9</v>
       </c>
       <c r="E48" s="14">
-        <v>46352</v>
+        <v>46291</v>
       </c>
       <c r="F48" s="9">
         <f t="shared" si="37"/>
-        <v>21.830136986301369</v>
+        <v>19.824657534246576</v>
       </c>
       <c r="G48" s="33"/>
       <c r="H48" s="24"/>
@@ -3439,9 +3448,9 @@
       <c r="B49" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="49">
-        <f>SUM(C47:C48)*30+D47</f>
-        <v>1982</v>
+      <c r="C49" s="49" cm="1">
+        <f t="array" ref="C49">SUM(C47:C48*40)+D47+D48</f>
+        <v>2212</v>
       </c>
       <c r="D49" s="50"/>
       <c r="F49" s="7"/>
@@ -3471,23 +3480,23 @@
     </row>
     <row r="51" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B51" s="43" t="s">
-        <v>42</v>
+        <v>75</v>
+      </c>
+      <c r="B51" s="44" t="s">
+        <v>89</v>
       </c>
       <c r="C51" s="7">
-        <v>16</v>
-      </c>
-      <c r="D51" s="11">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="D51" s="15">
+        <v>29</v>
       </c>
       <c r="E51" s="14">
-        <v>46260</v>
+        <v>46352</v>
       </c>
       <c r="F51" s="9">
         <f t="shared" ref="F51:F52" si="38">(E51-$AC$1)/365*12</f>
-        <v>18.805479452054794</v>
+        <v>21.830136986301369</v>
       </c>
       <c r="G51" s="33"/>
       <c r="K51" s="7"/>
@@ -3497,21 +3506,19 @@
     </row>
     <row r="52" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="6"/>
-      <c r="B52" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="C52" s="7">
-        <v>51</v>
-      </c>
-      <c r="D52" s="11">
-        <v>9</v>
-      </c>
+      <c r="B52" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="11">
+        <v>34</v>
+      </c>
+      <c r="D52" s="15"/>
       <c r="E52" s="14">
-        <v>46291</v>
+        <v>46352</v>
       </c>
       <c r="F52" s="9">
         <f t="shared" si="38"/>
-        <v>19.824657534246576</v>
+        <v>21.830136986301369</v>
       </c>
       <c r="G52" s="33"/>
       <c r="K52" s="7"/>
@@ -3523,9 +3530,9 @@
       <c r="B53" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C53" s="49" cm="1">
-        <f t="array" ref="C53">SUM(C51:C52*40)+D51+D52</f>
-        <v>2707</v>
+      <c r="C53" s="49">
+        <f>SUM(C51:C52)*30+D51</f>
+        <v>1349</v>
       </c>
       <c r="D53" s="50"/>
       <c r="F53" s="7"/>
@@ -3546,48 +3553,49 @@
       <c r="U54" s="24"/>
       <c r="AB54" s="7"/>
     </row>
-    <row r="55" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B55" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="C55" s="7">
-        <v>10</v>
-      </c>
-      <c r="D55" s="7">
-        <v>19</v>
-      </c>
-      <c r="E55" s="14">
-        <v>45528</v>
-      </c>
-      <c r="F55" s="16">
-        <f>(E55-$AC$1)/365*12</f>
-        <v>-5.2602739726027394</v>
-      </c>
+    <row r="55" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="43"/>
+      <c r="D55" s="7"/>
+      <c r="F55" s="7"/>
       <c r="G55" s="33"/>
       <c r="K55" s="7"/>
       <c r="U55" s="24"/>
       <c r="AB55" s="7"/>
     </row>
     <row r="56" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C56" s="49">
-        <f>SUM(C55)*30+D55</f>
-        <v>319</v>
-      </c>
-      <c r="D56" s="50"/>
-      <c r="F56" s="7"/>
+      <c r="A56" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B56" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C56" s="7">
+        <v>10</v>
+      </c>
+      <c r="D56" s="7">
+        <v>19</v>
+      </c>
+      <c r="E56" s="14">
+        <v>45528</v>
+      </c>
+      <c r="F56" s="16">
+        <f>(E56-$AC$1)/365*12</f>
+        <v>-5.2602739726027394</v>
+      </c>
       <c r="G56" s="33"/>
       <c r="K56" s="7"/>
       <c r="U56" s="24"/>
       <c r="AB56" s="7"/>
     </row>
-    <row r="57" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D57" s="7"/>
+    <row r="57" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="49">
+        <f>SUM(C56)*30+D56</f>
+        <v>319</v>
+      </c>
+      <c r="D57" s="50"/>
       <c r="F57" s="7"/>
       <c r="G57" s="33"/>
       <c r="K57" s="7"/>
@@ -4520,7 +4528,14 @@
       <c r="E195" s="10"/>
       <c r="F195" s="7"/>
     </row>
-    <row r="196" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="10"/>
+      <c r="B196" s="10"/>
+      <c r="C196" s="10"/>
+      <c r="D196" s="7"/>
+      <c r="E196" s="10"/>
+      <c r="F196" s="7"/>
+    </row>
     <row r="197" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="198" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="199" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4612,9 +4627,8 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="44">
     <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C56:D56"/>
     <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C57:D57"/>
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C37:D37"/>
@@ -4626,6 +4640,7 @@
     <mergeCell ref="J31:K31"/>
     <mergeCell ref="J35:K35"/>
     <mergeCell ref="J39:K39"/>
+    <mergeCell ref="C49:D49"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C28:D28"/>

</xml_diff>

<commit_message>
Update lot codes - 2025-02-04 16:06:57
</commit_message>
<xml_diff>
--- a/LotCode.xlsx
+++ b/LotCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf.sharepoint.com/sites/production-warehouse/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7386" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FDAA322-A064-4705-9B85-9D94138E5318}"/>
+  <xr:revisionPtr revIDLastSave="7387" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BEECE44-9877-43EA-8D7A-852972A19E28}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="a/VZ8kgdZMyU/a42HcB04O8OBNrnh4WxCIPRCv9GqcObOgYeM9oYcSfQqndR/nnirMykfzLaq88Ahwir6HajhQ==" workbookSaltValue="jsEDzk1n/+JkLoe+dWrmxg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
@@ -1125,7 +1125,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1703,7 +1703,6 @@
       <c r="AB10" s="7"/>
     </row>
     <row r="11" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="27"/>
       <c r="B11" s="7">
         <v>162036</v>
       </c>
@@ -1875,6 +1874,7 @@
       <c r="AB13" s="7"/>
     </row>
     <row r="14" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="27"/>
       <c r="D14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="33"/>

</xml_diff>

<commit_message>
Update lot codes - 2025-02-05 15:37:04
</commit_message>
<xml_diff>
--- a/LotCode.xlsx
+++ b/LotCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf.sharepoint.com/sites/production-warehouse/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7387" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BEECE44-9877-43EA-8D7A-852972A19E28}"/>
+  <xr:revisionPtr revIDLastSave="7391" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C08F98E8-F48F-4C7E-9605-6D7F0A4F5EAF}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="a/VZ8kgdZMyU/a42HcB04O8OBNrnh4WxCIPRCv9GqcObOgYeM9oYcSfQqndR/nnirMykfzLaq88Ahwir6HajhQ==" workbookSaltValue="jsEDzk1n/+JkLoe+dWrmxg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
@@ -638,7 +638,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -760,26 +760,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1125,7 +1122,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,7 +1344,7 @@
       <c r="AB3" s="12"/>
     </row>
     <row r="4" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="53"/>
+      <c r="A4" s="49"/>
       <c r="B4" s="40">
         <v>163236</v>
       </c>
@@ -1431,11 +1428,11 @@
       <c r="I5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="49">
+      <c r="J5" s="51">
         <f>SUM(J3:J4)*40+K3</f>
         <v>4336</v>
       </c>
-      <c r="K5" s="50"/>
+      <c r="K5" s="52"/>
       <c r="N5" s="33"/>
       <c r="O5" s="27"/>
       <c r="P5" s="7" t="s">
@@ -1458,22 +1455,22 @@
       <c r="W5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X5" s="49">
+      <c r="X5" s="51">
         <f>SUM(X3:X4)*6+Y3+Y4</f>
         <v>1122</v>
       </c>
-      <c r="Y5" s="50"/>
+      <c r="Y5" s="52"/>
       <c r="AB5" s="7"/>
     </row>
     <row r="6" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="51">
         <f>SUM(C3:C5)*40+D3</f>
         <v>6340</v>
       </c>
-      <c r="D6" s="50"/>
+      <c r="D6" s="52"/>
       <c r="F6" s="7"/>
       <c r="G6" s="33"/>
       <c r="K6" s="7"/>
@@ -1481,11 +1478,11 @@
       <c r="P6" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q6" s="49">
+      <c r="Q6" s="51">
         <f>SUM(Q3:Q5)*30+R3+R5</f>
         <v>7809</v>
       </c>
-      <c r="R6" s="50"/>
+      <c r="R6" s="52"/>
       <c r="U6" s="33"/>
       <c r="V6" s="10" t="s">
         <v>10</v>
@@ -1557,7 +1554,7 @@
         <v>46283</v>
       </c>
       <c r="F8" s="9">
-        <f t="shared" ref="F8:F9" si="7">(E8-$AC$1)/365*12</f>
+        <f t="shared" ref="F8:F10" si="7">(E8-$AC$1)/365*12</f>
         <v>19.56164383561644</v>
       </c>
       <c r="G8" s="33"/>
@@ -1618,28 +1615,25 @@
     <row r="9" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="36"/>
       <c r="B9" s="7">
-        <v>159367</v>
-      </c>
-      <c r="C9" s="7">
-        <v>22</v>
-      </c>
-      <c r="D9" s="7"/>
+        <v>158583</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7">
+        <v>4</v>
+      </c>
       <c r="E9" s="8">
-        <v>46283</v>
-      </c>
-      <c r="F9" s="9">
-        <f t="shared" si="7"/>
-        <v>19.56164383561644</v>
-      </c>
+        <v>46250</v>
+      </c>
+      <c r="F9" s="9"/>
       <c r="G9" s="33"/>
       <c r="I9" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="49">
+      <c r="J9" s="51">
         <f>SUM(J7:J8)*24+K7</f>
         <v>3634</v>
       </c>
-      <c r="K9" s="50"/>
+      <c r="K9" s="52"/>
       <c r="N9" s="33"/>
       <c r="P9" s="7" t="s">
         <v>48</v>
@@ -1659,28 +1653,28 @@
       <c r="W9" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X9" s="49">
+      <c r="X9" s="51">
         <f>SUM(X7:X8)*6+Y7+Y8</f>
         <v>412</v>
       </c>
-      <c r="Y9" s="50"/>
+      <c r="Y9" s="52"/>
       <c r="AB9" s="7"/>
     </row>
     <row r="10" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="27"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="7">
-        <v>161798</v>
-      </c>
-      <c r="C10" s="11">
-        <v>60</v>
+        <v>159367</v>
+      </c>
+      <c r="C10" s="7">
+        <v>22</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="8">
-        <v>46324</v>
+        <v>46283</v>
       </c>
       <c r="F10" s="9">
-        <f t="shared" ref="F10:F12" si="10">(E10-$AC$1)/365*12</f>
-        <v>20.909589041095892</v>
+        <f t="shared" si="7"/>
+        <v>19.56164383561644</v>
       </c>
       <c r="G10" s="33"/>
       <c r="K10" s="7"/>
@@ -1703,19 +1697,20 @@
       <c r="AB10" s="7"/>
     </row>
     <row r="11" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="27"/>
       <c r="B11" s="7">
-        <v>162036</v>
+        <v>161798</v>
       </c>
       <c r="C11" s="11">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="8">
-        <v>46337</v>
+        <v>46324</v>
       </c>
       <c r="F11" s="9">
-        <f t="shared" si="10"/>
-        <v>21.336986301369862</v>
+        <f t="shared" ref="F11:F13" si="10">(E11-$AC$1)/365*12</f>
+        <v>20.909589041095892</v>
       </c>
       <c r="G11" s="33"/>
       <c r="H11" s="6" t="s">
@@ -1739,11 +1734,11 @@
       <c r="P11" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q11" s="49">
+      <c r="Q11" s="51">
         <f>SUM(Q8:Q10)*30+R8</f>
         <v>6337</v>
       </c>
-      <c r="R11" s="50"/>
+      <c r="R11" s="52"/>
       <c r="U11" s="33"/>
       <c r="V11" s="6" t="s">
         <v>90</v>
@@ -1767,20 +1762,19 @@
       <c r="AB11" s="7"/>
     </row>
     <row r="12" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="27"/>
       <c r="B12" s="7">
-        <v>162037</v>
+        <v>162036</v>
       </c>
       <c r="C12" s="11">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="8">
-        <v>46359</v>
+        <v>46337</v>
       </c>
       <c r="F12" s="9">
         <f t="shared" si="10"/>
-        <v>22.06027397260274</v>
+        <v>21.336986301369862</v>
       </c>
       <c r="G12" s="33"/>
       <c r="H12" s="27"/>
@@ -1817,15 +1811,21 @@
       <c r="AB12" s="7"/>
     </row>
     <row r="13" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="49">
-        <f>SUM(C8:C12)*24+D8</f>
-        <v>2704</v>
-      </c>
-      <c r="D13" s="50"/>
-      <c r="F13" s="7"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="7">
+        <v>162037</v>
+      </c>
+      <c r="C13" s="11">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8">
+        <v>46359</v>
+      </c>
+      <c r="F13" s="9">
+        <f t="shared" si="10"/>
+        <v>22.06027397260274</v>
+      </c>
       <c r="G13" s="33"/>
       <c r="H13" s="27"/>
       <c r="I13" s="7">
@@ -1866,16 +1866,22 @@
       <c r="W13" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X13" s="49">
+      <c r="X13" s="51">
         <f>SUM(X11:X12)*6+Y11+Y12</f>
         <v>1240</v>
       </c>
-      <c r="Y13" s="50"/>
+      <c r="Y13" s="52"/>
       <c r="AB13" s="7"/>
     </row>
     <row r="14" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="27"/>
-      <c r="D14" s="7"/>
+      <c r="B14" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="51">
+        <f>SUM(C8:C13)*24+D8</f>
+        <v>2704</v>
+      </c>
+      <c r="D14" s="52"/>
       <c r="F14" s="7"/>
       <c r="G14" s="33"/>
       <c r="H14" s="27"/>
@@ -1915,43 +1921,27 @@
       <c r="AB14" s="7"/>
     </row>
     <row r="15" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="35">
-        <v>159366</v>
-      </c>
-      <c r="C15" s="7">
-        <v>7</v>
-      </c>
-      <c r="D15" s="7">
-        <v>18</v>
-      </c>
-      <c r="E15" s="8">
-        <v>46283</v>
-      </c>
-      <c r="F15" s="9">
-        <f>(E15-$AC$1)/365*12</f>
-        <v>19.56164383561644</v>
-      </c>
+      <c r="B15" s="27"/>
+      <c r="D15" s="7"/>
+      <c r="F15" s="7"/>
       <c r="G15" s="33"/>
       <c r="I15" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J15" s="49">
+      <c r="J15" s="51">
         <f>SUM(J11:J14)*24+K11</f>
         <v>5520</v>
       </c>
-      <c r="K15" s="50"/>
+      <c r="K15" s="52"/>
       <c r="N15" s="33"/>
       <c r="P15" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q15" s="49">
+      <c r="Q15" s="51">
         <f>SUM(Q13:Q14)*30+R13+R14</f>
         <v>3879</v>
       </c>
-      <c r="R15" s="50"/>
+      <c r="R15" s="52"/>
       <c r="U15" s="33"/>
       <c r="V15" s="6" t="s">
         <v>71</v>
@@ -1975,19 +1965,24 @@
       <c r="AB15" s="7"/>
     </row>
     <row r="16" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="B16" s="35">
-        <v>161793</v>
-      </c>
-      <c r="C16" s="11">
-        <v>68</v>
-      </c>
-      <c r="D16" s="7"/>
+        <v>159366</v>
+      </c>
+      <c r="C16" s="7">
+        <v>7</v>
+      </c>
+      <c r="D16" s="7">
+        <v>18</v>
+      </c>
       <c r="E16" s="8">
-        <v>46313</v>
+        <v>46283</v>
       </c>
       <c r="F16" s="9">
-        <f t="shared" ref="F16" si="14">(E16-$AC$1)/365*12</f>
-        <v>20.547945205479451</v>
+        <f>(E16-$AC$1)/365*12</f>
+        <v>19.56164383561644</v>
       </c>
       <c r="G16" s="33"/>
       <c r="K16" s="7"/>
@@ -2014,18 +2009,18 @@
     </row>
     <row r="17" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="35">
-        <v>161794</v>
+        <v>161793</v>
       </c>
       <c r="C17" s="11">
-        <v>174</v>
+        <v>68</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="8">
-        <v>46324</v>
+        <v>46313</v>
       </c>
       <c r="F17" s="9">
-        <f t="shared" ref="F17" si="15">(E17-$AC$1)/365*12</f>
-        <v>20.909589041095892</v>
+        <f t="shared" ref="F17" si="14">(E17-$AC$1)/365*12</f>
+        <v>20.547945205479451</v>
       </c>
       <c r="G17" s="33"/>
       <c r="H17" s="6" t="s">
@@ -2044,7 +2039,7 @@
         <v>46310</v>
       </c>
       <c r="M17" s="9">
-        <f t="shared" ref="M17:M19" si="16">(L17-$AC$1)/365*12</f>
+        <f t="shared" ref="M17:M19" si="15">(L17-$AC$1)/365*12</f>
         <v>20.449315068493153</v>
       </c>
       <c r="N17" s="33"/>
@@ -2064,30 +2059,35 @@
         <v>46199</v>
       </c>
       <c r="T17" s="9">
-        <f t="shared" ref="T17" si="17">(S17-$AC$1)/365*12</f>
+        <f t="shared" ref="T17" si="16">(S17-$AC$1)/365*12</f>
         <v>16.799999999999997</v>
       </c>
       <c r="U17" s="33"/>
       <c r="W17" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X17" s="49">
+      <c r="X17" s="51">
         <f>SUM(X15:X16)*6+Y15+Y16</f>
         <v>517</v>
       </c>
-      <c r="Y17" s="50"/>
+      <c r="Y17" s="52"/>
       <c r="AB17" s="7"/>
     </row>
     <row r="18" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="49">
-        <f>SUM(C15:C17)*24+D15</f>
-        <v>5994</v>
-      </c>
-      <c r="D18" s="50"/>
-      <c r="F18" s="7"/>
+      <c r="B18" s="35">
+        <v>161794</v>
+      </c>
+      <c r="C18" s="11">
+        <v>174</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8">
+        <v>46324</v>
+      </c>
+      <c r="F18" s="9">
+        <f t="shared" ref="F18" si="17">(E18-$AC$1)/365*12</f>
+        <v>20.909589041095892</v>
+      </c>
       <c r="G18" s="33"/>
       <c r="H18" s="6"/>
       <c r="I18" s="7">
@@ -2101,7 +2101,7 @@
         <v>46325</v>
       </c>
       <c r="M18" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>20.942465753424656</v>
       </c>
       <c r="N18" s="33"/>
@@ -2125,8 +2125,14 @@
       <c r="AB18" s="7"/>
     </row>
     <row r="19" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="43"/>
-      <c r="D19" s="7"/>
+      <c r="B19" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="51">
+        <f>SUM(C16:C18)*24+D16</f>
+        <v>5994</v>
+      </c>
+      <c r="D19" s="52"/>
       <c r="F19" s="7"/>
       <c r="G19" s="33"/>
       <c r="H19" s="6"/>
@@ -2141,18 +2147,18 @@
         <v>46361</v>
       </c>
       <c r="M19" s="9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>22.126027397260273</v>
       </c>
       <c r="N19" s="33"/>
       <c r="P19" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q19" s="49">
+      <c r="Q19" s="51">
         <f>SUM(Q17:Q18)*30+R17+R18</f>
         <v>1385</v>
       </c>
-      <c r="R19" s="50"/>
+      <c r="R19" s="52"/>
       <c r="U19" s="33"/>
       <c r="V19" s="6" t="s">
         <v>20</v>
@@ -2176,34 +2182,18 @@
       <c r="AB19" s="7"/>
     </row>
     <row r="20" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="44" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" s="11">
-        <v>5</v>
-      </c>
-      <c r="D20" s="7">
-        <v>10</v>
-      </c>
-      <c r="E20" s="8">
-        <v>46283</v>
-      </c>
-      <c r="F20" s="9">
-        <f t="shared" ref="F20" si="19">(E20-$AC$1)/365*12</f>
-        <v>19.56164383561644</v>
-      </c>
+      <c r="B20" s="43"/>
+      <c r="D20" s="7"/>
+      <c r="F20" s="7"/>
       <c r="G20" s="33"/>
       <c r="I20" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J20" s="49">
+      <c r="J20" s="51">
         <f>SUM(J17:J19)*12+K17</f>
         <v>2455</v>
       </c>
-      <c r="K20" s="50"/>
+      <c r="K20" s="52"/>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
       <c r="N20" s="33"/>
@@ -2215,26 +2205,31 @@
       <c r="W20" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X20" s="49">
+      <c r="X20" s="51">
         <f>SUM(X19*200)+Y19</f>
         <v>1118</v>
       </c>
-      <c r="Y20" s="50"/>
+      <c r="Y20" s="52"/>
       <c r="AB20" s="7"/>
     </row>
     <row r="21" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="27"/>
+      <c r="A21" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="B21" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="7">
-        <v>54</v>
+      <c r="C21" s="11">
+        <v>5</v>
+      </c>
+      <c r="D21" s="7">
+        <v>10</v>
       </c>
       <c r="E21" s="8">
         <v>46283</v>
       </c>
       <c r="F21" s="9">
-        <f t="shared" ref="F21:F22" si="20">(E21-$AC$1)/365*12</f>
+        <f t="shared" ref="F21" si="19">(E21-$AC$1)/365*12</f>
         <v>19.56164383561644</v>
       </c>
       <c r="G21" s="33"/>
@@ -2256,7 +2251,7 @@
         <v>46291</v>
       </c>
       <c r="T21" s="9">
-        <f t="shared" ref="T21:T22" si="21">(S21-$AC$1)/365*12</f>
+        <f t="shared" ref="T21:T22" si="20">(S21-$AC$1)/365*12</f>
         <v>19.824657534246576</v>
       </c>
       <c r="U21" s="33"/>
@@ -2265,17 +2260,17 @@
     <row r="22" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="27"/>
       <c r="B22" s="44" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C22" s="7">
-        <v>101</v>
+        <v>54</v>
       </c>
       <c r="E22" s="8">
-        <v>46303</v>
+        <v>46283</v>
       </c>
       <c r="F22" s="9">
-        <f t="shared" si="20"/>
-        <v>20.219178082191782</v>
+        <f t="shared" ref="F22:F23" si="21">(E22-$AC$1)/365*12</f>
+        <v>19.56164383561644</v>
       </c>
       <c r="G22" s="33"/>
       <c r="H22" s="6" t="s">
@@ -2309,7 +2304,7 @@
         <v>46291</v>
       </c>
       <c r="T22" s="9">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>19.824657534246576</v>
       </c>
       <c r="U22" s="33"/>
@@ -2335,15 +2330,20 @@
       <c r="AB22" s="7"/>
     </row>
     <row r="23" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="49">
-        <f>SUM(C20:C22)*12+D20</f>
-        <v>1930</v>
-      </c>
-      <c r="D23" s="50"/>
-      <c r="F23" s="7"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="7">
+        <v>101</v>
+      </c>
+      <c r="E23" s="8">
+        <v>46303</v>
+      </c>
+      <c r="F23" s="9">
+        <f t="shared" si="21"/>
+        <v>20.219178082191782</v>
+      </c>
       <c r="G23" s="33"/>
       <c r="I23" s="7" t="s">
         <v>87</v>
@@ -2365,59 +2365,49 @@
       <c r="P23" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q23" s="49">
+      <c r="Q23" s="51">
         <f>SUM(Q21:Q22)*30+R21</f>
         <v>1841</v>
       </c>
-      <c r="R23" s="50"/>
+      <c r="R23" s="52"/>
       <c r="U23" s="33"/>
       <c r="W23" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X23" s="49">
+      <c r="X23" s="51">
         <f>SUM(X22*200)+Y22</f>
         <v>780</v>
       </c>
-      <c r="Y23" s="50"/>
+      <c r="Y23" s="52"/>
       <c r="AB23" s="7"/>
     </row>
     <row r="24" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="43"/>
-      <c r="D24" s="7"/>
+      <c r="B24" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="51">
+        <f>SUM(C21:C23)*12+D21</f>
+        <v>1930</v>
+      </c>
+      <c r="D24" s="52"/>
       <c r="F24" s="7"/>
       <c r="G24" s="33"/>
       <c r="I24" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J24" s="49">
+      <c r="J24" s="51">
         <f>SUM(J22:J23)*30+K22+K23</f>
         <v>2722</v>
       </c>
-      <c r="K24" s="50"/>
+      <c r="K24" s="52"/>
       <c r="N24" s="33"/>
       <c r="U24" s="33"/>
       <c r="AB24" s="7"/>
     </row>
     <row r="25" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25" s="11">
-        <v>5</v>
-      </c>
-      <c r="D25" s="7">
-        <v>38</v>
-      </c>
-      <c r="E25" s="8">
-        <v>46211</v>
-      </c>
-      <c r="F25" s="9">
-        <f>(E25-$AC$1)/365*12</f>
-        <v>17.194520547945206</v>
-      </c>
+      <c r="B25" s="43"/>
+      <c r="D25" s="7"/>
+      <c r="F25" s="7"/>
       <c r="G25" s="33"/>
       <c r="K25" s="7"/>
       <c r="M25" s="10" t="s">
@@ -2444,7 +2434,7 @@
         <v>16.799999999999997</v>
       </c>
       <c r="U25" s="33"/>
-      <c r="V25" s="51" t="s">
+      <c r="V25" s="54" t="s">
         <v>73</v>
       </c>
       <c r="W25" s="7" t="s">
@@ -2466,20 +2456,25 @@
       <c r="AB25" s="7"/>
     </row>
     <row r="26" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="6"/>
+      <c r="A26" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="B26" s="45" t="s">
         <v>103</v>
       </c>
       <c r="C26" s="11">
-        <v>119</v>
+        <v>5</v>
       </c>
       <c r="D26" s="7">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E26" s="8">
         <v>46211</v>
       </c>
-      <c r="F26" s="9"/>
+      <c r="F26" s="9">
+        <f>(E26-$AC$1)/365*12</f>
+        <v>17.194520547945206</v>
+      </c>
       <c r="G26" s="33"/>
       <c r="H26" s="6" t="s">
         <v>23</v>
@@ -2518,7 +2513,7 @@
         <v>16.799999999999997</v>
       </c>
       <c r="U26" s="33"/>
-      <c r="V26" s="51"/>
+      <c r="V26" s="54"/>
       <c r="W26" s="7"/>
       <c r="X26" s="7"/>
       <c r="Y26" s="7"/>
@@ -2527,21 +2522,20 @@
       <c r="AB26" s="7"/>
     </row>
     <row r="27" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="29"/>
+      <c r="A27" s="6"/>
       <c r="B27" s="45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C27" s="11">
-        <v>9</v>
-      </c>
-      <c r="D27" s="7"/>
+        <v>119</v>
+      </c>
+      <c r="D27" s="7">
+        <v>33</v>
+      </c>
       <c r="E27" s="8">
-        <v>46302</v>
-      </c>
-      <c r="F27" s="9">
-        <f>(E27-$AC$1)/365*12</f>
-        <v>20.186301369863013</v>
-      </c>
+        <v>46211</v>
+      </c>
+      <c r="F27" s="9"/>
       <c r="G27" s="33"/>
       <c r="I27" s="7" t="s">
         <v>88</v>
@@ -2579,47 +2573,59 @@
       <c r="W27" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X27" s="49">
+      <c r="X27" s="51">
         <f>SUM(X25:X26)*4+Y25+Y26</f>
         <v>174</v>
       </c>
-      <c r="Y27" s="50"/>
+      <c r="Y27" s="52"/>
       <c r="AB27" s="7"/>
     </row>
     <row r="28" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="49">
-        <f>SUM(C25:C27)*40+D25+D26</f>
-        <v>5391</v>
-      </c>
-      <c r="D28" s="50"/>
-      <c r="F28" s="7"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="11">
+        <v>9</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="8">
+        <v>46302</v>
+      </c>
+      <c r="F28" s="9">
+        <f>(E28-$AC$1)/365*12</f>
+        <v>20.186301369863013</v>
+      </c>
       <c r="G28" s="33"/>
       <c r="I28" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J28" s="49">
+      <c r="J28" s="51">
         <f>SUM(J26:J27)*30+K26</f>
         <v>2292</v>
       </c>
-      <c r="K28" s="50"/>
+      <c r="K28" s="52"/>
       <c r="N28" s="33"/>
       <c r="P28" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q28" s="49">
+      <c r="Q28" s="51">
         <f>SUM(Q25:Q27)*30+R25+R26+R27</f>
         <v>2418</v>
       </c>
-      <c r="R28" s="50"/>
+      <c r="R28" s="52"/>
       <c r="U28" s="33"/>
       <c r="AB28" s="7"/>
     </row>
-    <row r="29" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="43"/>
-      <c r="D29" s="7"/>
+    <row r="29" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="51">
+        <f>SUM(C26:C28)*40+D26+D27</f>
+        <v>5391</v>
+      </c>
+      <c r="D29" s="52"/>
       <c r="F29" s="7"/>
       <c r="G29" s="33"/>
       <c r="K29" s="7"/>
@@ -2647,25 +2653,9 @@
       <c r="AB29" s="8"/>
     </row>
     <row r="30" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="7">
-        <v>8</v>
-      </c>
-      <c r="D30" s="7">
-        <v>14</v>
-      </c>
-      <c r="E30" s="8">
-        <v>46211</v>
-      </c>
-      <c r="F30" s="9">
-        <f>(E30-$AC$1)/365*12</f>
-        <v>17.194520547945206</v>
-      </c>
+      <c r="B30" s="43"/>
+      <c r="D30" s="7"/>
+      <c r="F30" s="7"/>
       <c r="G30" s="33"/>
       <c r="H30" s="6" t="s">
         <v>29</v>
@@ -2723,13 +2713,18 @@
       </c>
     </row>
     <row r="31" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="B31" s="44" t="s">
         <v>53</v>
       </c>
       <c r="C31" s="7">
-        <v>55</v>
-      </c>
-      <c r="D31" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="D31" s="7">
+        <v>14</v>
+      </c>
       <c r="E31" s="8">
         <v>46211</v>
       </c>
@@ -2741,11 +2736,11 @@
       <c r="I31" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J31" s="49">
+      <c r="J31" s="51">
         <f>SUM(J30)*30+K30</f>
         <v>234</v>
       </c>
-      <c r="K31" s="50"/>
+      <c r="K31" s="52"/>
       <c r="N31" s="33"/>
       <c r="O31" s="6"/>
       <c r="P31" s="7" t="s">
@@ -2766,27 +2761,27 @@
       <c r="W31" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X31" s="49">
+      <c r="X31" s="51">
         <f>SUM(X29:X30)*30+Y29</f>
         <v>1270</v>
       </c>
-      <c r="Y31" s="50"/>
+      <c r="Y31" s="52"/>
       <c r="AB31" s="7"/>
     </row>
     <row r="32" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="44" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="C32" s="7">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="8">
-        <v>46248</v>
+        <v>46211</v>
       </c>
       <c r="F32" s="9">
         <f>(E32-$AC$1)/365*12</f>
-        <v>18.410958904109588</v>
+        <v>17.194520547945206</v>
       </c>
       <c r="G32" s="33"/>
       <c r="K32" s="7"/>
@@ -2794,24 +2789,29 @@
       <c r="P32" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q32" s="49">
+      <c r="Q32" s="51">
         <f>SUM(Q30:Q31)*30+R30</f>
         <v>609</v>
       </c>
-      <c r="R32" s="50"/>
+      <c r="R32" s="52"/>
       <c r="U32" s="33"/>
       <c r="AB32" s="7"/>
     </row>
     <row r="33" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="49">
-        <f>SUM(C30:C32)*24+D30</f>
-        <v>3446</v>
-      </c>
-      <c r="D33" s="50"/>
-      <c r="F33" s="7"/>
+      <c r="B33" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="7">
+        <v>80</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="8">
+        <v>46248</v>
+      </c>
+      <c r="F33" s="9">
+        <f>(E33-$AC$1)/365*12</f>
+        <v>18.410958904109588</v>
+      </c>
       <c r="G33" s="33"/>
       <c r="H33" s="17" t="s">
         <v>65</v>
@@ -2856,8 +2856,14 @@
       <c r="AB33" s="7"/>
     </row>
     <row r="34" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="43"/>
-      <c r="D34" s="7"/>
+      <c r="B34" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="51">
+        <f>SUM(C31:C33)*24+D31</f>
+        <v>3446</v>
+      </c>
+      <c r="D34" s="52"/>
       <c r="F34" s="7"/>
       <c r="G34" s="33"/>
       <c r="I34" s="7">
@@ -2910,34 +2916,18 @@
       <c r="AB34" s="7"/>
     </row>
     <row r="35" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="C35" s="7">
-        <v>8</v>
-      </c>
-      <c r="D35" s="7">
-        <v>7</v>
-      </c>
-      <c r="E35" s="8">
-        <v>46312</v>
-      </c>
-      <c r="F35" s="9">
-        <f>(E35-$AC$1)/365*12</f>
-        <v>20.515068493150686</v>
-      </c>
+      <c r="B35" s="43"/>
+      <c r="D35" s="7"/>
+      <c r="F35" s="7"/>
       <c r="G35" s="33"/>
       <c r="I35" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J35" s="49">
+      <c r="J35" s="51">
         <f>SUM(J33:J34)*24+K33</f>
         <v>1129</v>
       </c>
-      <c r="K35" s="50"/>
+      <c r="K35" s="52"/>
       <c r="N35" s="33"/>
       <c r="O35" s="6"/>
       <c r="P35" s="7" t="s">
@@ -2958,22 +2948,26 @@
       <c r="W35" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X35" s="49">
+      <c r="X35" s="51">
         <f>SUM(X33:X34)*18+Y33</f>
         <v>1175</v>
       </c>
-      <c r="Y35" s="50"/>
+      <c r="Y35" s="52"/>
       <c r="AB35" s="7"/>
     </row>
     <row r="36" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="27"/>
+      <c r="A36" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="B36" s="44" t="s">
         <v>86</v>
       </c>
       <c r="C36" s="7">
-        <v>79</v>
-      </c>
-      <c r="D36" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="D36" s="7">
+        <v>7</v>
+      </c>
       <c r="E36" s="8">
         <v>46312</v>
       </c>
@@ -2987,26 +2981,32 @@
       <c r="P36" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q36" s="49">
+      <c r="Q36" s="51">
         <f>SUM(Q34:Q35)*30+R34</f>
         <v>828</v>
       </c>
-      <c r="R36" s="50"/>
+      <c r="R36" s="52"/>
       <c r="S36" s="7"/>
       <c r="T36" s="7"/>
       <c r="U36" s="33"/>
       <c r="AB36" s="7"/>
     </row>
     <row r="37" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="49">
-        <f>SUM(C35:C36)*24+D35</f>
-        <v>2095</v>
-      </c>
-      <c r="D37" s="50"/>
-      <c r="F37" s="7"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="7">
+        <v>79</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="8">
+        <v>46312</v>
+      </c>
+      <c r="F37" s="9">
+        <f>(E37-$AC$1)/365*12</f>
+        <v>20.515068493150686</v>
+      </c>
       <c r="G37" s="33"/>
       <c r="H37" s="6" t="s">
         <v>66</v>
@@ -3053,8 +3053,14 @@
       <c r="AB37" s="7"/>
     </row>
     <row r="38" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="43"/>
-      <c r="D38" s="7"/>
+      <c r="B38" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="51">
+        <f>SUM(C36:C37)*24+D36</f>
+        <v>2095</v>
+      </c>
+      <c r="D38" s="52"/>
       <c r="F38" s="7"/>
       <c r="G38" s="33"/>
       <c r="I38" s="7">
@@ -3095,42 +3101,26 @@
       <c r="W38" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X38" s="49">
+      <c r="X38" s="51">
         <f>SUM(X37:X37)*18+Y37</f>
         <v>2</v>
       </c>
-      <c r="Y38" s="50"/>
+      <c r="Y38" s="52"/>
       <c r="AB38" s="7"/>
     </row>
     <row r="39" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" s="11">
-        <v>7</v>
-      </c>
-      <c r="D39" s="7">
-        <v>27</v>
-      </c>
-      <c r="E39" s="14">
-        <v>46260</v>
-      </c>
-      <c r="F39" s="9">
-        <f>(E39-$AC$1)/365*12</f>
-        <v>18.805479452054794</v>
-      </c>
+      <c r="B39" s="43"/>
+      <c r="D39" s="7"/>
+      <c r="F39" s="7"/>
       <c r="G39" s="33"/>
       <c r="I39" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J39" s="49">
+      <c r="J39" s="51">
         <f>SUM(J37:J38)*24+K37</f>
         <v>972</v>
       </c>
-      <c r="K39" s="50"/>
+      <c r="K39" s="52"/>
       <c r="N39" s="33"/>
       <c r="O39" s="24"/>
       <c r="P39" s="7" t="s">
@@ -3151,21 +3141,24 @@
       <c r="AB39" s="7"/>
     </row>
     <row r="40" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="B40" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="C40" s="40">
-        <v>81</v>
+        <v>45</v>
+      </c>
+      <c r="C40" s="11">
+        <v>7</v>
       </c>
       <c r="D40" s="7">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E40" s="14">
-        <v>46352</v>
+        <v>46260</v>
       </c>
       <c r="F40" s="9">
         <f>(E40-$AC$1)/365*12</f>
-        <v>21.830136986301369</v>
+        <v>18.805479452054794</v>
       </c>
       <c r="G40" s="33"/>
       <c r="I40" s="13"/>
@@ -3193,15 +3186,22 @@
       <c r="AB40" s="7"/>
     </row>
     <row r="41" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="49">
-        <f>SUM(C39:C40)*30+D39+D40</f>
-        <v>2689</v>
-      </c>
-      <c r="D41" s="50"/>
-      <c r="F41" s="7"/>
+      <c r="B41" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="C41" s="40">
+        <v>81</v>
+      </c>
+      <c r="D41" s="7">
+        <v>22</v>
+      </c>
+      <c r="E41" s="14">
+        <v>46352</v>
+      </c>
+      <c r="F41" s="9">
+        <f>(E41-$AC$1)/365*12</f>
+        <v>21.830136986301369</v>
+      </c>
       <c r="G41" s="33"/>
       <c r="H41" s="6" t="s">
         <v>67</v>
@@ -3226,17 +3226,23 @@
       <c r="P41" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="Q41" s="49">
+      <c r="Q41" s="51">
         <f>SUM(Q38:Q40)*30+R38+R40</f>
         <v>3245</v>
       </c>
-      <c r="R41" s="50"/>
+      <c r="R41" s="52"/>
       <c r="U41" s="34"/>
       <c r="AB41" s="7"/>
     </row>
     <row r="42" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="43"/>
-      <c r="D42" s="7"/>
+      <c r="B42" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="51">
+        <f>SUM(C40:C41)*30+D40+D41</f>
+        <v>2689</v>
+      </c>
+      <c r="D42" s="52"/>
       <c r="F42" s="7"/>
       <c r="G42" s="33"/>
       <c r="H42" s="27"/>
@@ -3259,34 +3265,18 @@
       <c r="AB42" s="7"/>
     </row>
     <row r="43" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="C43" s="7">
-        <v>5</v>
-      </c>
-      <c r="D43" s="7">
-        <v>8</v>
-      </c>
-      <c r="E43" s="14">
-        <v>46291</v>
-      </c>
-      <c r="F43" s="9">
-        <f>(E43-$AC$1)/365*12</f>
-        <v>19.824657534246576</v>
-      </c>
+      <c r="B43" s="43"/>
+      <c r="D43" s="7"/>
+      <c r="F43" s="7"/>
       <c r="G43" s="33"/>
       <c r="I43" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J43" s="49">
+      <c r="J43" s="51">
         <f>SUM(J41:J42)*24+K41</f>
         <v>555</v>
       </c>
-      <c r="K43" s="50"/>
+      <c r="K43" s="52"/>
       <c r="N43" s="33"/>
       <c r="O43" s="6" t="s">
         <v>37</v>
@@ -3297,15 +3287,19 @@
       <c r="U43" s="24"/>
       <c r="AB43" s="7"/>
     </row>
-    <row r="44" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="6"/>
+    <row r="44" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="B44" s="44" t="s">
         <v>46</v>
       </c>
       <c r="C44" s="7">
-        <v>48</v>
-      </c>
-      <c r="D44" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="D44" s="7">
+        <v>8</v>
+      </c>
       <c r="E44" s="14">
         <v>46291</v>
       </c>
@@ -3321,15 +3315,21 @@
       <c r="AB44" s="7"/>
     </row>
     <row r="45" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C45" s="49">
-        <f>SUM(C43:C44)*30+D43</f>
-        <v>1598</v>
-      </c>
-      <c r="D45" s="50"/>
-      <c r="F45" s="7"/>
+      <c r="A45" s="6"/>
+      <c r="B45" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" s="7">
+        <v>48</v>
+      </c>
+      <c r="D45" s="7"/>
+      <c r="E45" s="14">
+        <v>46291</v>
+      </c>
+      <c r="F45" s="9">
+        <f>(E45-$AC$1)/365*12</f>
+        <v>19.824657534246576</v>
+      </c>
       <c r="G45" s="33"/>
       <c r="H45" s="6" t="s">
         <v>68</v>
@@ -3361,9 +3361,14 @@
       <c r="AB45" s="7"/>
     </row>
     <row r="46" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="47"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
+      <c r="B46" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="51">
+        <f>SUM(C44:C45)*30+D44</f>
+        <v>1598</v>
+      </c>
+      <c r="D46" s="52"/>
       <c r="F46" s="7"/>
       <c r="G46" s="33"/>
       <c r="I46" s="7">
@@ -3385,57 +3390,44 @@
       <c r="AB46" s="7"/>
     </row>
     <row r="47" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B47" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="C47" s="7">
-        <v>16</v>
-      </c>
-      <c r="D47" s="11">
-        <v>3</v>
-      </c>
-      <c r="E47" s="14">
-        <v>46260</v>
-      </c>
-      <c r="F47" s="9">
-        <f t="shared" ref="F47:F48" si="37">(E47-$AC$1)/365*12</f>
-        <v>18.805479452054794</v>
-      </c>
+      <c r="B47" s="47"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="F47" s="7"/>
       <c r="G47" s="33"/>
       <c r="H47" s="36"/>
       <c r="I47" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J47" s="49">
+      <c r="J47" s="51">
         <f>SUM(J45:J46)*24+K45</f>
         <v>1414</v>
       </c>
-      <c r="K47" s="50"/>
+      <c r="K47" s="52"/>
       <c r="N47" s="33"/>
       <c r="S47" s="4"/>
       <c r="U47" s="24"/>
       <c r="AB47" s="7"/>
     </row>
-    <row r="48" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="6"/>
+    <row r="48" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="B48" s="43" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C48" s="7">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="D48" s="11">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E48" s="14">
-        <v>46291</v>
+        <v>46260</v>
       </c>
       <c r="F48" s="9">
-        <f t="shared" si="37"/>
-        <v>19.824657534246576</v>
+        <f t="shared" ref="F48:F49" si="37">(E48-$AC$1)/365*12</f>
+        <v>18.805479452054794</v>
       </c>
       <c r="G48" s="33"/>
       <c r="H48" s="24"/>
@@ -3445,15 +3437,23 @@
       <c r="AB48" s="7"/>
     </row>
     <row r="49" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C49" s="49" cm="1">
-        <f t="array" ref="C49">SUM(C47:C48*40)+D47+D48</f>
-        <v>2212</v>
-      </c>
-      <c r="D49" s="50"/>
-      <c r="F49" s="7"/>
+      <c r="A49" s="6"/>
+      <c r="B49" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="7">
+        <v>39</v>
+      </c>
+      <c r="D49" s="11">
+        <v>9</v>
+      </c>
+      <c r="E49" s="14">
+        <v>46291</v>
+      </c>
+      <c r="F49" s="9">
+        <f t="shared" si="37"/>
+        <v>19.824657534246576</v>
+      </c>
       <c r="G49" s="33"/>
       <c r="I49" s="11"/>
       <c r="J49" s="11"/>
@@ -3464,14 +3464,20 @@
       <c r="U49" s="24"/>
       <c r="AB49" s="7"/>
     </row>
-    <row r="50" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="43"/>
-      <c r="D50" s="7"/>
+    <row r="50" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="51" cm="1">
+        <f t="array" ref="C50">SUM(C48:C49*40)+D48+D49</f>
+        <v>2212</v>
+      </c>
+      <c r="D50" s="52"/>
       <c r="F50" s="7"/>
       <c r="G50" s="33"/>
       <c r="I50" s="39"/>
-      <c r="J50" s="52"/>
-      <c r="K50" s="52"/>
+      <c r="J50" s="53"/>
+      <c r="K50" s="53"/>
       <c r="L50" s="24"/>
       <c r="M50" s="24"/>
       <c r="N50" s="24"/>
@@ -3479,45 +3485,33 @@
       <c r="AB50" s="7"/>
     </row>
     <row r="51" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B51" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" s="7">
-        <v>10</v>
-      </c>
-      <c r="D51" s="15">
-        <v>29</v>
-      </c>
-      <c r="E51" s="14">
-        <v>46352</v>
-      </c>
-      <c r="F51" s="9">
-        <f t="shared" ref="F51:F52" si="38">(E51-$AC$1)/365*12</f>
-        <v>21.830136986301369</v>
-      </c>
+      <c r="B51" s="43"/>
+      <c r="D51" s="7"/>
+      <c r="F51" s="7"/>
       <c r="G51" s="33"/>
       <c r="K51" s="7"/>
       <c r="N51" s="24"/>
       <c r="U51" s="24"/>
       <c r="AB51" s="7"/>
     </row>
-    <row r="52" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="6"/>
+    <row r="52" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="B52" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="C52" s="11">
-        <v>34</v>
-      </c>
-      <c r="D52" s="15"/>
+      <c r="C52" s="7">
+        <v>10</v>
+      </c>
+      <c r="D52" s="15">
+        <v>29</v>
+      </c>
       <c r="E52" s="14">
         <v>46352</v>
       </c>
       <c r="F52" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" ref="F52:F53" si="38">(E52-$AC$1)/365*12</f>
         <v>21.830136986301369</v>
       </c>
       <c r="G52" s="33"/>
@@ -3527,24 +3521,36 @@
       <c r="AB52" s="7"/>
     </row>
     <row r="53" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C53" s="49">
-        <f>SUM(C51:C52)*30+D51</f>
-        <v>1349</v>
-      </c>
-      <c r="D53" s="50"/>
-      <c r="F53" s="7"/>
+      <c r="A53" s="6"/>
+      <c r="B53" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" s="11">
+        <v>34</v>
+      </c>
+      <c r="D53" s="15"/>
+      <c r="E53" s="14">
+        <v>46352</v>
+      </c>
+      <c r="F53" s="9">
+        <f t="shared" si="38"/>
+        <v>21.830136986301369</v>
+      </c>
       <c r="G53" s="33"/>
       <c r="K53" s="7"/>
       <c r="N53" s="24"/>
       <c r="U53" s="24"/>
       <c r="AB53" s="7"/>
     </row>
-    <row r="54" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="43"/>
-      <c r="D54" s="7"/>
+    <row r="54" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="51">
+        <f>SUM(C52:C53)*30+D52</f>
+        <v>1349</v>
+      </c>
+      <c r="D54" s="52"/>
       <c r="F54" s="7"/>
       <c r="G54" s="33"/>
       <c r="K54" s="7"/>
@@ -3562,52 +3568,53 @@
       <c r="U55" s="24"/>
       <c r="AB55" s="7"/>
     </row>
-    <row r="56" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B56" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="C56" s="7">
-        <v>10</v>
-      </c>
-      <c r="D56" s="7">
-        <v>19</v>
-      </c>
-      <c r="E56" s="14">
-        <v>45528</v>
-      </c>
-      <c r="F56" s="16">
-        <f>(E56-$AC$1)/365*12</f>
-        <v>-5.2602739726027394</v>
-      </c>
+    <row r="56" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="43"/>
+      <c r="D56" s="7"/>
+      <c r="F56" s="7"/>
       <c r="G56" s="33"/>
       <c r="K56" s="7"/>
       <c r="U56" s="24"/>
       <c r="AB56" s="7"/>
     </row>
     <row r="57" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C57" s="49">
-        <f>SUM(C56)*30+D56</f>
-        <v>319</v>
-      </c>
-      <c r="D57" s="50"/>
-      <c r="F57" s="7"/>
+      <c r="A57" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C57" s="7">
+        <v>10</v>
+      </c>
+      <c r="D57" s="7">
+        <v>19</v>
+      </c>
+      <c r="E57" s="14">
+        <v>45528</v>
+      </c>
+      <c r="F57" s="16">
+        <f>(E57-$AC$1)/365*12</f>
+        <v>-5.2602739726027394</v>
+      </c>
       <c r="G57" s="33"/>
       <c r="K57" s="7"/>
       <c r="U57" s="24"/>
       <c r="AB57" s="7"/>
     </row>
-    <row r="58" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D58" s="7"/>
+    <row r="58" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="51">
+        <f>SUM(C57)*30+D57</f>
+        <v>319</v>
+      </c>
+      <c r="D58" s="52"/>
       <c r="F58" s="7"/>
       <c r="G58" s="33"/>
       <c r="K58" s="7"/>
-      <c r="S58" s="54"/>
+      <c r="S58" s="50"/>
       <c r="U58" s="24"/>
       <c r="AB58" s="7"/>
     </row>
@@ -4536,7 +4543,14 @@
       <c r="E196" s="10"/>
       <c r="F196" s="7"/>
     </row>
-    <row r="197" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A197" s="10"/>
+      <c r="B197" s="10"/>
+      <c r="C197" s="10"/>
+      <c r="D197" s="7"/>
+      <c r="E197" s="10"/>
+      <c r="F197" s="7"/>
+    </row>
     <row r="198" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="199" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="200" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4626,30 +4640,17 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="44">
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="V25:V26"/>
+    <mergeCell ref="X31:Y31"/>
+    <mergeCell ref="X27:Y27"/>
+    <mergeCell ref="X38:Y38"/>
+    <mergeCell ref="X35:Y35"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="X9:Y9"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="X17:Y17"/>
+    <mergeCell ref="X20:Y20"/>
     <mergeCell ref="Q41:R41"/>
     <mergeCell ref="Q6:R6"/>
     <mergeCell ref="Q11:R11"/>
@@ -4659,17 +4660,30 @@
     <mergeCell ref="Q19:R19"/>
     <mergeCell ref="Q32:R32"/>
     <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="X9:Y9"/>
-    <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="X17:Y17"/>
-    <mergeCell ref="X20:Y20"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="V25:V26"/>
-    <mergeCell ref="X31:Y31"/>
-    <mergeCell ref="X27:Y27"/>
-    <mergeCell ref="X38:Y38"/>
-    <mergeCell ref="X35:Y35"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="C50:D50"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4687,12 +4701,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e752113-b2fb-4b78-ae69-b10b93a6ace4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a2a82fc2-af7c-43c6-84e4-151c3b8f78f4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4937,20 +4953,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e752113-b2fb-4b78-ae69-b10b93a6ace4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a2a82fc2-af7c-43c6-84e4-151c3b8f78f4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64C959BB-4F03-4A27-81AC-6DE1AA020D13}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E564C7A4-BCA4-4794-8A6C-B04A14263787}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4e752113-b2fb-4b78-ae69-b10b93a6ace4"/>
+    <ds:schemaRef ds:uri="a2a82fc2-af7c-43c6-84e4-151c3b8f78f4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4975,12 +4992,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E564C7A4-BCA4-4794-8A6C-B04A14263787}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64C959BB-4F03-4A27-81AC-6DE1AA020D13}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4e752113-b2fb-4b78-ae69-b10b93a6ace4"/>
-    <ds:schemaRef ds:uri="a2a82fc2-af7c-43c6-84e4-151c3b8f78f4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>